<commit_message>
Gave Shroomin the ability to reform if the cloud doesn't infect anything. Hopefully this will buff their longevity against guys like the plants
</commit_message>
<xml_diff>
--- a/unit stats.xlsx
+++ b/unit stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas\Documents\wargame\wargame-tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F9F279-3460-4B7A-AC19-74B644C76B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62407D3-93BD-413F-B995-D1341DEB98DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -608,9 +608,6 @@
     <t>Spore Cloud (X)</t>
   </si>
   <si>
-    <t>Releases a cloud of basic spores that fills an area of radius X (2 if not provided) for 3 turns. Each enemy unit that starts or ends its turn within the cloud either becomes infected with the specific Spore type, or adds a counter to an existing Spore infection</t>
-  </si>
-  <si>
     <t>Toxin Spores</t>
   </si>
   <si>
@@ -990,6 +987,9 @@
   </si>
   <si>
     <t>Map was 36x36.  The sporeblowers were very effective.  Perhaps the Beetle Knights need more HP.  Right now they have 14 for Stags and 20 for Hercules.  4 True AOE damage per plant added up fast.  The Knights got up close and started hacking in, but the plants were clustered up enough and could throw enough poison clouds that it was hard to get a knight to stick.  What might have helped would be a Magus, since Royal Decree lets the Knights get a second turn, and they won't end up stuck right in front of the enemy lines.  This might also be more of an imbalance in the game type itself, as the Plant's low movement and power acceleration heavily favors them in a kill game.  This will need more testing, but we do NOT want a balance consisting of auto-winning kill games and auto-losing objective games</t>
+  </si>
+  <si>
+    <t>Releases a cloud of basic spores that fills an area of radius X (2 if not provided) for 3 turns. Each enemy unit that starts or ends its turn within the cloud either becomes infected with the specific Spore type, or adds a counter to an existing Spore infection.  If no enemy units are infected with this cloud after the 3 turns, then return the unit to the battlefield at full Wounds.</t>
   </si>
 </sst>
 </file>
@@ -3954,8 +3954,8 @@
   </sheetPr>
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -6079,7 +6079,9 @@
   </sheetPr>
   <dimension ref="A1:AA21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6106,7 +6108,7 @@
         <v>188</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>189</v>
+        <v>316</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -6114,10 +6116,10 @@
         <v>159</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>190</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -6125,10 +6127,10 @@
         <v>159</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>192</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -6136,10 +6138,10 @@
         <v>159</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>194</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -6147,10 +6149,10 @@
         <v>159</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>196</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -6158,10 +6160,10 @@
         <v>159</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>198</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -6169,32 +6171,32 @@
         <v>159</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>200</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>203</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>205</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -6202,87 +6204,87 @@
         <v>158</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>207</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>210</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>212</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>214</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>136</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>217</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>219</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>221</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>222</v>
       </c>
       <c r="D18" s="16"/>
       <c r="E18" s="6"/>
@@ -6311,13 +6313,13 @@
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>223</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.2">
@@ -6325,10 +6327,10 @@
         <v>161</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>225</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.2">
@@ -6339,7 +6341,7 @@
         <v>122</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -6364,12 +6366,12 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>0</v>
@@ -6381,128 +6383,128 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="14" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>249</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B17" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="18" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>0</v>
@@ -6511,7 +6513,7 @@
         <v>165</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>187</v>
@@ -6519,10 +6521,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>258</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>259</v>
       </c>
       <c r="C21" s="4">
         <v>24</v>
@@ -6531,15 +6533,15 @@
         <v>6</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C22" s="4">
         <v>24</v>
@@ -6548,32 +6550,32 @@
         <v>5</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>263</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>264</v>
       </c>
       <c r="D23" s="4">
         <v>8</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -6594,7 +6596,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B1" s="4">
         <f>6*9</f>
@@ -6607,7 +6609,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B2" s="12">
         <f>18*7</f>
@@ -6616,7 +6618,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B3" s="12">
         <f>10*2</f>
@@ -6625,172 +6627,172 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>283</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C32" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B42" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B43" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B45" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B46" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -6800,42 +6802,42 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B49" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B50" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B57" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B59" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -6860,22 +6862,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>311</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="98.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -6883,19 +6885,19 @@
         <v>44682</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>313</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>314</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>161</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>315</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>316</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated tables. Added beetle knight stub set
</commit_message>
<xml_diff>
--- a/unit stats.xlsx
+++ b/unit stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas\Documents\wargame\wargame-tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62407D3-93BD-413F-B995-D1341DEB98DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD778BC-C9A3-4F23-A044-A78ED3E6ABD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="322">
   <si>
     <t>Name</t>
   </si>
@@ -755,12 +755,6 @@
     <t>Grants Flying</t>
   </si>
   <si>
-    <t>Exoskeleton</t>
-  </si>
-  <si>
-    <t>Grants Burrow and +1 Armor</t>
-  </si>
-  <si>
     <t>Bone Spitters</t>
   </si>
   <si>
@@ -824,18 +818,12 @@
     <t>Mend</t>
   </si>
   <si>
-    <t xml:space="preserve">Remove up to 6 damage from a creature you control with Reshape. </t>
-  </si>
-  <si>
     <t>Combine</t>
   </si>
   <si>
     <t>Unlimited</t>
   </si>
   <si>
-    <t>Select two models you control with Reshape that are within 3" of one another.  Remove both of them from the game and add a new model in its place.  The new model has Reshape X, where X is the total Reshape value of the sacrificed models.  For Power, Toughness, Armor, Damage, choose the highest of the sacrificed models.  For Attack Cost and Move Cost, choose the lowest of the two.  For Wounds, add the total maximum Wounds of each sacrificed model.  The model starts with Y damage taken, where Y is the total damage taken by the sacificed models divided by two.</t>
-  </si>
-  <si>
     <t>Recycle</t>
   </si>
   <si>
@@ -990,6 +978,33 @@
   </si>
   <si>
     <t>Releases a cloud of basic spores that fills an area of radius X (2 if not provided) for 3 turns. Each enemy unit that starts or ends its turn within the cloud either becomes infected with the specific Spore type, or adds a counter to an existing Spore infection.  If no enemy units are infected with this cloud after the 3 turns, then return the unit to the battlefield at full Wounds.</t>
+  </si>
+  <si>
+    <t>True Damage 2;Burning Steps</t>
+  </si>
+  <si>
+    <t>Water Steps</t>
+  </si>
+  <si>
+    <t>Select two models you control with Reshape that are within 3" of one another.  Remove both of them from the game and add a new model in its place.  The new model has Reshape X, where X is the total Reshape value of the sacrificed models.  For Power, Toughness, Armor, Damage, choose the highest of the sacrificed models.  For Attack Cost and Move Cost, choose the lowest of the two.  For Wounds, add the total maximum Wounds of each sacrificed model.  The model starts with  the total Damage of the combined units.  You may use up to one felled model for this.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remove up to 4 damage from a creature you control with Reshape. </t>
+  </si>
+  <si>
+    <t>You may remove a model with Reshape 2+ from the battlefield.  For every two levels of Reshape, create a Flesh Golem</t>
+  </si>
+  <si>
+    <t>Tunneling Claws</t>
+  </si>
+  <si>
+    <t>Grants Burrow</t>
+  </si>
+  <si>
+    <t>Hardened Carapace</t>
+  </si>
+  <si>
+    <t>+1 Armor</t>
   </si>
 </sst>
 </file>
@@ -999,7 +1014,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmmm\ d\,\ yyyy"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1041,6 +1056,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1050,7 +1072,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1065,11 +1087,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1094,6 +1131,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2371,7 +2420,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
@@ -2415,7 +2464,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>21</v>
       </c>
@@ -2459,7 +2508,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>25</v>
       </c>
@@ -2500,7 +2549,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>28</v>
       </c>
@@ -2538,7 +2587,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>31</v>
       </c>
@@ -2576,7 +2625,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>34</v>
       </c>
@@ -2611,7 +2660,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>36</v>
       </c>
@@ -2646,7 +2695,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>38</v>
       </c>
@@ -2687,7 +2736,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>41</v>
       </c>
@@ -2725,7 +2774,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>44</v>
       </c>
@@ -2763,7 +2812,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>46</v>
       </c>
@@ -2807,7 +2856,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>49</v>
       </c>
@@ -2848,7 +2897,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>52</v>
       </c>
@@ -2889,7 +2938,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>55</v>
       </c>
@@ -2930,7 +2979,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>58</v>
       </c>
@@ -2974,7 +3023,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>62</v>
       </c>
@@ -3015,7 +3064,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>65</v>
       </c>
@@ -3056,7 +3105,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>68</v>
       </c>
@@ -3097,7 +3146,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>71</v>
       </c>
@@ -3135,7 +3184,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>73</v>
       </c>
@@ -3173,7 +3222,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>75</v>
       </c>
@@ -3211,7 +3260,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>77</v>
       </c>
@@ -3249,7 +3298,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>79</v>
       </c>
@@ -3287,7 +3336,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>81</v>
       </c>
@@ -3325,7 +3374,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>83</v>
       </c>
@@ -3363,7 +3412,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>85</v>
       </c>
@@ -3401,7 +3450,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>87</v>
       </c>
@@ -3445,7 +3494,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>90</v>
       </c>
@@ -3954,9 +4003,9 @@
   </sheetPr>
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3968,7 +4017,7 @@
     <col min="12" max="12" width="38.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4009,7 +4058,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -4028,7 +4077,7 @@
       <c r="F2" s="1">
         <v>5</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="20">
         <v>20</v>
       </c>
       <c r="H2" s="4">
@@ -4050,7 +4099,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>128</v>
       </c>
@@ -4069,7 +4118,7 @@
       <c r="F3" s="1">
         <v>5</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="20">
         <v>20</v>
       </c>
       <c r="H3" s="4">
@@ -4091,7 +4140,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>19</v>
       </c>
@@ -4110,7 +4159,7 @@
       <c r="F4" s="4">
         <v>7</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="21">
         <v>40</v>
       </c>
       <c r="H4" s="4">
@@ -4132,7 +4181,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>132</v>
       </c>
@@ -4151,7 +4200,7 @@
       <c r="F5" s="4">
         <v>10</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="21">
         <v>56</v>
       </c>
       <c r="H5" s="4">
@@ -4171,7 +4220,7 @@
       </c>
       <c r="M5" s="4"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
@@ -4190,7 +4239,7 @@
       <c r="F6" s="4">
         <v>4</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="21">
         <v>12</v>
       </c>
       <c r="H6" s="4">
@@ -4206,7 +4255,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>25</v>
       </c>
@@ -4225,7 +4274,7 @@
       <c r="F7" s="4">
         <v>4</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="21">
         <v>8</v>
       </c>
       <c r="H7" s="4">
@@ -4244,7 +4293,13 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G8" s="22"/>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G9" s="22"/>
+    </row>
+    <row r="10" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>28</v>
       </c>
@@ -4260,8 +4315,8 @@
       <c r="F10" s="4">
         <v>3</v>
       </c>
-      <c r="G10" s="4">
-        <v>6</v>
+      <c r="G10" s="21">
+        <v>8</v>
       </c>
       <c r="H10" s="4">
         <v>0</v>
@@ -4275,8 +4330,11 @@
       <c r="K10" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L10" s="15" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>31</v>
       </c>
@@ -4292,8 +4350,8 @@
       <c r="F11" s="4">
         <v>2</v>
       </c>
-      <c r="G11" s="4">
-        <v>6</v>
+      <c r="G11" s="21">
+        <v>8</v>
       </c>
       <c r="H11" s="4">
         <v>0</v>
@@ -4308,7 +4366,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>34</v>
       </c>
@@ -4324,8 +4382,8 @@
       <c r="F12" s="4">
         <v>4</v>
       </c>
-      <c r="G12" s="4">
-        <v>8</v>
+      <c r="G12" s="21">
+        <v>12</v>
       </c>
       <c r="H12" s="4">
         <v>1</v>
@@ -4336,8 +4394,11 @@
       <c r="K12" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L12" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>36</v>
       </c>
@@ -4353,8 +4414,8 @@
       <c r="F13" s="4">
         <v>3</v>
       </c>
-      <c r="G13" s="4">
-        <v>10</v>
+      <c r="G13" s="21">
+        <v>14</v>
       </c>
       <c r="H13" s="4">
         <v>2</v>
@@ -4365,8 +4426,11 @@
       <c r="K13" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L13" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>38</v>
       </c>
@@ -4385,7 +4449,7 @@
       <c r="F14" s="4">
         <v>2</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="21">
         <v>9</v>
       </c>
       <c r="H14" s="4">
@@ -4401,7 +4465,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>41</v>
       </c>
@@ -4409,7 +4473,7 @@
         <v>42</v>
       </c>
       <c r="C15" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>43</v>
@@ -4420,7 +4484,7 @@
       <c r="F15" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="22" t="s">
         <v>43</v>
       </c>
       <c r="H15" s="4" t="s">
@@ -4433,7 +4497,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>44</v>
       </c>
@@ -4452,7 +4516,7 @@
       <c r="F16" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="22" t="s">
         <v>43</v>
       </c>
       <c r="H16" s="4" t="s">
@@ -4465,7 +4529,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G17" s="22"/>
+    </row>
+    <row r="18" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>46</v>
       </c>
@@ -4484,8 +4551,8 @@
       <c r="F18" s="4">
         <v>3</v>
       </c>
-      <c r="G18" s="4">
-        <v>5</v>
+      <c r="G18" s="21">
+        <v>6</v>
       </c>
       <c r="H18" s="4">
         <v>0</v>
@@ -4503,7 +4570,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>49</v>
       </c>
@@ -4522,7 +4589,7 @@
       <c r="F19" s="4">
         <v>3</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="21">
         <v>10</v>
       </c>
       <c r="H19" s="4">
@@ -4538,7 +4605,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>137</v>
       </c>
@@ -4557,8 +4624,8 @@
       <c r="F20" s="4">
         <v>3</v>
       </c>
-      <c r="G20" s="4">
-        <v>5</v>
+      <c r="G20" s="21">
+        <v>6</v>
       </c>
       <c r="H20" s="4">
         <v>0</v>
@@ -4573,7 +4640,10 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G21" s="22"/>
+    </row>
+    <row r="22" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>55</v>
       </c>
@@ -4592,7 +4662,7 @@
       <c r="F22" s="4">
         <v>3</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="21">
         <v>7</v>
       </c>
       <c r="H22" s="4">
@@ -4608,7 +4678,10 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G23" s="22"/>
+    </row>
+    <row r="24" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>58</v>
       </c>
@@ -4627,7 +4700,7 @@
       <c r="F24" s="4">
         <v>6</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G24" s="21">
         <v>14</v>
       </c>
       <c r="H24" s="4">
@@ -4646,7 +4719,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>62</v>
       </c>
@@ -4665,7 +4738,7 @@
       <c r="F25" s="4">
         <v>5</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G25" s="21">
         <v>12</v>
       </c>
       <c r="H25" s="4">
@@ -4681,7 +4754,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>65</v>
       </c>
@@ -4700,7 +4773,7 @@
       <c r="F26" s="4">
         <v>4</v>
       </c>
-      <c r="G26" s="4">
+      <c r="G26" s="21">
         <v>6</v>
       </c>
       <c r="H26" s="4">
@@ -4716,7 +4789,10 @@
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G27" s="22"/>
+    </row>
+    <row r="28" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>68</v>
       </c>
@@ -4735,7 +4811,7 @@
       <c r="F28" s="4">
         <v>3</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G28" s="21">
         <v>8</v>
       </c>
       <c r="H28" s="4">
@@ -4751,7 +4827,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>71</v>
       </c>
@@ -4767,7 +4843,7 @@
       <c r="F29" s="4">
         <v>3</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G29" s="21">
         <v>8</v>
       </c>
       <c r="H29" s="4">
@@ -4783,7 +4859,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>73</v>
       </c>
@@ -4799,7 +4875,7 @@
       <c r="F30" s="4">
         <v>3</v>
       </c>
-      <c r="G30" s="4">
+      <c r="G30" s="21">
         <v>8</v>
       </c>
       <c r="H30" s="4">
@@ -4815,7 +4891,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>75</v>
       </c>
@@ -4831,7 +4907,7 @@
       <c r="F31" s="4">
         <v>3</v>
       </c>
-      <c r="G31" s="4">
+      <c r="G31" s="21">
         <v>8</v>
       </c>
       <c r="H31" s="4">
@@ -4847,7 +4923,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>77</v>
       </c>
@@ -4863,7 +4939,7 @@
       <c r="F32" s="4">
         <v>3</v>
       </c>
-      <c r="G32" s="4">
+      <c r="G32" s="21">
         <v>8</v>
       </c>
       <c r="H32" s="4">
@@ -4879,7 +4955,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>79</v>
       </c>
@@ -4895,7 +4971,7 @@
       <c r="F33" s="4">
         <v>3</v>
       </c>
-      <c r="G33" s="4">
+      <c r="G33" s="21">
         <v>8</v>
       </c>
       <c r="H33" s="4">
@@ -4911,7 +4987,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>81</v>
       </c>
@@ -4927,7 +5003,7 @@
       <c r="F34" s="4">
         <v>3</v>
       </c>
-      <c r="G34" s="4">
+      <c r="G34" s="21">
         <v>8</v>
       </c>
       <c r="H34" s="4">
@@ -4943,7 +5019,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>83</v>
       </c>
@@ -4959,7 +5035,7 @@
       <c r="F35" s="4">
         <v>3</v>
       </c>
-      <c r="G35" s="4">
+      <c r="G35" s="21">
         <v>8</v>
       </c>
       <c r="H35" s="4">
@@ -4975,7 +5051,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>85</v>
       </c>
@@ -4991,7 +5067,7 @@
       <c r="F36" s="4">
         <v>3</v>
       </c>
-      <c r="G36" s="4">
+      <c r="G36" s="21">
         <v>8</v>
       </c>
       <c r="H36" s="4">
@@ -5007,7 +5083,10 @@
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G37" s="22"/>
+    </row>
+    <row r="38" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>87</v>
       </c>
@@ -5026,7 +5105,7 @@
       <c r="F38" s="4">
         <v>0</v>
       </c>
-      <c r="G38" s="4">
+      <c r="G38" s="21">
         <v>1</v>
       </c>
       <c r="H38" s="4">
@@ -5045,12 +5124,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C39" s="4">
         <v>1</v>
@@ -5064,7 +5143,7 @@
       <c r="F39" s="4">
         <v>3</v>
       </c>
-      <c r="G39" s="4">
+      <c r="G39" s="21">
         <v>8</v>
       </c>
       <c r="H39" s="4">
@@ -5073,122 +5152,122 @@
       <c r="I39" s="4">
         <v>1</v>
       </c>
-      <c r="J39" s="4"/>
       <c r="K39" s="4">
         <v>10</v>
       </c>
       <c r="L39" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C40" s="4">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="D40" s="4">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="E40" s="4">
         <v>3</v>
       </c>
       <c r="F40" s="4">
-        <v>3</v>
-      </c>
-      <c r="G40" s="4">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="G40" s="21">
+        <v>16</v>
       </c>
       <c r="H40" s="4">
         <v>0</v>
       </c>
       <c r="I40" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K40" s="4">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="L40" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C41" s="4">
         <v>0.9</v>
       </c>
       <c r="D41" s="4">
-        <v>2.9</v>
+        <v>2.8</v>
       </c>
       <c r="E41" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F41" s="4">
+        <v>5</v>
+      </c>
+      <c r="G41" s="21">
+        <v>28</v>
+      </c>
+      <c r="H41" s="4">
+        <v>1</v>
+      </c>
+      <c r="I41" s="4">
+        <v>3</v>
+      </c>
+      <c r="K41" s="4">
+        <v>35</v>
+      </c>
+      <c r="L41" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C42" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="D42" s="8">
+        <v>2.7</v>
+      </c>
+      <c r="E42" s="9">
+        <v>6</v>
+      </c>
+      <c r="F42" s="9">
+        <v>6</v>
+      </c>
+      <c r="G42" s="21">
+        <v>44</v>
+      </c>
+      <c r="H42" s="9">
+        <v>1</v>
+      </c>
+      <c r="I42" s="9">
         <v>4</v>
       </c>
-      <c r="G41" s="4">
-        <v>10</v>
-      </c>
-      <c r="H41" s="4">
-        <v>0</v>
-      </c>
-      <c r="I41" s="4">
-        <v>2</v>
-      </c>
-      <c r="K41" s="4">
-        <v>20</v>
-      </c>
-      <c r="L41" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C42" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="D42" s="4">
-        <v>2.8</v>
-      </c>
-      <c r="E42" s="4">
-        <v>5</v>
-      </c>
-      <c r="F42" s="4">
-        <v>5</v>
-      </c>
-      <c r="G42" s="4">
-        <v>12</v>
-      </c>
-      <c r="H42" s="4">
-        <v>1</v>
-      </c>
-      <c r="I42" s="4">
-        <v>3</v>
-      </c>
-      <c r="K42" s="4">
-        <v>35</v>
-      </c>
-      <c r="L42" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="7" t="s">
-        <v>102</v>
+      <c r="J42" s="6"/>
+      <c r="K42" s="9">
+        <v>55</v>
+      </c>
+      <c r="L42" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>105</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>103</v>
@@ -5197,108 +5276,111 @@
         <v>0.8</v>
       </c>
       <c r="D43" s="8">
-        <v>2.7</v>
-      </c>
-      <c r="E43" s="9">
-        <v>6</v>
-      </c>
-      <c r="F43" s="9">
-        <v>6</v>
-      </c>
-      <c r="G43" s="9">
+        <v>2.6</v>
+      </c>
+      <c r="E43" s="8">
+        <v>7</v>
+      </c>
+      <c r="F43" s="8">
+        <v>7</v>
+      </c>
+      <c r="G43" s="21">
+        <v>64</v>
+      </c>
+      <c r="H43" s="9">
+        <v>1</v>
+      </c>
+      <c r="I43" s="8">
+        <v>5</v>
+      </c>
+      <c r="J43" s="6"/>
+      <c r="K43" s="8">
+        <v>80</v>
+      </c>
+      <c r="L43" s="11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C44" s="4">
+        <v>1</v>
+      </c>
+      <c r="D44" s="4">
+        <v>3</v>
+      </c>
+      <c r="E44" s="4">
+        <v>4</v>
+      </c>
+      <c r="F44" s="4">
+        <v>4</v>
+      </c>
+      <c r="G44" s="21">
         <v>14</v>
       </c>
-      <c r="H43" s="9">
-        <v>1</v>
-      </c>
-      <c r="I43" s="9">
+      <c r="H44" s="4">
+        <v>0</v>
+      </c>
+      <c r="I44" s="4">
         <v>4</v>
       </c>
-      <c r="J43" s="6"/>
-      <c r="K43" s="9">
-        <v>55</v>
-      </c>
-      <c r="L43" s="10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A44" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C44" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="D44" s="8">
-        <v>2.6</v>
-      </c>
-      <c r="E44" s="8">
-        <v>7</v>
-      </c>
-      <c r="F44" s="8">
-        <v>7</v>
-      </c>
-      <c r="G44" s="8">
-        <v>16</v>
-      </c>
-      <c r="H44" s="9">
-        <v>1</v>
-      </c>
-      <c r="I44" s="8">
-        <v>5</v>
-      </c>
-      <c r="J44" s="6"/>
-      <c r="K44" s="8">
-        <v>80</v>
-      </c>
-      <c r="L44" s="11" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C45" s="4">
-        <v>1</v>
-      </c>
-      <c r="D45" s="4">
-        <v>3</v>
-      </c>
-      <c r="E45" s="4">
-        <v>4</v>
-      </c>
-      <c r="F45" s="4">
-        <v>4</v>
-      </c>
-      <c r="G45" s="4">
-        <v>14</v>
-      </c>
-      <c r="H45" s="4">
-        <v>0</v>
-      </c>
-      <c r="I45" s="4">
-        <v>4</v>
-      </c>
-      <c r="K45" s="4">
+      <c r="K44" s="4">
         <v>25</v>
       </c>
-      <c r="L45" s="4" t="s">
+      <c r="L44" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G45" s="22"/>
+    </row>
+    <row r="46" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C46" s="4">
+        <v>2</v>
+      </c>
+      <c r="D46" s="4">
+        <v>3</v>
+      </c>
+      <c r="E46" s="4">
+        <v>2</v>
+      </c>
+      <c r="F46" s="4">
+        <v>3</v>
+      </c>
+      <c r="G46" s="21">
+        <v>8</v>
+      </c>
+      <c r="H46" s="4">
+        <v>0</v>
+      </c>
+      <c r="I46" s="4">
+        <v>0</v>
+      </c>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4">
+        <v>10</v>
+      </c>
+      <c r="L46" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C47" s="4">
         <v>2</v>
@@ -5312,7 +5394,7 @@
       <c r="F47" s="4">
         <v>3</v>
       </c>
-      <c r="G47" s="4">
+      <c r="G47" s="21">
         <v>8</v>
       </c>
       <c r="H47" s="4">
@@ -5321,7 +5403,9 @@
       <c r="I47" s="4">
         <v>0</v>
       </c>
-      <c r="J47" s="4"/>
+      <c r="J47" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="K47" s="4">
         <v>10</v>
       </c>
@@ -5329,137 +5413,137 @@
         <v>112</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C48" s="4">
-        <v>2</v>
-      </c>
-      <c r="D48" s="4">
-        <v>3</v>
+        <v>117</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="E48" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" s="4">
-        <v>3</v>
-      </c>
-      <c r="G48" s="4">
+        <v>0</v>
+      </c>
+      <c r="G48" s="21">
+        <v>1</v>
+      </c>
+      <c r="H48" s="4">
+        <v>0</v>
+      </c>
+      <c r="I48" s="4">
+        <v>1</v>
+      </c>
+      <c r="K48" s="4">
+        <v>5</v>
+      </c>
+      <c r="L48" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C49" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="D49" s="4">
+        <v>3</v>
+      </c>
+      <c r="E49" s="4">
+        <v>7</v>
+      </c>
+      <c r="F49" s="4">
+        <v>7</v>
+      </c>
+      <c r="G49" s="21">
+        <v>15</v>
+      </c>
+      <c r="H49" s="4">
+        <v>2</v>
+      </c>
+      <c r="I49" s="4">
+        <v>3</v>
+      </c>
+      <c r="J49" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="K49" s="4">
+        <v>50</v>
+      </c>
+      <c r="L49" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C50" s="4">
+        <v>2</v>
+      </c>
+      <c r="D50" s="4">
+        <v>3</v>
+      </c>
+      <c r="E50" s="4">
+        <v>2</v>
+      </c>
+      <c r="F50" s="4">
+        <v>0</v>
+      </c>
+      <c r="G50" s="21">
         <v>8</v>
       </c>
-      <c r="H48" s="4">
-        <v>0</v>
-      </c>
-      <c r="I48" s="4">
-        <v>0</v>
-      </c>
-      <c r="J48" s="4" t="s">
+      <c r="H50" s="4">
+        <v>0</v>
+      </c>
+      <c r="I50" s="4">
+        <v>0</v>
+      </c>
+      <c r="J50" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="K48" s="4">
+      <c r="K50" s="4">
         <v>10</v>
       </c>
-      <c r="L48" s="4" t="s">
+      <c r="L50" s="4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A49" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E49" s="4">
-        <v>1</v>
-      </c>
-      <c r="F49" s="4">
-        <v>0</v>
-      </c>
-      <c r="G49" s="4">
-        <v>1</v>
-      </c>
-      <c r="H49" s="4">
-        <v>0</v>
-      </c>
-      <c r="I49" s="4">
-        <v>1</v>
-      </c>
-      <c r="K49" s="4">
-        <v>5</v>
-      </c>
-      <c r="L49" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A50" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="C50" s="4">
-        <v>1.5</v>
-      </c>
-      <c r="D50" s="4">
-        <v>3</v>
-      </c>
-      <c r="E50" s="4">
-        <v>7</v>
-      </c>
-      <c r="F50" s="4">
-        <v>7</v>
-      </c>
-      <c r="G50" s="4">
-        <v>15</v>
-      </c>
-      <c r="H50" s="4">
-        <v>2</v>
-      </c>
-      <c r="I50" s="4">
-        <v>3</v>
-      </c>
-      <c r="J50" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="K50" s="4">
-        <v>50</v>
-      </c>
-      <c r="L50" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="C51" s="4">
         <v>2</v>
       </c>
       <c r="D51" s="4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E51" s="4">
         <v>2</v>
       </c>
       <c r="F51" s="4">
-        <v>0</v>
-      </c>
-      <c r="G51" s="4">
+        <v>6</v>
+      </c>
+      <c r="G51" s="21">
         <v>8</v>
       </c>
       <c r="H51" s="4">
@@ -5475,29 +5559,29 @@
         <v>10</v>
       </c>
       <c r="L51" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>123</v>
+        <v>142</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>124</v>
+        <v>143</v>
       </c>
       <c r="C52" s="4">
         <v>2</v>
       </c>
-      <c r="D52" s="4">
-        <v>6</v>
+      <c r="D52" s="4" t="s">
+        <v>144</v>
       </c>
       <c r="E52" s="4">
         <v>2</v>
       </c>
-      <c r="F52" s="4">
-        <v>6</v>
-      </c>
-      <c r="G52" s="4">
+      <c r="F52" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="G52" s="21">
         <v>8</v>
       </c>
       <c r="H52" s="4">
@@ -5507,55 +5591,19 @@
         <v>0</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>115</v>
+        <v>146</v>
       </c>
       <c r="K52" s="4">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="L52" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A53" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="C53" s="4">
-        <v>2</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="E53" s="4">
-        <v>2</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="G53" s="4">
-        <v>8</v>
-      </c>
-      <c r="H53" s="4">
-        <v>0</v>
-      </c>
-      <c r="I53" s="4">
-        <v>0</v>
-      </c>
-      <c r="J53" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="K53" s="4">
-        <v>8</v>
-      </c>
-      <c r="L53" s="4" t="s">
         <v>147</v>
       </c>
     </row>
+    <row r="53" spans="1:12" ht="12.75" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6079,7 +6127,7 @@
   </sheetPr>
   <dimension ref="A1:AA21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -6108,7 +6156,7 @@
         <v>188</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -6354,14 +6402,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:E24"/>
+  <dimension ref="A2:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.5703125" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="71.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6428,154 +6479,172 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
-        <v>238</v>
+        <v>318</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
-        <v>239</v>
+        <v>319</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="14" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B17" s="15" t="s">
+        <v>320</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="14" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="4" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="18" t="s">
         <v>252</v>
-      </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="18" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="C21" s="4">
-        <v>24</v>
-      </c>
-      <c r="D21" s="4">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>254</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>259</v>
+        <v>187</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C22" s="4">
         <v>24</v>
       </c>
       <c r="D22" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>263</v>
+        <v>258</v>
+      </c>
+      <c r="C23" s="4">
+        <v>24</v>
       </c>
       <c r="D23" s="4">
+        <v>3</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="D24" s="4">
         <v>8</v>
       </c>
-      <c r="E23" s="4" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>265</v>
+      <c r="E24" s="23" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="C25">
+        <v>12</v>
+      </c>
+      <c r="D25" s="15">
+        <v>6</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -6596,7 +6665,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B1" s="4">
         <f>6*9</f>
@@ -6609,7 +6678,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B2" s="12">
         <f>18*7</f>
@@ -6618,7 +6687,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B3" s="12">
         <f>10*2</f>
@@ -6627,172 +6696,172 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C32" s="4" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B42" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B43" s="4" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B45" s="4" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B46" s="4" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -6802,42 +6871,42 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B49" s="4" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B50" s="4" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B57" s="4" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B59" s="4" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -6862,22 +6931,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>307</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>309</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>310</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="98.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -6885,19 +6954,19 @@
         <v>44682</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>161</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated wound totals for Psi-hive and tweaked Tunnel Monsters
</commit_message>
<xml_diff>
--- a/unit stats.xlsx
+++ b/unit stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas\Documents\wargame\wargame-tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD778BC-C9A3-4F23-A044-A78ED3E6ABD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44253B47-AA33-4F97-8760-53511015BC01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="323">
   <si>
     <t>Name</t>
   </si>
@@ -647,12 +647,6 @@
     <t>General</t>
   </si>
   <si>
-    <t>Tremorsense X</t>
-  </si>
-  <si>
-    <t>Grants sight of all enemy units which end the turn within X inches</t>
-  </si>
-  <si>
     <t>Blind</t>
   </si>
   <si>
@@ -1005,6 +999,15 @@
   </si>
   <si>
     <t>+1 Armor</t>
+  </si>
+  <si>
+    <t>Tremorsense; Blind;Burrow</t>
+  </si>
+  <si>
+    <t>Tremorsense</t>
+  </si>
+  <si>
+    <t>When burrowed, ignore Blind penalties if you Unburrow within 2 inches of an enemy model that moved last turn</t>
   </si>
 </sst>
 </file>
@@ -1935,7 +1938,7 @@
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2008,7 +2011,7 @@
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -4005,7 +4008,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4331,7 +4334,7 @@
         <v>15</v>
       </c>
       <c r="L10" s="15" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4395,7 +4398,7 @@
         <v>15</v>
       </c>
       <c r="L12" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4427,7 +4430,7 @@
         <v>15</v>
       </c>
       <c r="L13" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4689,10 +4692,10 @@
         <v>59</v>
       </c>
       <c r="C24" s="4">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="D24" s="4">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="E24" s="4">
         <v>6</v>
@@ -4701,13 +4704,13 @@
         <v>6</v>
       </c>
       <c r="G24" s="21">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H24" s="4">
         <v>0</v>
       </c>
       <c r="I24" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J24" s="4" t="s">
         <v>60</v>
@@ -4716,7 +4719,7 @@
         <v>25</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>61</v>
+        <v>320</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4730,28 +4733,28 @@
         <v>1</v>
       </c>
       <c r="D25" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E25" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F25" s="4">
         <v>5</v>
       </c>
       <c r="G25" s="21">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H25" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I25" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K25" s="4">
         <v>20</v>
       </c>
-      <c r="L25" s="4" t="s">
-        <v>64</v>
+      <c r="L25" s="15" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4762,10 +4765,10 @@
         <v>66</v>
       </c>
       <c r="C26" s="4">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="D26" s="4">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="E26" s="4">
         <v>4</v>
@@ -4774,19 +4777,19 @@
         <v>4</v>
       </c>
       <c r="G26" s="21">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H26" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I26" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K26" s="4">
         <v>10</v>
       </c>
-      <c r="L26" s="4" t="s">
-        <v>67</v>
+      <c r="L26" s="15" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4812,7 +4815,7 @@
         <v>3</v>
       </c>
       <c r="G28" s="21">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="H28" s="4">
         <v>0</v>
@@ -4844,7 +4847,7 @@
         <v>3</v>
       </c>
       <c r="G29" s="21">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="H29" s="4">
         <v>0</v>
@@ -4876,7 +4879,7 @@
         <v>3</v>
       </c>
       <c r="G30" s="21">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="H30" s="4">
         <v>0</v>
@@ -4908,7 +4911,7 @@
         <v>3</v>
       </c>
       <c r="G31" s="21">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="H31" s="4">
         <v>0</v>
@@ -4940,7 +4943,7 @@
         <v>3</v>
       </c>
       <c r="G32" s="21">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="H32" s="4">
         <v>0</v>
@@ -4972,7 +4975,7 @@
         <v>3</v>
       </c>
       <c r="G33" s="21">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="H33" s="4">
         <v>0</v>
@@ -5004,7 +5007,7 @@
         <v>3</v>
       </c>
       <c r="G34" s="21">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="H34" s="4">
         <v>0</v>
@@ -5036,7 +5039,7 @@
         <v>3</v>
       </c>
       <c r="G35" s="21">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="H35" s="4">
         <v>0</v>
@@ -5068,7 +5071,7 @@
         <v>3</v>
       </c>
       <c r="G36" s="21">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="H36" s="4">
         <v>0</v>
@@ -6128,7 +6131,7 @@
   <dimension ref="A1:AA21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6156,7 +6159,7 @@
         <v>188</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -6230,10 +6233,10 @@
         <v>201</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>202</v>
+        <v>321</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>203</v>
+        <v>322</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -6241,10 +6244,10 @@
         <v>201</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -6252,43 +6255,43 @@
         <v>158</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>208</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -6299,7 +6302,7 @@
         <v>136</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -6307,10 +6310,10 @@
         <v>201</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.2">
@@ -6318,10 +6321,10 @@
         <v>201</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.2">
@@ -6329,10 +6332,10 @@
         <v>201</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D18" s="16"/>
       <c r="E18" s="6"/>
@@ -6364,10 +6367,10 @@
         <v>201</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.2">
@@ -6375,10 +6378,10 @@
         <v>161</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.2">
@@ -6389,7 +6392,7 @@
         <v>122</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -6417,12 +6420,12 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>0</v>
@@ -6434,137 +6437,137 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="14" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="14" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="14" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="14" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B17" s="15" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="14" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B18" s="4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="18" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>0</v>
@@ -6573,7 +6576,7 @@
         <v>165</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>187</v>
@@ -6581,10 +6584,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C22" s="4">
         <v>24</v>
@@ -6593,15 +6596,15 @@
         <v>6</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C23" s="4">
         <v>24</v>
@@ -6610,32 +6613,32 @@
         <v>3</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D24" s="4">
         <v>8</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C25">
         <v>12</v>
@@ -6644,7 +6647,7 @@
         <v>6</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -6665,7 +6668,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B1" s="4">
         <f>6*9</f>
@@ -6678,7 +6681,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B2" s="12">
         <f>18*7</f>
@@ -6687,7 +6690,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B3" s="12">
         <f>10*2</f>
@@ -6696,172 +6699,172 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C32" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B42" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B43" s="4" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B45" s="4" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B46" s="4" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -6871,42 +6874,42 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B49" s="4" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B50" s="4" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B57" s="4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B59" s="4" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -6931,22 +6934,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>305</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="98.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -6954,19 +6957,19 @@
         <v>44682</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>161</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated book with stats for beetles, elementals, and FCP. Updated stat tables in xlsx
</commit_message>
<xml_diff>
--- a/unit stats.xlsx
+++ b/unit stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas\Documents\wargame\wargame-tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7E3CF1-CB29-478C-B735-1D6BF186C238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B341C204-0B05-4AA2-BCDE-5A5C28298C8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20520" yWindow="4665" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="324">
   <si>
     <t>Name</t>
   </si>
@@ -1008,6 +1008,9 @@
   </si>
   <si>
     <t>When burrowed, ignore Blind penalties if you Unburrow within 2 inches of an enemy model that moved last turn</t>
+  </si>
+  <si>
+    <t>Flesh Colossus</t>
   </si>
 </sst>
 </file>
@@ -4007,8 +4010,8 @@
   <dimension ref="A1:M53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G37" sqref="G37"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4447,13 +4450,13 @@
         <v>3</v>
       </c>
       <c r="E14" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F14" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G14" s="21">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="H14" s="4">
         <v>1</v>
@@ -4508,7 +4511,7 @@
         <v>45</v>
       </c>
       <c r="C16" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>43</v>
@@ -5164,7 +5167,7 @@
     </row>
     <row r="40" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>97</v>
@@ -5176,7 +5179,7 @@
         <v>2.9</v>
       </c>
       <c r="E40" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F40" s="4">
         <v>4</v>
@@ -5199,7 +5202,7 @@
     </row>
     <row r="41" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>100</v>
@@ -5234,7 +5237,7 @@
     </row>
     <row r="42" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>102</v>
+        <v>323</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>103</v>

</xml_diff>

<commit_message>
Added new pictures in and updated stats
</commit_message>
<xml_diff>
--- a/unit stats.xlsx
+++ b/unit stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas\Documents\wargame\wargame-tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7EAECD-1F4E-4A99-BD1B-E9E00C5C3014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E754037-514F-42E1-8B41-A8C39B3D3392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20520" yWindow="4665" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20520" yWindow="4665" windowWidth="20640" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="338">
   <si>
     <t>Name</t>
   </si>
@@ -635,9 +635,6 @@
     <t>Summon Spores</t>
   </si>
   <si>
-    <t>Creates a spore cloud at a location, or adds 3 rounds to an existing cloud while increasing its radius by half</t>
-  </si>
-  <si>
     <t>Infect X</t>
   </si>
   <si>
@@ -722,9 +719,6 @@
     <t>Growth Hormones</t>
   </si>
   <si>
-    <t>Grants the unit +1 Toughness and +1 Power</t>
-  </si>
-  <si>
     <t>Sharpened Claws</t>
   </si>
   <si>
@@ -770,9 +764,6 @@
     <t>Restoration Gene</t>
   </si>
   <si>
-    <t>Grants Regeneration 1</t>
-  </si>
-  <si>
     <t>Focused Instincts</t>
   </si>
   <si>
@@ -971,9 +962,6 @@
     <t>Map was 36x36.  The sporeblowers were very effective.  Perhaps the Beetle Knights need more HP.  Right now they have 14 for Stags and 20 for Hercules.  4 True AOE damage per plant added up fast.  The Knights got up close and started hacking in, but the plants were clustered up enough and could throw enough poison clouds that it was hard to get a knight to stick.  What might have helped would be a Magus, since Royal Decree lets the Knights get a second turn, and they won't end up stuck right in front of the enemy lines.  This might also be more of an imbalance in the game type itself, as the Plant's low movement and power acceleration heavily favors them in a kill game.  This will need more testing, but we do NOT want a balance consisting of auto-winning kill games and auto-losing objective games</t>
   </si>
   <si>
-    <t>Releases a cloud of basic spores that fills an area of radius X (2 if not provided) for 3 turns. Each enemy unit that starts or ends its turn within the cloud either becomes infected with the specific Spore type, or adds a counter to an existing Spore infection.  If no enemy units are infected with this cloud after the 3 turns, then return the unit to the battlefield at full Wounds.</t>
-  </si>
-  <si>
     <t>True Damage 2;Burning Steps</t>
   </si>
   <si>
@@ -998,9 +986,6 @@
     <t>Hardened Carapace</t>
   </si>
   <si>
-    <t>+1 Armor</t>
-  </si>
-  <si>
     <t>Tremorsense; Blind;Burrow</t>
   </si>
   <si>
@@ -1011,6 +996,63 @@
   </si>
   <si>
     <t>Flesh Colossus</t>
+  </si>
+  <si>
+    <t>Spore Cloud, Infect</t>
+  </si>
+  <si>
+    <t>Hydra</t>
+  </si>
+  <si>
+    <t>Melee unit.  Copies itself when it dies</t>
+  </si>
+  <si>
+    <t>Hydra Spores</t>
+  </si>
+  <si>
+    <t>When the Hydra dies, create an additional Spore Cloud within 3 inches of the model.  Both clouds have a single counter on them, and will reform a Hydra if not absorbed</t>
+  </si>
+  <si>
+    <t>Spore Cloud, Hydra Spores, Infect</t>
+  </si>
+  <si>
+    <t>Large melee unit.  Limited offensive capability, but has high wounds  and generates clouds when hit</t>
+  </si>
+  <si>
+    <t>Spore Cloud, Breakaway Spores</t>
+  </si>
+  <si>
+    <t>Breakaway Spores</t>
+  </si>
+  <si>
+    <t>Spore Colony</t>
+  </si>
+  <si>
+    <t>Releases a cloud of basic spores that fills an area of radius X (2 if not provided) for 3 turns. Each enemy unit that ends its turn within the cloud either becomes infected with the specific Spore type, or adds a counter to an existing Spore infection.  If no enemy units are infected with this cloud after the 3 turns, then return the unit to the battlefield at full Wounds.</t>
+  </si>
+  <si>
+    <t>Creates a spore cloud at a location, or adds 3 rounds to an existing cloud while increasing its radius by 2 inches</t>
+  </si>
+  <si>
+    <t>When the Spore Colony takes damage, for every 3 damage you may generate a Spore Cloud within 3 inches of the Spore Colony that has two counters on it.  If this is not absorbed, create a Grunt upon dissolution of the cloud</t>
+  </si>
+  <si>
+    <t>Spellcaster: Fleshcraft. Resape</t>
+  </si>
+  <si>
+    <t>Hardened Bones</t>
+  </si>
+  <si>
+    <t>+1 Toughness</t>
+  </si>
+  <si>
+    <t>+1 Power</t>
+  </si>
+  <si>
+    <t>Grants Regeneration 2</t>
+  </si>
+  <si>
+    <t>+0.5 Armor</t>
   </si>
 </sst>
 </file>
@@ -1112,7 +1154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1147,6 +1189,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4007,11 +4061,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:M53"/>
+  <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18:K20"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A44" sqref="A44:XFD44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4337,7 +4391,7 @@
         <v>15</v>
       </c>
       <c r="L10" s="15" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4401,7 +4455,7 @@
         <v>15</v>
       </c>
       <c r="L12" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4433,7 +4487,7 @@
         <v>15</v>
       </c>
       <c r="L13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4573,7 +4627,7 @@
         <v>7</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>48</v>
+        <v>319</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4648,42 +4702,78 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G21" s="22"/>
-    </row>
-    <row r="22" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="4">
-        <v>1</v>
-      </c>
-      <c r="D22" s="4">
-        <v>3</v>
-      </c>
-      <c r="E22" s="4">
-        <v>3</v>
-      </c>
-      <c r="F22" s="4">
+    <row r="21" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="24" t="s">
+        <v>320</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>321</v>
+      </c>
+      <c r="C21" s="25">
+        <v>1</v>
+      </c>
+      <c r="D21" s="25">
+        <v>3</v>
+      </c>
+      <c r="E21" s="25">
+        <v>2</v>
+      </c>
+      <c r="F21" s="25">
+        <v>2</v>
+      </c>
+      <c r="G21" s="21">
+        <v>14</v>
+      </c>
+      <c r="H21" s="25">
+        <v>0</v>
+      </c>
+      <c r="I21" s="25">
+        <v>2</v>
+      </c>
+      <c r="J21" s="24"/>
+      <c r="K21" s="25">
+        <v>20</v>
+      </c>
+      <c r="L21" s="15" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="24" t="s">
+        <v>328</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>325</v>
+      </c>
+      <c r="C22" s="25">
+        <v>1</v>
+      </c>
+      <c r="D22" s="25">
+        <v>3</v>
+      </c>
+      <c r="E22" s="25">
+        <v>5</v>
+      </c>
+      <c r="F22" s="25">
         <v>3</v>
       </c>
       <c r="G22" s="21">
-        <v>7</v>
-      </c>
-      <c r="H22" s="4">
-        <v>1</v>
-      </c>
-      <c r="I22" s="4">
-        <v>2</v>
-      </c>
-      <c r="K22" s="4">
-        <v>10</v>
-      </c>
-      <c r="M22" s="4" t="s">
-        <v>57</v>
+        <v>60</v>
+      </c>
+      <c r="H22" s="25">
+        <v>0</v>
+      </c>
+      <c r="I22" s="25">
+        <v>2</v>
+      </c>
+      <c r="J22" s="24">
+        <v>2</v>
+      </c>
+      <c r="K22" s="25">
+        <v>40</v>
+      </c>
+      <c r="L22" s="15" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4691,98 +4781,63 @@
     </row>
     <row r="24" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C24" s="4">
         <v>1</v>
       </c>
       <c r="D24" s="4">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="E24" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F24" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G24" s="21">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="H24" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" s="4">
-        <v>0</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="K24" s="4">
-        <v>25</v>
-      </c>
-      <c r="L24" s="4" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" s="4">
-        <v>1</v>
-      </c>
-      <c r="D25" s="4">
-        <v>3</v>
-      </c>
-      <c r="E25" s="4">
-        <v>5</v>
-      </c>
-      <c r="F25" s="4">
-        <v>5</v>
-      </c>
-      <c r="G25" s="21">
-        <v>16</v>
-      </c>
-      <c r="H25" s="4">
-        <v>0</v>
-      </c>
-      <c r="I25" s="4">
-        <v>0</v>
-      </c>
-      <c r="K25" s="4">
-        <v>20</v>
-      </c>
-      <c r="L25" s="15" t="s">
-        <v>320</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="M24" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G25" s="22"/>
     </row>
     <row r="26" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C26" s="4">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="D26" s="4">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="E26" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F26" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G26" s="21">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="H26" s="4">
         <v>0</v>
@@ -4790,86 +4845,95 @@
       <c r="I26" s="4">
         <v>0</v>
       </c>
+      <c r="J26" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="K26" s="4">
-        <v>10</v>
-      </c>
-      <c r="L26" s="15" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G27" s="22"/>
+        <v>25</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="4">
+        <v>1</v>
+      </c>
+      <c r="D27" s="4">
+        <v>3</v>
+      </c>
+      <c r="E27" s="4">
+        <v>5</v>
+      </c>
+      <c r="F27" s="4">
+        <v>5</v>
+      </c>
+      <c r="G27" s="21">
+        <v>16</v>
+      </c>
+      <c r="H27" s="4">
+        <v>0</v>
+      </c>
+      <c r="I27" s="4">
+        <v>0</v>
+      </c>
+      <c r="K27" s="4">
+        <v>20</v>
+      </c>
+      <c r="L27" s="15" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="28" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C28" s="4">
-        <v>1.5</v>
+        <v>0.7</v>
       </c>
       <c r="D28" s="4">
         <v>3</v>
       </c>
       <c r="E28" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F28" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G28" s="21">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H28" s="4">
         <v>0</v>
       </c>
       <c r="I28" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K28" s="4">
-        <v>15</v>
-      </c>
-      <c r="L28" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C29" s="4">
-        <v>1.5</v>
-      </c>
-      <c r="D29" s="4">
-        <v>3</v>
-      </c>
-      <c r="E29" s="4">
-        <v>3</v>
-      </c>
-      <c r="F29" s="4">
-        <v>3</v>
-      </c>
-      <c r="G29" s="21">
-        <v>15</v>
-      </c>
-      <c r="H29" s="4">
-        <v>0</v>
-      </c>
-      <c r="I29" s="4">
-        <v>2</v>
-      </c>
-      <c r="K29" s="4">
-        <v>20</v>
-      </c>
-      <c r="L29" s="4" t="s">
-        <v>72</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="L28" s="15" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G29" s="22"/>
     </row>
     <row r="30" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>73</v>
+        <v>68</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="C30" s="4">
         <v>1.5</v>
@@ -4884,24 +4948,24 @@
         <v>3</v>
       </c>
       <c r="G30" s="21">
+        <v>12</v>
+      </c>
+      <c r="H30" s="4">
+        <v>0</v>
+      </c>
+      <c r="I30" s="4">
+        <v>2</v>
+      </c>
+      <c r="K30" s="4">
         <v>15</v>
       </c>
-      <c r="H30" s="4">
-        <v>0</v>
-      </c>
-      <c r="I30" s="4">
-        <v>2</v>
-      </c>
-      <c r="K30" s="4">
-        <v>20</v>
-      </c>
       <c r="L30" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C31" s="4">
         <v>1.5</v>
@@ -4928,12 +4992,12 @@
         <v>20</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C32" s="4">
         <v>1.5</v>
@@ -4960,12 +5024,12 @@
         <v>20</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C33" s="4">
         <v>1.5</v>
@@ -4992,12 +5056,12 @@
         <v>20</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C34" s="4">
         <v>1.5</v>
@@ -5024,12 +5088,12 @@
         <v>20</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C35" s="4">
         <v>1.5</v>
@@ -5056,15 +5120,15 @@
         <v>20</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C36" s="4">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D36" s="4">
         <v>3</v>
@@ -5088,506 +5152,494 @@
         <v>20</v>
       </c>
       <c r="L36" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G37" s="22"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C37" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="D37" s="4">
+        <v>3</v>
+      </c>
+      <c r="E37" s="4">
+        <v>3</v>
+      </c>
+      <c r="F37" s="4">
+        <v>3</v>
+      </c>
+      <c r="G37" s="21">
+        <v>15</v>
+      </c>
+      <c r="H37" s="4">
+        <v>0</v>
+      </c>
+      <c r="I37" s="4">
+        <v>2</v>
+      </c>
+      <c r="K37" s="4">
+        <v>20</v>
+      </c>
+      <c r="L37" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="38" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C38" s="4">
-        <v>3</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>43</v>
+        <v>1</v>
+      </c>
+      <c r="D38" s="4">
+        <v>3</v>
       </c>
       <c r="E38" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F38" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G38" s="21">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="H38" s="4">
         <v>0</v>
       </c>
       <c r="I38" s="4">
-        <v>0</v>
-      </c>
-      <c r="J38" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="K38" s="4" t="s">
-        <v>43</v>
+        <v>2</v>
+      </c>
+      <c r="K38" s="4">
+        <v>20</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C39" s="4">
-        <v>1</v>
-      </c>
-      <c r="D39" s="4">
-        <v>3</v>
-      </c>
-      <c r="E39" s="4">
-        <v>3</v>
-      </c>
-      <c r="F39" s="4">
-        <v>3</v>
-      </c>
-      <c r="G39" s="21">
-        <v>8</v>
-      </c>
-      <c r="H39" s="4">
-        <v>0</v>
-      </c>
-      <c r="I39" s="4">
-        <v>1</v>
-      </c>
-      <c r="K39" s="4">
-        <v>10</v>
-      </c>
-      <c r="L39" s="4" t="s">
-        <v>95</v>
-      </c>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G39" s="22"/>
     </row>
     <row r="40" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C40" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="D40" s="4">
-        <v>2.9</v>
+        <v>3</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="E40" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F40" s="4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G40" s="21">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="H40" s="4">
         <v>0</v>
       </c>
       <c r="I40" s="4">
-        <v>2</v>
-      </c>
-      <c r="K40" s="4">
-        <v>20</v>
+        <v>0</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K40" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="L40" s="4" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C41" s="4">
+        <v>1</v>
+      </c>
+      <c r="D41" s="4">
+        <v>3</v>
+      </c>
+      <c r="E41" s="4">
+        <v>3</v>
+      </c>
+      <c r="F41" s="4">
+        <v>3</v>
+      </c>
+      <c r="G41" s="21">
+        <v>8</v>
+      </c>
+      <c r="H41" s="4">
+        <v>0</v>
+      </c>
+      <c r="I41" s="4">
+        <v>1</v>
+      </c>
+      <c r="K41" s="4">
+        <v>10</v>
+      </c>
+      <c r="L41" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C42" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="D42" s="4">
+        <v>2.9</v>
+      </c>
+      <c r="E42" s="4">
+        <v>4</v>
+      </c>
+      <c r="F42" s="4">
+        <v>4</v>
+      </c>
+      <c r="G42" s="21">
+        <v>16</v>
+      </c>
+      <c r="H42" s="4">
+        <v>0</v>
+      </c>
+      <c r="I42" s="4">
+        <v>2</v>
+      </c>
+      <c r="K42" s="4">
+        <v>20</v>
+      </c>
+      <c r="L42" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B43" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C41" s="4">
+      <c r="C43" s="4">
         <v>0.9</v>
       </c>
-      <c r="D41" s="4">
+      <c r="D43" s="4">
         <v>2.8</v>
       </c>
-      <c r="E41" s="4">
+      <c r="E43" s="4">
         <v>5</v>
       </c>
-      <c r="F41" s="4">
+      <c r="F43" s="4">
         <v>5</v>
       </c>
-      <c r="G41" s="21">
+      <c r="G43" s="21">
         <v>28</v>
       </c>
-      <c r="H41" s="4">
-        <v>1</v>
-      </c>
-      <c r="I41" s="4">
-        <v>3</v>
-      </c>
-      <c r="K41" s="4">
+      <c r="H43" s="4">
+        <v>1</v>
+      </c>
+      <c r="I43" s="4">
+        <v>3</v>
+      </c>
+      <c r="K43" s="4">
         <v>35</v>
       </c>
-      <c r="L41" s="4" t="s">
+      <c r="L43" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
-        <v>323</v>
-      </c>
-      <c r="B42" s="7" t="s">
+    <row r="44" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="B44" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C42" s="8">
+      <c r="C44" s="8">
         <v>0.8</v>
       </c>
-      <c r="D42" s="8">
+      <c r="D44" s="8">
         <v>2.7</v>
       </c>
-      <c r="E42" s="9">
+      <c r="E44" s="9">
         <v>6</v>
       </c>
-      <c r="F42" s="9">
+      <c r="F44" s="9">
         <v>6</v>
       </c>
-      <c r="G42" s="21">
+      <c r="G44" s="21">
         <v>44</v>
       </c>
-      <c r="H42" s="9">
-        <v>1</v>
-      </c>
-      <c r="I42" s="9">
+      <c r="H44" s="9">
+        <v>1</v>
+      </c>
+      <c r="I44" s="9">
         <v>4</v>
       </c>
-      <c r="J42" s="6"/>
-      <c r="K42" s="9">
+      <c r="J44" s="6"/>
+      <c r="K44" s="9">
         <v>55</v>
       </c>
-      <c r="L42" s="10" t="s">
+      <c r="L44" s="10" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
+    <row r="45" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B45" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C43" s="8">
+      <c r="C45" s="8">
         <v>0.8</v>
       </c>
-      <c r="D43" s="8">
+      <c r="D45" s="8">
         <v>2.6</v>
       </c>
-      <c r="E43" s="8">
+      <c r="E45" s="8">
         <v>7</v>
       </c>
-      <c r="F43" s="8">
+      <c r="F45" s="8">
         <v>7</v>
       </c>
-      <c r="G43" s="21">
+      <c r="G45" s="21">
         <v>64</v>
       </c>
-      <c r="H43" s="9">
-        <v>1</v>
-      </c>
-      <c r="I43" s="8">
+      <c r="H45" s="9">
+        <v>1</v>
+      </c>
+      <c r="I45" s="8">
         <v>5</v>
       </c>
-      <c r="J43" s="6"/>
-      <c r="K43" s="8">
+      <c r="J45" s="6"/>
+      <c r="K45" s="8">
         <v>80</v>
       </c>
-      <c r="L43" s="11" t="s">
+      <c r="L45" s="11" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
+    <row r="46" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B46" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C44" s="4">
-        <v>1</v>
-      </c>
-      <c r="D44" s="4">
-        <v>3</v>
-      </c>
-      <c r="E44" s="4">
+      <c r="C46" s="4">
+        <v>1</v>
+      </c>
+      <c r="D46" s="4">
+        <v>3</v>
+      </c>
+      <c r="E46" s="4">
         <v>4</v>
       </c>
-      <c r="F44" s="4">
+      <c r="F46" s="4">
         <v>4</v>
       </c>
-      <c r="G44" s="21">
-        <v>14</v>
-      </c>
-      <c r="H44" s="4">
-        <v>0</v>
-      </c>
-      <c r="I44" s="4">
+      <c r="G46" s="21">
+        <v>20</v>
+      </c>
+      <c r="H46" s="4">
+        <v>0</v>
+      </c>
+      <c r="I46" s="4">
         <v>4</v>
       </c>
-      <c r="K44" s="4">
+      <c r="K46" s="4">
         <v>25</v>
       </c>
-      <c r="L44" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G45" s="22"/>
-    </row>
-    <row r="46" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
+      <c r="L46" s="4" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G47" s="22"/>
+    </row>
+    <row r="48" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B48" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C46" s="4">
-        <v>2</v>
-      </c>
-      <c r="D46" s="4">
-        <v>3</v>
-      </c>
-      <c r="E46" s="4">
-        <v>2</v>
-      </c>
-      <c r="F46" s="4">
-        <v>3</v>
-      </c>
-      <c r="G46" s="21">
+      <c r="C48" s="4">
+        <v>2</v>
+      </c>
+      <c r="D48" s="4">
+        <v>3</v>
+      </c>
+      <c r="E48" s="4">
+        <v>2</v>
+      </c>
+      <c r="F48" s="4">
+        <v>3</v>
+      </c>
+      <c r="G48" s="21">
         <v>8</v>
       </c>
-      <c r="H46" s="4">
-        <v>0</v>
-      </c>
-      <c r="I46" s="4">
-        <v>0</v>
-      </c>
-      <c r="J46" s="4"/>
-      <c r="K46" s="4">
+      <c r="H48" s="4">
+        <v>0</v>
+      </c>
+      <c r="I48" s="4">
+        <v>0</v>
+      </c>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4">
         <v>10</v>
       </c>
-      <c r="L46" s="4" t="s">
+      <c r="L48" s="4" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C47" s="4">
-        <v>2</v>
-      </c>
-      <c r="D47" s="4">
-        <v>3</v>
-      </c>
-      <c r="E47" s="4">
-        <v>2</v>
-      </c>
-      <c r="F47" s="4">
-        <v>3</v>
-      </c>
-      <c r="G47" s="21">
-        <v>8</v>
-      </c>
-      <c r="H47" s="4">
-        <v>0</v>
-      </c>
-      <c r="I47" s="4">
-        <v>0</v>
-      </c>
-      <c r="J47" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="K47" s="4">
-        <v>10</v>
-      </c>
-      <c r="L47" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E48" s="4">
-        <v>1</v>
-      </c>
-      <c r="F48" s="4">
-        <v>0</v>
-      </c>
-      <c r="G48" s="21">
-        <v>1</v>
-      </c>
-      <c r="H48" s="4">
-        <v>0</v>
-      </c>
-      <c r="I48" s="4">
-        <v>1</v>
-      </c>
-      <c r="K48" s="4">
-        <v>5</v>
-      </c>
-      <c r="L48" s="4" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C49" s="4">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="D49" s="4">
         <v>3</v>
       </c>
       <c r="E49" s="4">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F49" s="4">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G49" s="21">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="H49" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I49" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="K49" s="4">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="L49" s="4" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>139</v>
+        <v>116</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="C50" s="4">
-        <v>2</v>
-      </c>
-      <c r="D50" s="4">
-        <v>3</v>
+        <v>117</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="E50" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F50" s="4">
         <v>0</v>
       </c>
       <c r="G50" s="21">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H50" s="4">
         <v>0</v>
       </c>
       <c r="I50" s="4">
-        <v>0</v>
-      </c>
-      <c r="J50" s="4" t="s">
-        <v>115</v>
+        <v>1</v>
       </c>
       <c r="K50" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="L50" s="4" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C51" s="4">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="D51" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E51" s="4">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F51" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G51" s="21">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="H51" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I51" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="K51" s="4">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="L51" s="4" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C52" s="4">
         <v>2</v>
       </c>
-      <c r="D52" s="4" t="s">
-        <v>144</v>
+      <c r="D52" s="4">
+        <v>3</v>
       </c>
       <c r="E52" s="4">
         <v>2</v>
       </c>
-      <c r="F52" s="4" t="s">
-        <v>145</v>
+      <c r="F52" s="4">
+        <v>0</v>
       </c>
       <c r="G52" s="21">
         <v>8</v>
@@ -5599,16 +5651,92 @@
         <v>0</v>
       </c>
       <c r="J52" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="K52" s="4">
+        <v>10</v>
+      </c>
+      <c r="L52" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C53" s="4">
+        <v>2</v>
+      </c>
+      <c r="D53" s="4">
+        <v>6</v>
+      </c>
+      <c r="E53" s="4">
+        <v>2</v>
+      </c>
+      <c r="F53" s="4">
+        <v>6</v>
+      </c>
+      <c r="G53" s="21">
+        <v>8</v>
+      </c>
+      <c r="H53" s="4">
+        <v>0</v>
+      </c>
+      <c r="I53" s="4">
+        <v>0</v>
+      </c>
+      <c r="J53" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="K53" s="4">
+        <v>10</v>
+      </c>
+      <c r="L53" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C54" s="4">
+        <v>2</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E54" s="4">
+        <v>2</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="G54" s="21">
+        <v>8</v>
+      </c>
+      <c r="H54" s="4">
+        <v>0</v>
+      </c>
+      <c r="I54" s="4">
+        <v>0</v>
+      </c>
+      <c r="J54" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="K52" s="4">
+      <c r="K54" s="4">
         <v>8</v>
       </c>
-      <c r="L52" s="4" t="s">
+      <c r="L54" s="4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="55" spans="1:12" ht="12.75" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6133,271 +6261,294 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA21"/>
+  <dimension ref="A1:AA23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="118" style="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>186</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="23" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>159</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C2" s="23" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>159</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="23" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>159</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="23" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>159</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="23" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>159</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="23" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>159</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="23" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>327</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>322</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="B8" s="4" t="s">
+      <c r="C10" s="23" t="s">
         <v>199</v>
       </c>
-      <c r="C8" s="4" t="s">
+    </row>
+    <row r="11" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="B11" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="B10" s="4" t="s">
+      <c r="C12" s="23" t="s">
         <v>202</v>
       </c>
-      <c r="C10" s="4" t="s">
+    </row>
+    <row r="13" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="B11" s="4" t="s">
+      <c r="C13" s="23" t="s">
         <v>204</v>
       </c>
-      <c r="C11" s="4" t="s">
+    </row>
+    <row r="14" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="B14" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="C14" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="C12" s="4" t="s">
+    </row>
+    <row r="15" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="B13" s="4" t="s">
+      <c r="C15" s="23" t="s">
         <v>209</v>
       </c>
-      <c r="C13" s="4" t="s">
+    </row>
+    <row r="16" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="B14" s="4" t="s">
+      <c r="C16" s="23" t="s">
         <v>211</v>
       </c>
-      <c r="C14" s="4" t="s">
+    </row>
+    <row r="17" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C17" s="23" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C15" s="15" t="s">
+    <row r="18" spans="1:27" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="B16" s="4" t="s">
+      <c r="C18" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="C16" s="4" t="s">
+    </row>
+    <row r="19" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="B17" s="4" t="s">
+      <c r="C19" s="23" t="s">
         <v>216</v>
       </c>
-      <c r="C17" s="4" t="s">
+    </row>
+    <row r="20" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="B18" s="5" t="s">
+      <c r="C20" s="26" t="s">
         <v>218</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="D20" s="16"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="6"/>
+      <c r="U20" s="6"/>
+      <c r="V20" s="6"/>
+      <c r="W20" s="6"/>
+      <c r="X20" s="6"/>
+      <c r="Y20" s="6"/>
+      <c r="Z20" s="6"/>
+      <c r="AA20" s="6"/>
+    </row>
+    <row r="21" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="6"/>
-      <c r="R18" s="6"/>
-      <c r="S18" s="6"/>
-      <c r="T18" s="6"/>
-      <c r="U18" s="6"/>
-      <c r="V18" s="6"/>
-      <c r="W18" s="6"/>
-      <c r="X18" s="6"/>
-      <c r="Y18" s="6"/>
-      <c r="Z18" s="6"/>
-      <c r="AA18" s="6"/>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="B19" s="4" t="s">
+      <c r="C21" s="23" t="s">
         <v>220</v>
       </c>
-      <c r="C19" s="4" t="s">
+    </row>
+    <row r="22" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+      <c r="C22" s="23" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="C20" s="4" t="s">
+      <c r="B23" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23" s="23" t="s">
         <v>223</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -6410,10 +6561,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:E25"/>
+  <dimension ref="A2:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6423,14 +6574,14 @@
     <col min="5" max="5" width="71.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>0</v>
@@ -6440,219 +6591,228 @@
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="14" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B6" s="15" t="s">
+        <v>333</v>
+      </c>
+      <c r="C6" s="15"/>
+      <c r="D6" s="14" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B7" s="4" t="s">
         <v>226</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="14" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="4" t="s">
-        <v>230</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="14" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C9" s="4"/>
-      <c r="D9" s="4" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D9" s="14" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
-        <v>316</v>
+        <v>232</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
-        <v>236</v>
+        <v>312</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B13" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B14" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="14" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B13" s="4" t="s">
+    <row r="15" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B15" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="14" t="s">
+      <c r="C15" s="4"/>
+      <c r="D15" s="4" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B16" s="4" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B14" s="4" t="s">
+      <c r="D16" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4" t="s">
+    </row>
+    <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B17" s="4" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="4" t="s">
+      <c r="C17" s="4"/>
+      <c r="D17" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="D15" s="4" t="s">
+    </row>
+    <row r="18" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B18" s="15" t="s">
+        <v>314</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="14" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B19" s="4" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B16" s="4" t="s">
+      <c r="C19" s="4"/>
+      <c r="D19" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4" t="s">
+    </row>
+    <row r="20" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="18" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B17" s="15" t="s">
-        <v>318</v>
-      </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="14" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="4" t="s">
+    <row r="22" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4" t="s">
+      <c r="B22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="18" t="s">
+      <c r="E22" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+      <c r="B23" s="4" t="s">
         <v>251</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="C22" s="4">
-        <v>24</v>
-      </c>
-      <c r="D22" s="4">
-        <v>6</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>256</v>
       </c>
       <c r="C23" s="4">
         <v>24</v>
       </c>
       <c r="D23" s="4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>258</v>
+      <c r="C24" s="4">
+        <v>24</v>
       </c>
       <c r="D24" s="4">
+        <v>3</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="D25" s="4">
         <v>8</v>
       </c>
-      <c r="E24" s="23" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="C25">
+      <c r="E25" s="23" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="C26">
         <v>12</v>
       </c>
-      <c r="D25" s="15">
+      <c r="D26" s="15">
         <v>6</v>
       </c>
-      <c r="E25" s="15" t="s">
-        <v>315</v>
+      <c r="E26" s="15" t="s">
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -6667,13 +6827,15 @@
   </sheetPr>
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65:L65"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B1" s="4">
         <f>6*9</f>
@@ -6686,7 +6848,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B2" s="12">
         <f>18*7</f>
@@ -6695,7 +6857,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B3" s="12">
         <f>10*2</f>
@@ -6704,172 +6866,172 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C32" s="4" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B42" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B43" s="4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B45" s="4" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B46" s="4" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -6879,42 +7041,42 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B49" s="4" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B50" s="4" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B57" s="4" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B59" s="4" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -6939,22 +7101,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>302</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="98.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -6962,19 +7124,19 @@
         <v>44682</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>161</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added war wasp, some balance changes. Included new pictures. Added primer
</commit_message>
<xml_diff>
--- a/unit stats.xlsx
+++ b/unit stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas\Documents\wargame\wargame-tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E754037-514F-42E1-8B41-A8C39B3D3392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E191B980-924B-4B30-B629-A5682A9D15AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20520" yWindow="4665" windowWidth="20640" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="342">
   <si>
     <t>Name</t>
   </si>
@@ -1053,6 +1053,18 @@
   </si>
   <si>
     <t>+0.5 Armor</t>
+  </si>
+  <si>
+    <t>War Wasp</t>
+  </si>
+  <si>
+    <t>May take a War Wasp</t>
+  </si>
+  <si>
+    <t>Mount usable by the Emissary. May not otherwise be selected</t>
+  </si>
+  <si>
+    <t>6R</t>
   </si>
 </sst>
 </file>
@@ -4063,9 +4075,9 @@
   </sheetPr>
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A44" sqref="A44:XFD44"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J53" sqref="J53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4314,6 +4326,9 @@
       <c r="L6" s="4" t="s">
         <v>135</v>
       </c>
+      <c r="M6" s="15" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="7" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -4335,7 +4350,7 @@
         <v>4</v>
       </c>
       <c r="G7" s="21">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="H7" s="4">
         <v>0</v>
@@ -4354,7 +4369,39 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G8" s="22"/>
+      <c r="A8" s="15" t="s">
+        <v>338</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>340</v>
+      </c>
+      <c r="C8" s="15">
+        <v>0.75</v>
+      </c>
+      <c r="D8" s="15">
+        <v>3</v>
+      </c>
+      <c r="E8" s="15">
+        <v>4</v>
+      </c>
+      <c r="F8" s="15">
+        <v>4</v>
+      </c>
+      <c r="G8" s="22">
+        <v>16</v>
+      </c>
+      <c r="H8" s="15">
+        <v>1</v>
+      </c>
+      <c r="I8" s="15">
+        <v>0</v>
+      </c>
+      <c r="K8" s="15">
+        <v>20</v>
+      </c>
+      <c r="L8" s="15" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G9" s="22"/>
@@ -5651,7 +5698,7 @@
         <v>0</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>115</v>
+        <v>341</v>
       </c>
       <c r="K52" s="4">
         <v>10</v>
@@ -6563,7 +6610,7 @@
   </sheetPr>
   <dimension ref="A2:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -7091,11 +7138,14 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="3" width="20.85546875" customWidth="1"/>
+    <col min="6" max="6" width="85.140625" customWidth="1"/>
     <col min="7" max="7" width="38.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7119,7 +7169,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="98.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="221.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="19">
         <v>44682</v>
       </c>
@@ -7135,7 +7185,7 @@
       <c r="E2" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="23" t="s">
         <v>306</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Included Royal Emissary image
</commit_message>
<xml_diff>
--- a/unit stats.xlsx
+++ b/unit stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas\Documents\wargame\wargame-tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E191B980-924B-4B30-B629-A5682A9D15AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9AB7D6-BB8E-4AB6-B176-259C237BDB7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="343">
   <si>
     <t>Name</t>
   </si>
@@ -1065,6 +1065,9 @@
   </si>
   <si>
     <t>6R</t>
+  </si>
+  <si>
+    <t>Root, Seed 16, When Attacking, this unit may spend additional AP.  For each 3 AP spent, increase the Attack's Range by 3 inches</t>
   </si>
 </sst>
 </file>
@@ -4077,7 +4080,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J53" sqref="J53"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4312,7 +4315,7 @@
         <v>4</v>
       </c>
       <c r="G6" s="21">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H6" s="4">
         <v>1</v>
@@ -4321,7 +4324,7 @@
         <v>2</v>
       </c>
       <c r="K6" s="4">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="L6" s="4" t="s">
         <v>135</v>
@@ -5704,7 +5707,7 @@
         <v>10</v>
       </c>
       <c r="L52" s="4" t="s">
-        <v>112</v>
+        <v>342</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -6311,7 +6314,7 @@
   <dimension ref="A1:AA23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated stats and filled out some hive court unit descriptions in the manual
</commit_message>
<xml_diff>
--- a/unit stats.xlsx
+++ b/unit stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas\Documents\wargame\wargame-tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A497AAD-7259-4BB6-96C3-27CB6DEAD51C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2BE83D-8614-42A9-8EE7-99D72F534CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="359">
   <si>
     <t>Name</t>
   </si>
@@ -818,15 +818,9 @@
     <t>shaman x2</t>
   </si>
   <si>
-    <t>Tunnel Bruiser x4</t>
-  </si>
-  <si>
     <t>Tunnel Delver x2</t>
   </si>
   <si>
-    <t>Tunnel Mite x6</t>
-  </si>
-  <si>
     <t>Wanderer w/ Rifle (4pts) 14 pts x 14 = 196</t>
   </si>
   <si>
@@ -1110,6 +1104,18 @@
   </si>
   <si>
     <t>5R</t>
+  </si>
+  <si>
+    <t>Tunnel Sapper x2</t>
+  </si>
+  <si>
+    <t>Tunnel Worm x3 OR Tunnel bruiser</t>
+  </si>
+  <si>
+    <t>Tunnel Mite x8</t>
+  </si>
+  <si>
+    <t>Tunnel Worm x4</t>
   </si>
 </sst>
 </file>
@@ -4141,9 +4147,9 @@
   </sheetPr>
   <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J52" sqref="J52"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4393,7 +4399,7 @@
         <v>135</v>
       </c>
       <c r="M6" s="15" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4436,10 +4442,10 @@
     </row>
     <row r="8" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
+        <v>334</v>
+      </c>
+      <c r="B8" s="15" t="s">
         <v>336</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>338</v>
       </c>
       <c r="C8" s="15">
         <v>0.75</v>
@@ -4504,7 +4510,7 @@
         <v>15</v>
       </c>
       <c r="L10" s="15" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4568,7 +4574,7 @@
         <v>15</v>
       </c>
       <c r="L12" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4740,7 +4746,7 @@
         <v>7</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4817,10 +4823,10 @@
     </row>
     <row r="21" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C21" s="25">
         <v>1</v>
@@ -4848,15 +4854,15 @@
         <v>20</v>
       </c>
       <c r="L21" s="15" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="24" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C22" s="25">
         <v>1</v>
@@ -4886,7 +4892,7 @@
         <v>40</v>
       </c>
       <c r="L22" s="15" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4935,7 +4941,7 @@
         <v>58</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C26" s="4">
         <v>1</v>
@@ -4944,7 +4950,7 @@
         <v>2.5</v>
       </c>
       <c r="E26" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" s="4">
         <v>6</v>
@@ -4965,7 +4971,7 @@
         <v>30</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4973,7 +4979,7 @@
         <v>62</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C27" s="4">
         <v>1</v>
@@ -4982,7 +4988,7 @@
         <v>6</v>
       </c>
       <c r="E27" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" s="4">
         <v>4</v>
@@ -5000,7 +5006,7 @@
         <v>25</v>
       </c>
       <c r="L27" s="15" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -5008,7 +5014,7 @@
         <v>65</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C28" s="4">
         <v>0.8</v>
@@ -5035,15 +5041,15 @@
         <v>5</v>
       </c>
       <c r="L28" s="15" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C29" s="15">
         <v>1</v>
@@ -5070,15 +5076,15 @@
         <v>10</v>
       </c>
       <c r="L29" s="15" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C30" s="15">
         <v>1</v>
@@ -5087,7 +5093,7 @@
         <v>6</v>
       </c>
       <c r="E30" s="15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F30" s="15">
         <v>4</v>
@@ -5105,12 +5111,12 @@
         <v>20</v>
       </c>
       <c r="L30" s="15" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G31" s="22" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -5552,7 +5558,7 @@
     </row>
     <row r="46" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>103</v>
@@ -5654,7 +5660,7 @@
         <v>25</v>
       </c>
       <c r="L48" s="4" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -5693,7 +5699,7 @@
         <v>10</v>
       </c>
       <c r="L50" s="4" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -5725,13 +5731,13 @@
         <v>0</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="K51" s="4">
         <v>10</v>
       </c>
       <c r="L51" s="4" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -5766,7 +5772,7 @@
         <v>5</v>
       </c>
       <c r="L52" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -5836,13 +5842,13 @@
         <v>0</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="K54" s="4">
         <v>10</v>
       </c>
       <c r="L54" s="4" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -5918,7 +5924,7 @@
         <v>8</v>
       </c>
       <c r="L56" s="4" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="12.75" x14ac:dyDescent="0.2"/>
@@ -6506,7 +6512,7 @@
         <v>187</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
@@ -6561,7 +6567,7 @@
         <v>196</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
@@ -6569,10 +6575,10 @@
         <v>158</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
@@ -6580,10 +6586,10 @@
         <v>158</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
@@ -6602,10 +6608,10 @@
         <v>199</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
@@ -6810,16 +6816,16 @@
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="14" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B6" s="15" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="14" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -6860,11 +6866,11 @@
     </row>
     <row r="11" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -6900,7 +6906,7 @@
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -6922,11 +6928,11 @@
     </row>
     <row r="18" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B18" s="15" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="14" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
@@ -6991,7 +6997,7 @@
         <v>3</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -7008,7 +7014,7 @@
         <v>8</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
@@ -7025,7 +7031,7 @@
         <v>6</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -7038,19 +7044,23 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C59"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65:L65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="37.85546875" style="27" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="23" t="s">
         <v>256</v>
       </c>
-      <c r="B1" s="4">
+      <c r="B1" s="23">
         <f>6*9</f>
         <v>54</v>
       </c>
@@ -7059,8 +7069,8 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="s">
         <v>257</v>
       </c>
       <c r="B2" s="12">
@@ -7068,8 +7078,8 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="23" t="s">
         <v>258</v>
       </c>
       <c r="B3" s="12">
@@ -7077,219 +7087,251 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="23" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="B6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="B7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="23" t="s">
+        <v>355</v>
+      </c>
+      <c r="B8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="23" t="s">
+        <v>358</v>
+      </c>
+      <c r="B9">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="23" t="s">
+        <v>356</v>
+      </c>
+      <c r="B10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="23"/>
+    </row>
+    <row r="12" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="23" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+    <row r="14" spans="1:3" ht="71.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="23" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+    <row r="17" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="23" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+    <row r="19" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="23" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+    <row r="21" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="23" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+    <row r="23" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="23" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="23" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+    <row r="25" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="23" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="23" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="23" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
+    <row r="29" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C29" s="4" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
+    <row r="30" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="23" t="s">
+        <v>269</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="23" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="C28" s="4" t="s">
+    </row>
+    <row r="32" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="23" t="s">
+        <v>272</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
+    <row r="33" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="23" t="s">
+        <v>273</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="C29" s="4" t="s">
+    </row>
+    <row r="34" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="23" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
+      <c r="C34" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
+    </row>
+    <row r="35" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A36" s="23" t="s">
         <v>276</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C32" s="4" t="s">
+    </row>
+    <row r="37" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A37" s="23" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
+    <row r="38" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A38" s="23" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
+    <row r="39" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A39" s="23" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
+    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="23" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
+    <row r="43" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A44" s="23" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
+      <c r="B44" s="4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B45" s="4" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
+    <row r="46" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A47" s="23" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B42" s="4" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B43" s="4" t="s">
+      <c r="B47" s="4" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="4" t="s">
+    <row r="48" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B48" s="4" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B45" s="4" t="s">
+    <row r="49" spans="1:2" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="50" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A50" s="23" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B46" s="4" t="s">
+      <c r="B50" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B51" s="4" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="4" t="s">
+    <row r="52" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B52" s="4" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B48" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B49" s="4" t="s">
+    <row r="54" spans="1:2" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="55" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="23" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B50" s="4" t="s">
+    <row r="56" spans="1:2" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="57" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="23" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="4" t="s">
+    <row r="58" spans="1:2" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="59" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A59" s="23" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="4" t="s">
+      <c r="B59" s="4" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="4" t="s">
+    <row r="60" spans="1:2" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="61" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A61" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="B61" s="4" t="s">
         <v>293</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B57" s="4" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" s="4" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B59" s="4" t="s">
-        <v>295</v>
       </c>
     </row>
   </sheetData>
@@ -7317,22 +7359,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>299</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="221.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -7340,19 +7382,19 @@
         <v>44682</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>160</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the Plants a lot to account for the game testing Ron and I had.  Big changes were the unification of Seed costs to 12, and the filling out of the seed cannon and seedblower as long-range and short-range guns.  Also dropped the points costs for the Fleshcrafter Priest to allow for more flexible armies in the 100-point range. Updated the FCP abilities sheet to make choices more balanced.
</commit_message>
<xml_diff>
--- a/unit stats.xlsx
+++ b/unit stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas\Documents\wargame\wargame-tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2BE83D-8614-42A9-8EE7-99D72F534CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523B5E79-7077-4E8F-8524-3911AEB76853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="370">
   <si>
     <t>Name</t>
   </si>
@@ -464,9 +464,6 @@
     <t>Shoots a burst of spores/acid (idk yet).  Sets up a direct damage area effect until EOR</t>
   </si>
   <si>
-    <t>Root, Seed 16, True Damage 4</t>
-  </si>
-  <si>
     <t>Mine Plant</t>
   </si>
   <si>
@@ -725,9 +722,6 @@
     <t>Bloated Body</t>
   </si>
   <si>
-    <t>+2 Wounds</t>
-  </si>
-  <si>
     <t>Autonomous Twitch Fibers</t>
   </si>
   <si>
@@ -743,21 +737,12 @@
     <t>Bone Spitters</t>
   </si>
   <si>
-    <t>R12 P + 1 AP1</t>
-  </si>
-  <si>
     <t>Tentacles</t>
   </si>
   <si>
-    <t>Units within Melee range attempting to move out of Melee range cannot, provided that you choose to deny the movement AND the unit attempting to restrain the fleeing model has a Power greater than or equal to the fleeing model's Power</t>
-  </si>
-  <si>
     <t>Sub-Brain Installation</t>
   </si>
   <si>
-    <t>+2 Activation Points</t>
-  </si>
-  <si>
     <t>Restoration Gene</t>
   </si>
   <si>
@@ -776,9 +761,6 @@
     <t>Pneumatic Bone Spitters</t>
   </si>
   <si>
-    <t>Gives Attack R24.</t>
-  </si>
-  <si>
     <t>Spells</t>
   </si>
   <si>
@@ -962,9 +944,6 @@
     <t>Select two models you control with Reshape that are within 3" of one another.  Remove both of them from the game and add a new model in its place.  The new model has Reshape X, where X is the total Reshape value of the sacrificed models.  For Power, Toughness, Armor, Damage, choose the highest of the sacrificed models.  For Attack Cost and Move Cost, choose the lowest of the two.  For Wounds, add the total maximum Wounds of each sacrificed model.  The model starts with  the total Damage of the combined units.  You may use up to one felled model for this.</t>
   </si>
   <si>
-    <t xml:space="preserve">Remove up to 4 damage from a creature you control with Reshape. </t>
-  </si>
-  <si>
     <t>You may remove a model with Reshape 2+ from the battlefield.  For every two levels of Reshape, create a Flesh Golem</t>
   </si>
   <si>
@@ -1037,9 +1016,6 @@
     <t>+1 Power</t>
   </si>
   <si>
-    <t>Grants Regeneration 2</t>
-  </si>
-  <si>
     <t>+0.5 Armor</t>
   </si>
   <si>
@@ -1052,9 +1028,6 @@
     <t>Mount usable by the Emissary. May not otherwise be selected</t>
   </si>
   <si>
-    <t>Root, Seed 16, When Attacking, this unit may spend additional AP.  For each 3 AP spent, increase the Attack's Range by 3 inches</t>
-  </si>
-  <si>
     <t>Tunneling cave beast. Functions as a portal. 40 MM base</t>
   </si>
   <si>
@@ -1097,15 +1070,9 @@
     <t>You may take one Root Cluster for free.  Starts rooted.  Seed 8</t>
   </si>
   <si>
-    <t>2R</t>
-  </si>
-  <si>
     <t>Root, Seed 12, True Damage 2, When an enemy unit is within 3 inches of this, it triggers a free Opportunity Attack from this unit.  This can be avoided with a penalty level; otherwise this unit automatically explodes, leaving behind a Root Cluster and damaging all enemy units within Range.  The Root Cluster share's this unit's Seed ability</t>
   </si>
   <si>
-    <t>5R</t>
-  </si>
-  <si>
     <t>Tunnel Sapper x2</t>
   </si>
   <si>
@@ -1116,6 +1083,72 @@
   </si>
   <si>
     <t>Tunnel Worm x4</t>
+  </si>
+  <si>
+    <t>Root, Seed 12, You may spend additional AP when attacking.  For each two points spent add: 1 Power, Armor Penetration 1, or 2 inches of range.</t>
+  </si>
+  <si>
+    <t>7R</t>
+  </si>
+  <si>
+    <t>Root, Seed 12, You may spend additional AP when attacking.  For each two points spent add 2 inches of range.</t>
+  </si>
+  <si>
+    <t>5R (Mininum 3" range)</t>
+  </si>
+  <si>
+    <t>9-16R</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> High damage activated fire</t>
+  </si>
+  <si>
+    <t>Root, Seed 12, Armor Pen 2, You may spend additional AP when attacking.  For each two points spent add: 1 Power, Armor Penetration 1, or 2 inches of range.</t>
+  </si>
+  <si>
+    <t>Spellcaster: Geomancy</t>
+  </si>
+  <si>
+    <t>Hive Courts</t>
+  </si>
+  <si>
+    <t>Queen's Will</t>
+  </si>
+  <si>
+    <t>0-6</t>
+  </si>
+  <si>
+    <t>Choose a friendly Hive Court model.  If it is between 12 and 18 inches away, spend 4 AP.  If it is out of line of sight or greater than 18" away, spend 6 AP.  Then spend any amount of AP you wish.  The targeted model may then take actions as though it were its turn and may spend AP equivalent to the spent AP in addition to its own.  This effect does not end the Emissary's  turn.</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remove up to twice X damage from a creature you control with Reshape. </t>
+  </si>
+  <si>
+    <t>Grants Regeneration 3</t>
+  </si>
+  <si>
+    <t>Gives Attack R14.</t>
+  </si>
+  <si>
+    <t>R8 P + 1 AP1</t>
+  </si>
+  <si>
+    <t>Enemy units cannot move out of melee range with this unit.</t>
+  </si>
+  <si>
+    <t>Multi-Strike</t>
+  </si>
+  <si>
+    <t>The model may declare Attacks against multiple units with the same Attack Action</t>
+  </si>
+  <si>
+    <t>Grants Multi-strike</t>
+  </si>
+  <si>
+    <t>+2 Wounds per Reshape level</t>
   </si>
 </sst>
 </file>
@@ -1217,7 +1250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1266,6 +1299,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4148,8 +4185,8 @@
   <dimension ref="A1:M57"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4158,7 +4195,7 @@
     <col min="2" max="2" width="55.5703125" customWidth="1"/>
     <col min="6" max="6" width="5.7109375" customWidth="1"/>
     <col min="8" max="8" width="13.42578125" customWidth="1"/>
-    <col min="12" max="12" width="38.7109375" customWidth="1"/>
+    <col min="12" max="12" width="55.140625" style="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4195,7 +4232,7 @@
       <c r="K1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="28" t="s">
         <v>14</v>
       </c>
       <c r="M1" s="4" t="s">
@@ -4236,7 +4273,7 @@
       <c r="K2" s="4">
         <v>25</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="23" t="s">
         <v>127</v>
       </c>
       <c r="M2" s="4" t="s">
@@ -4277,7 +4314,7 @@
       <c r="K3" s="4">
         <v>30</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="23" t="s">
         <v>130</v>
       </c>
       <c r="M3" s="4" t="s">
@@ -4318,7 +4355,7 @@
       <c r="K4" s="4">
         <v>50</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="23" t="s">
         <v>131</v>
       </c>
       <c r="M4" s="4" t="s">
@@ -4359,7 +4396,7 @@
       <c r="K5" s="4">
         <v>70</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="L5" s="23" t="s">
         <v>134</v>
       </c>
       <c r="M5" s="4"/>
@@ -4395,11 +4432,11 @@
       <c r="K6" s="4">
         <v>20</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="L6" s="23" t="s">
         <v>135</v>
       </c>
       <c r="M6" s="15" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4433,7 +4470,7 @@
       <c r="K7" s="4">
         <v>15</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="L7" s="23" t="s">
         <v>136</v>
       </c>
       <c r="M7" s="4" t="s">
@@ -4442,10 +4479,10 @@
     </row>
     <row r="8" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="C8" s="15">
         <v>0.75</v>
@@ -4471,7 +4508,7 @@
       <c r="K8" s="15">
         <v>20</v>
       </c>
-      <c r="L8" s="15" t="s">
+      <c r="L8" s="23" t="s">
         <v>136</v>
       </c>
     </row>
@@ -4509,8 +4546,8 @@
       <c r="K10" s="4">
         <v>15</v>
       </c>
-      <c r="L10" s="15" t="s">
-        <v>304</v>
+      <c r="L10" s="23" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4573,8 +4610,8 @@
       <c r="K12" s="4">
         <v>15</v>
       </c>
-      <c r="L12" t="s">
-        <v>305</v>
+      <c r="L12" s="27" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4605,8 +4642,8 @@
       <c r="K13" s="4">
         <v>15</v>
       </c>
-      <c r="L13" t="s">
-        <v>212</v>
+      <c r="L13" s="27" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4640,8 +4677,8 @@
       <c r="K14" s="4">
         <v>30</v>
       </c>
-      <c r="L14" s="4" t="s">
-        <v>40</v>
+      <c r="L14" s="23" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4745,8 +4782,8 @@
       <c r="K18" s="21">
         <v>7</v>
       </c>
-      <c r="L18" s="4" t="s">
-        <v>315</v>
+      <c r="L18" s="23" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4781,11 +4818,11 @@
       <c r="K19" s="21">
         <v>10</v>
       </c>
-      <c r="L19" s="4" t="s">
+      <c r="L19" s="23" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
         <v>137</v>
       </c>
@@ -4817,16 +4854,16 @@
       <c r="K20" s="21">
         <v>9</v>
       </c>
-      <c r="L20" s="4" t="s">
+      <c r="L20" s="23" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="C21" s="25">
         <v>1</v>
@@ -4853,16 +4890,16 @@
       <c r="K21" s="25">
         <v>20</v>
       </c>
-      <c r="L21" s="15" t="s">
-        <v>320</v>
+      <c r="L21" s="23" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="24" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="C22" s="25">
         <v>1</v>
@@ -4891,8 +4928,8 @@
       <c r="K22" s="25">
         <v>40</v>
       </c>
-      <c r="L22" s="15" t="s">
-        <v>322</v>
+      <c r="L22" s="23" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4941,7 +4978,7 @@
         <v>58</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="C26" s="4">
         <v>1</v>
@@ -4970,8 +5007,8 @@
       <c r="K26" s="4">
         <v>30</v>
       </c>
-      <c r="L26" s="4" t="s">
-        <v>343</v>
+      <c r="L26" s="23" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4979,7 +5016,7 @@
         <v>62</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="C27" s="4">
         <v>1</v>
@@ -5005,8 +5042,8 @@
       <c r="K27" s="4">
         <v>25</v>
       </c>
-      <c r="L27" s="15" t="s">
-        <v>339</v>
+      <c r="L27" s="23" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -5014,7 +5051,7 @@
         <v>65</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="C28" s="4">
         <v>0.8</v>
@@ -5040,16 +5077,16 @@
       <c r="K28" s="4">
         <v>5</v>
       </c>
-      <c r="L28" s="15" t="s">
-        <v>341</v>
+      <c r="L28" s="23" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="C29" s="15">
         <v>1</v>
@@ -5075,16 +5112,16 @@
       <c r="K29" s="15">
         <v>10</v>
       </c>
-      <c r="L29" s="15" t="s">
-        <v>343</v>
+      <c r="L29" s="23" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="C30" s="15">
         <v>1</v>
@@ -5110,13 +5147,13 @@
       <c r="K30" s="15">
         <v>20</v>
       </c>
-      <c r="L30" s="15" t="s">
-        <v>348</v>
+      <c r="L30" s="23" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G31" s="22" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -5150,7 +5187,7 @@
       <c r="K32" s="4">
         <v>15</v>
       </c>
-      <c r="L32" s="4" t="s">
+      <c r="L32" s="23" t="s">
         <v>70</v>
       </c>
     </row>
@@ -5182,7 +5219,7 @@
       <c r="K33" s="4">
         <v>20</v>
       </c>
-      <c r="L33" s="4" t="s">
+      <c r="L33" s="23" t="s">
         <v>72</v>
       </c>
     </row>
@@ -5214,7 +5251,7 @@
       <c r="K34" s="4">
         <v>20</v>
       </c>
-      <c r="L34" s="4" t="s">
+      <c r="L34" s="23" t="s">
         <v>74</v>
       </c>
     </row>
@@ -5246,7 +5283,7 @@
       <c r="K35" s="4">
         <v>20</v>
       </c>
-      <c r="L35" s="4" t="s">
+      <c r="L35" s="23" t="s">
         <v>76</v>
       </c>
     </row>
@@ -5278,7 +5315,7 @@
       <c r="K36" s="4">
         <v>20</v>
       </c>
-      <c r="L36" s="4" t="s">
+      <c r="L36" s="23" t="s">
         <v>78</v>
       </c>
     </row>
@@ -5310,7 +5347,7 @@
       <c r="K37" s="4">
         <v>20</v>
       </c>
-      <c r="L37" s="4" t="s">
+      <c r="L37" s="23" t="s">
         <v>80</v>
       </c>
     </row>
@@ -5342,7 +5379,7 @@
       <c r="K38" s="4">
         <v>20</v>
       </c>
-      <c r="L38" s="4" t="s">
+      <c r="L38" s="23" t="s">
         <v>82</v>
       </c>
     </row>
@@ -5374,7 +5411,7 @@
       <c r="K39" s="4">
         <v>20</v>
       </c>
-      <c r="L39" s="4" t="s">
+      <c r="L39" s="23" t="s">
         <v>84</v>
       </c>
     </row>
@@ -5406,7 +5443,7 @@
       <c r="K40" s="4">
         <v>20</v>
       </c>
-      <c r="L40" s="4" t="s">
+      <c r="L40" s="23" t="s">
         <v>86</v>
       </c>
     </row>
@@ -5447,7 +5484,7 @@
       <c r="K42" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="L42" s="4" t="s">
+      <c r="L42" s="23" t="s">
         <v>89</v>
       </c>
     </row>
@@ -5482,7 +5519,7 @@
       <c r="K43" s="4">
         <v>10</v>
       </c>
-      <c r="L43" s="4" t="s">
+      <c r="L43" s="23" t="s">
         <v>95</v>
       </c>
     </row>
@@ -5517,7 +5554,7 @@
       <c r="K44" s="4">
         <v>20</v>
       </c>
-      <c r="L44" s="4" t="s">
+      <c r="L44" s="23" t="s">
         <v>98</v>
       </c>
     </row>
@@ -5552,13 +5589,13 @@
       <c r="K45" s="4">
         <v>35</v>
       </c>
-      <c r="L45" s="4" t="s">
+      <c r="L45" s="23" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>103</v>
@@ -5588,7 +5625,7 @@
       <c r="K46" s="9">
         <v>55</v>
       </c>
-      <c r="L46" s="10" t="s">
+      <c r="L46" s="26" t="s">
         <v>104</v>
       </c>
     </row>
@@ -5624,7 +5661,7 @@
       <c r="K47" s="8">
         <v>80</v>
       </c>
-      <c r="L47" s="11" t="s">
+      <c r="L47" s="26" t="s">
         <v>106</v>
       </c>
     </row>
@@ -5657,10 +5694,10 @@
         <v>4</v>
       </c>
       <c r="K48" s="4">
-        <v>25</v>
-      </c>
-      <c r="L48" s="4" t="s">
-        <v>328</v>
+        <v>20</v>
+      </c>
+      <c r="L48" s="23" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -5698,28 +5735,28 @@
       <c r="K50" s="4">
         <v>10</v>
       </c>
-      <c r="L50" s="4" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L50" s="23" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>114</v>
+        <v>123</v>
+      </c>
+      <c r="B51" s="15" t="s">
+        <v>353</v>
       </c>
       <c r="C51" s="4">
         <v>2</v>
       </c>
       <c r="D51" s="4">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E51" s="4">
         <v>2</v>
       </c>
       <c r="F51" s="4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G51" s="21">
         <v>8</v>
@@ -5731,13 +5768,13 @@
         <v>0</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="K51" s="4">
         <v>10</v>
       </c>
-      <c r="L51" s="4" t="s">
-        <v>350</v>
+      <c r="L51" s="23" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -5771,8 +5808,8 @@
       <c r="K52" s="4">
         <v>5</v>
       </c>
-      <c r="L52" s="4" t="s">
-        <v>351</v>
+      <c r="L52" s="23" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -5809,11 +5846,11 @@
       <c r="K53" s="4">
         <v>50</v>
       </c>
-      <c r="L53" s="4" t="s">
+      <c r="L53" s="23" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>139</v>
       </c>
@@ -5824,7 +5861,7 @@
         <v>2</v>
       </c>
       <c r="D54" s="4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E54" s="4">
         <v>2</v>
@@ -5842,33 +5879,33 @@
         <v>0</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="K54" s="4">
         <v>10</v>
       </c>
-      <c r="L54" s="4" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L54" s="23" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="C55" s="4">
         <v>2</v>
       </c>
       <c r="D55" s="4">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E55" s="4">
         <v>2</v>
       </c>
       <c r="F55" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G55" s="21">
         <v>8</v>
@@ -5880,33 +5917,33 @@
         <v>0</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>115</v>
+        <v>349</v>
       </c>
       <c r="K55" s="4">
         <v>10</v>
       </c>
-      <c r="L55" s="4" t="s">
+      <c r="L55" s="23" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="77.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
+      <c r="B56" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="C56" s="4">
+        <v>2</v>
+      </c>
+      <c r="D56" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="C56" s="4">
-        <v>2</v>
-      </c>
-      <c r="D56" s="4" t="s">
+      <c r="E56" s="4">
+        <v>2</v>
+      </c>
+      <c r="F56" s="4" t="s">
         <v>144</v>
-      </c>
-      <c r="E56" s="4">
-        <v>2</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>145</v>
       </c>
       <c r="G56" s="21">
         <v>8</v>
@@ -5918,13 +5955,13 @@
         <v>0</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K56" s="4">
-        <v>8</v>
-      </c>
-      <c r="L56" s="4" t="s">
-        <v>353</v>
+        <v>10</v>
+      </c>
+      <c r="L56" s="23" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="12.75" x14ac:dyDescent="0.2"/>
@@ -5952,33 +5989,33 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>153</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B2" s="4">
         <v>5</v>
@@ -6009,7 +6046,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B3" s="4">
         <v>6</v>
@@ -6040,7 +6077,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B4" s="4">
         <v>4</v>
@@ -6071,7 +6108,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B5" s="4">
         <v>2</v>
@@ -6102,7 +6139,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B6" s="4">
         <v>4</v>
@@ -6133,7 +6170,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B7" s="4">
         <v>1</v>
@@ -6164,7 +6201,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B8" s="15">
         <v>5</v>
@@ -6195,7 +6232,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -6231,30 +6268,30 @@
         <v>6</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>165</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>167</v>
-      </c>
-      <c r="B2" s="4">
-        <v>0</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>168</v>
       </c>
       <c r="D2" s="4">
         <v>-1</v>
@@ -6263,7 +6300,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H2" s="4">
         <v>2</v>
@@ -6271,22 +6308,22 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>171</v>
-      </c>
       <c r="C3" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>168</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>169</v>
       </c>
       <c r="H3" s="4">
         <v>2</v>
@@ -6294,7 +6331,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B4" s="4">
         <v>4</v>
@@ -6317,7 +6354,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B5" s="4">
         <v>4</v>
@@ -6340,7 +6377,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B6" s="4">
         <v>0</v>
@@ -6352,7 +6389,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H6" s="4">
         <v>2</v>
@@ -6360,22 +6397,22 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>175</v>
-      </c>
-      <c r="B7" s="4">
-        <v>0</v>
-      </c>
-      <c r="C7" s="4">
-        <v>0</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>176</v>
       </c>
       <c r="H7" s="4">
         <v>3</v>
@@ -6383,22 +6420,22 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="B8" s="4">
-        <v>0</v>
-      </c>
-      <c r="C8" s="4">
-        <v>0</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0</v>
-      </c>
-      <c r="E8" s="14" t="s">
+      <c r="G8" s="4" t="s">
         <v>178</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>179</v>
       </c>
       <c r="H8" s="4">
         <v>4</v>
@@ -6406,25 +6443,25 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>180</v>
-      </c>
-      <c r="B9" s="4">
-        <v>0</v>
-      </c>
-      <c r="C9" s="4">
-        <v>0</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0</v>
-      </c>
-      <c r="F9" s="4">
-        <v>0</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>181</v>
       </c>
       <c r="H9" s="4">
         <v>3</v>
@@ -6432,7 +6469,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B10" s="4">
         <v>0</v>
@@ -6444,7 +6481,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H10" s="4">
         <v>2</v>
@@ -6452,19 +6489,19 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>183</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>184</v>
       </c>
       <c r="H11" s="4">
         <v>4</v>
@@ -6480,10 +6517,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA23"/>
+  <dimension ref="A1:AA24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6495,279 +6532,290 @@
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>185</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C3" s="23" t="s">
         <v>188</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C4" s="23" t="s">
         <v>190</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C5" s="23" t="s">
         <v>192</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C6" s="23" t="s">
         <v>194</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="C10" s="23" t="s">
         <v>197</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="23" t="s">
         <v>200</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="C13" s="23" t="s">
         <v>202</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="C14" s="23" t="s">
         <v>205</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C15" s="23" t="s">
         <v>207</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C16" s="23" t="s">
         <v>209</v>
-      </c>
-      <c r="C16" s="23" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="17" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>136</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="18" spans="1:27" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C18" s="23" t="s">
         <v>212</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="19" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C19" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="C19" s="23" t="s">
+    </row>
+    <row r="20" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="20" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="B20" s="5" t="s">
+      <c r="C21" s="26" t="s">
         <v>216</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="D21" s="16"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="6"/>
+      <c r="U21" s="6"/>
+      <c r="V21" s="6"/>
+      <c r="W21" s="6"/>
+      <c r="X21" s="6"/>
+      <c r="Y21" s="6"/>
+      <c r="Z21" s="6"/>
+      <c r="AA21" s="6"/>
+    </row>
+    <row r="22" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="6"/>
-      <c r="R20" s="6"/>
-      <c r="S20" s="6"/>
-      <c r="T20" s="6"/>
-      <c r="U20" s="6"/>
-      <c r="V20" s="6"/>
-      <c r="W20" s="6"/>
-      <c r="X20" s="6"/>
-      <c r="Y20" s="6"/>
-      <c r="Z20" s="6"/>
-      <c r="AA20" s="6"/>
-    </row>
-    <row r="21" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="B21" s="4" t="s">
+      <c r="C22" s="23" t="s">
         <v>218</v>
       </c>
-      <c r="C21" s="23" t="s">
+    </row>
+    <row r="23" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="22" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="B22" s="4" t="s">
+      <c r="C23" s="23" t="s">
         <v>220</v>
       </c>
-      <c r="C22" s="23" t="s">
+    </row>
+    <row r="24" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C24" s="23" t="s">
         <v>221</v>
-      </c>
-    </row>
-    <row r="23" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C23" s="23" t="s">
-        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -6780,198 +6828,198 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:E26"/>
+  <dimension ref="A2:E27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.5703125" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="71.140625" customWidth="1"/>
+    <col min="5" max="5" width="71.140625" style="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="14" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B6" s="15" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="14" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="14" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="14" t="s">
-        <v>228</v>
+        <v>369</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="14" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
-        <v>234</v>
+        <v>364</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4" t="s">
-        <v>236</v>
+        <v>365</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B14" s="4" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="14" t="s">
-        <v>238</v>
+        <v>368</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B15" s="4" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4" t="s">
-        <v>332</v>
+        <v>362</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B16" s="4" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B17" s="4" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B18" s="15" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="14" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B19" s="4" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4" t="s">
-        <v>245</v>
+        <v>363</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+        <v>242</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C23" s="4">
         <v>24</v>
@@ -6979,50 +7027,50 @@
       <c r="D23" s="4">
         <v>6</v>
       </c>
-      <c r="E23" s="4" t="s">
-        <v>251</v>
+      <c r="E23" s="23" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="C24" s="4">
-        <v>24</v>
-      </c>
-      <c r="D24" s="4">
-        <v>3</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>307</v>
+        <v>18</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D25" s="4">
         <v>8</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>249</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>255</v>
       </c>
       <c r="C26">
         <v>12</v>
@@ -7030,8 +7078,25 @@
       <c r="D26" s="15">
         <v>6</v>
       </c>
-      <c r="E26" s="15" t="s">
-        <v>308</v>
+      <c r="E26" s="23" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="15" t="s">
+        <v>356</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>357</v>
+      </c>
+      <c r="C27" s="29" t="s">
+        <v>248</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>358</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -7046,8 +7111,8 @@
   </sheetPr>
   <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7058,7 +7123,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="B1" s="23">
         <f>6*9</f>
@@ -7071,7 +7136,7 @@
     </row>
     <row r="2" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="B2" s="12">
         <f>18*7</f>
@@ -7080,7 +7145,7 @@
     </row>
     <row r="3" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="B3" s="12">
         <f>10*2</f>
@@ -7089,7 +7154,7 @@
     </row>
     <row r="6" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B6">
         <v>50</v>
@@ -7097,7 +7162,7 @@
     </row>
     <row r="7" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
-        <v>357</v>
+        <v>346</v>
       </c>
       <c r="B7">
         <v>40</v>
@@ -7105,7 +7170,7 @@
     </row>
     <row r="8" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
-        <v>355</v>
+        <v>344</v>
       </c>
       <c r="B8">
         <v>40</v>
@@ -7113,7 +7178,7 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
-        <v>358</v>
+        <v>347</v>
       </c>
       <c r="B9">
         <v>40</v>
@@ -7121,7 +7186,7 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
-        <v>356</v>
+        <v>345</v>
       </c>
       <c r="B10">
         <v>30</v>
@@ -7133,162 +7198,162 @@
     <row r="12" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="71.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="22" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="23" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="23" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="26" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="23" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="23" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="23" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C29" s="4" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="23" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="23" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="23" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="23" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="23" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="36" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="23" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="23" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="23" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="23" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="23" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="44" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="23" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B45" s="4" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="47" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="23" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B48" s="4" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="50" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="23" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>136</v>
@@ -7296,42 +7361,42 @@
     </row>
     <row r="51" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B51" s="4" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B52" s="4" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="55" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="23" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="57" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="23" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="59" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="23" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="61" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="23" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -7359,22 +7424,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="221.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -7382,19 +7447,19 @@
         <v>44682</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Hive courts battle illustration and updated some text.
</commit_message>
<xml_diff>
--- a/unit stats.xlsx
+++ b/unit stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas\Documents\wargame\wargame-tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523B5E79-7077-4E8F-8524-3911AEB76853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D9D693-F0E5-4A35-9613-4132D85A58A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -4184,9 +4184,9 @@
   </sheetPr>
   <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L42" sqref="L42"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L51" sqref="L51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6830,7 +6830,7 @@
   </sheetPr>
   <dimension ref="A2:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated rules and added more FCP abilities.  Fleshed out some spells
</commit_message>
<xml_diff>
--- a/unit stats.xlsx
+++ b/unit stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas\Documents\wargame\wargame-tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D9D693-F0E5-4A35-9613-4132D85A58A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C754DD-22E6-4B01-A798-3D4C513A90CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="377">
   <si>
     <t>Name</t>
   </si>
@@ -776,9 +776,6 @@
     <t>Resculpt</t>
   </si>
   <si>
-    <t xml:space="preserve">Lower the level of a unit you control with Reshape.  You may then increase the level of another unit you control with Reshape.  Damage stays on the transformed creatues, as does used focus. </t>
-  </si>
-  <si>
     <t>Mend</t>
   </si>
   <si>
@@ -941,12 +938,6 @@
     <t>Water Steps</t>
   </si>
   <si>
-    <t>Select two models you control with Reshape that are within 3" of one another.  Remove both of them from the game and add a new model in its place.  The new model has Reshape X, where X is the total Reshape value of the sacrificed models.  For Power, Toughness, Armor, Damage, choose the highest of the sacrificed models.  For Attack Cost and Move Cost, choose the lowest of the two.  For Wounds, add the total maximum Wounds of each sacrificed model.  The model starts with  the total Damage of the combined units.  You may use up to one felled model for this.</t>
-  </si>
-  <si>
-    <t>You may remove a model with Reshape 2+ from the battlefield.  For every two levels of Reshape, create a Flesh Golem</t>
-  </si>
-  <si>
     <t>Tunneling Claws</t>
   </si>
   <si>
@@ -1149,6 +1140,36 @@
   </si>
   <si>
     <t>+2 Wounds per Reshape level</t>
+  </si>
+  <si>
+    <t>Sweat Secretion</t>
+  </si>
+  <si>
+    <t>Grants Dodge</t>
+  </si>
+  <si>
+    <t>Select two models you control with Reshape that are within 3" of one another.  Remove both of them from the game and add a new model in its place.  The new model has Reshape X, where X is the total Reshape value of the sacrificed models.  For Power, Toughness, Armor, Damage, choose the highest of the sacrificed models.  For Attack Cost and Move Cost, choose the lowest of the two.  For Wounds, add the total maximum Wounds of each sacrificed model.  The model starts with  the total Damage of the combined units.  You may use up to one felled model for this, though it counts as having one fewer Reshape Level.</t>
+  </si>
+  <si>
+    <t>Breakaway</t>
+  </si>
+  <si>
+    <t>Deal 2 damage to a creature with Reshape 1+, then create a Flesh Pile within 2" of it.</t>
+  </si>
+  <si>
+    <t>Gonad Synthesis</t>
+  </si>
+  <si>
+    <t>At the beginning of each round create a Flesh Pile within 2" of this unit.  Those units may take actions this round.</t>
+  </si>
+  <si>
+    <t>Reshape 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lower the level of a unit you control with Reshape.  You may then increase the level of another unit you control with Reshape OR create a Flesh Drone within 2" of the targeted model.  Damage stays on the transformed creatures, as does used focus. </t>
+  </si>
+  <si>
+    <t>You may remove a model with Reshape from the battlefield.  For every level of Reshape, create a Flesh Drone.  Slain models may be used, but count as having one fewer level of Reshape, and all models resulting from a slain model enter the battlefield with 7 damage</t>
   </si>
 </sst>
 </file>
@@ -4184,9 +4205,9 @@
   </sheetPr>
   <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L51" sqref="L51"/>
+      <selection pane="bottomLeft" activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4436,7 +4457,7 @@
         <v>135</v>
       </c>
       <c r="M6" s="15" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4479,10 +4500,10 @@
     </row>
     <row r="8" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C8" s="15">
         <v>0.75</v>
@@ -4547,7 +4568,7 @@
         <v>15</v>
       </c>
       <c r="L10" s="23" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4611,7 +4632,7 @@
         <v>15</v>
       </c>
       <c r="L12" s="27" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4678,7 +4699,7 @@
         <v>30</v>
       </c>
       <c r="L14" s="23" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4783,7 +4804,7 @@
         <v>7</v>
       </c>
       <c r="L18" s="23" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4860,10 +4881,10 @@
     </row>
     <row r="21" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C21" s="25">
         <v>1</v>
@@ -4891,15 +4912,15 @@
         <v>20</v>
       </c>
       <c r="L21" s="23" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="24" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C22" s="25">
         <v>1</v>
@@ -4929,7 +4950,7 @@
         <v>40</v>
       </c>
       <c r="L22" s="23" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -4978,7 +4999,7 @@
         <v>58</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C26" s="4">
         <v>1</v>
@@ -5008,7 +5029,7 @@
         <v>30</v>
       </c>
       <c r="L26" s="23" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -5016,7 +5037,7 @@
         <v>62</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C27" s="4">
         <v>1</v>
@@ -5043,7 +5064,7 @@
         <v>25</v>
       </c>
       <c r="L27" s="23" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -5051,7 +5072,7 @@
         <v>65</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C28" s="4">
         <v>0.8</v>
@@ -5078,15 +5099,15 @@
         <v>5</v>
       </c>
       <c r="L28" s="23" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C29" s="15">
         <v>1</v>
@@ -5113,15 +5134,15 @@
         <v>10</v>
       </c>
       <c r="L29" s="23" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C30" s="15">
         <v>1</v>
@@ -5148,12 +5169,12 @@
         <v>20</v>
       </c>
       <c r="L30" s="23" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G31" s="22" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -5485,7 +5506,7 @@
         <v>43</v>
       </c>
       <c r="L42" s="23" t="s">
-        <v>89</v>
+        <v>374</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -5595,7 +5616,7 @@
     </row>
     <row r="46" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>103</v>
@@ -5697,7 +5718,7 @@
         <v>20</v>
       </c>
       <c r="L48" s="23" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -5736,7 +5757,7 @@
         <v>10</v>
       </c>
       <c r="L50" s="23" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="39" thickBot="1" x14ac:dyDescent="0.25">
@@ -5744,7 +5765,7 @@
         <v>123</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C51" s="4">
         <v>2</v>
@@ -5768,13 +5789,13 @@
         <v>0</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="K51" s="4">
         <v>10</v>
       </c>
       <c r="L51" s="23" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -5809,7 +5830,7 @@
         <v>5</v>
       </c>
       <c r="L52" s="23" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -5879,13 +5900,13 @@
         <v>0</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="K54" s="4">
         <v>10</v>
       </c>
       <c r="L54" s="23" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="39" thickBot="1" x14ac:dyDescent="0.25">
@@ -5917,13 +5938,13 @@
         <v>0</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="K55" s="4">
         <v>10</v>
       </c>
       <c r="L55" s="23" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="77.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -5961,7 +5982,7 @@
         <v>10</v>
       </c>
       <c r="L56" s="23" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="12.75" x14ac:dyDescent="0.2"/>
@@ -6520,7 +6541,7 @@
   <dimension ref="A1:AA24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6549,7 +6570,7 @@
         <v>186</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
@@ -6604,7 +6625,7 @@
         <v>195</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
@@ -6612,10 +6633,10 @@
         <v>157</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
@@ -6623,10 +6644,10 @@
         <v>157</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
@@ -6645,10 +6666,10 @@
         <v>198</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
@@ -6744,10 +6765,10 @@
         <v>198</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="21" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
@@ -6828,10 +6849,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:E27"/>
+  <dimension ref="A2:E30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6864,16 +6885,16 @@
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="14" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B6" s="15" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="14" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -6891,7 +6912,7 @@
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="14" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -6914,11 +6935,11 @@
     </row>
     <row r="11" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -6927,7 +6948,7 @@
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -6936,167 +6957,201 @@
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B14" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="14" t="s">
-        <v>368</v>
+      <c r="B14" s="15" t="s">
+        <v>372</v>
+      </c>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B15" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C15" s="4"/>
-      <c r="D15" s="4" t="s">
-        <v>362</v>
+      <c r="D15" s="14" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B16" s="4" t="s">
-        <v>235</v>
-      </c>
+        <v>234</v>
+      </c>
+      <c r="C16" s="4"/>
       <c r="D16" s="4" t="s">
-        <v>236</v>
+        <v>359</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B17" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="C17" s="4"/>
+        <v>235</v>
+      </c>
       <c r="D17" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B18" s="15" t="s">
-        <v>304</v>
-      </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="14" t="s">
-        <v>325</v>
+        <v>367</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B19" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4" t="s">
-        <v>363</v>
+        <v>238</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="18" t="s">
+      <c r="B20" s="15" t="s">
+        <v>301</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="14" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B21" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="18" t="s">
         <v>240</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="E22" s="23" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="C23" s="4">
-        <v>24</v>
-      </c>
-      <c r="D23" s="4">
-        <v>6</v>
-      </c>
-      <c r="E23" s="23" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="C24" s="4">
-        <v>18</v>
+        <v>0</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>163</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>360</v>
+        <v>242</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>243</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
+      </c>
+      <c r="C25" s="4">
+        <v>24</v>
       </c>
       <c r="D25" s="4">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>243</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="C26">
+        <v>245</v>
+      </c>
+      <c r="C26" s="4">
+        <v>18</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="E26" s="23" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A27" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>370</v>
+      </c>
+      <c r="C27" s="15">
+        <v>18</v>
+      </c>
+      <c r="D27" s="15">
+        <v>4</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="D28" s="4">
+        <v>8</v>
+      </c>
+      <c r="E28" s="23" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="C29">
         <v>12</v>
       </c>
-      <c r="D26" s="15">
+      <c r="D29" s="15">
         <v>6</v>
       </c>
-      <c r="E26" s="23" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="15" t="s">
+      <c r="E29" s="23" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="15" t="s">
+        <v>353</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>354</v>
+      </c>
+      <c r="C30" s="29" t="s">
+        <v>247</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>355</v>
+      </c>
+      <c r="E30" s="23" t="s">
         <v>356</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>357</v>
-      </c>
-      <c r="C27" s="29" t="s">
-        <v>248</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>358</v>
-      </c>
-      <c r="E27" s="23" t="s">
-        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -7123,7 +7178,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B1" s="23">
         <f>6*9</f>
@@ -7136,7 +7191,7 @@
     </row>
     <row r="2" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B2" s="12">
         <f>18*7</f>
@@ -7145,7 +7200,7 @@
     </row>
     <row r="3" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B3" s="12">
         <f>10*2</f>
@@ -7154,7 +7209,7 @@
     </row>
     <row r="6" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B6">
         <v>50</v>
@@ -7162,7 +7217,7 @@
     </row>
     <row r="7" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B7">
         <v>40</v>
@@ -7170,7 +7225,7 @@
     </row>
     <row r="8" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B8">
         <v>40</v>
@@ -7178,7 +7233,7 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B9">
         <v>40</v>
@@ -7186,7 +7241,7 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B10">
         <v>30</v>
@@ -7198,134 +7253,134 @@
     <row r="12" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="71.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="22" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="23" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="26" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="23" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="23" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C29" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="23" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="23" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="23" t="s">
+        <v>265</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>266</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="23" t="s">
+        <v>266</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>267</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="23" t="s">
+        <v>267</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>268</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="36" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="23" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="23" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="23" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="23" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="23" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="44" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="23" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>232</v>
@@ -7333,27 +7388,27 @@
     </row>
     <row r="45" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B45" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="47" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="23" t="s">
+        <v>276</v>
+      </c>
+      <c r="B47" s="4" t="s">
         <v>277</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B48" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="50" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="23" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>136</v>
@@ -7361,42 +7416,42 @@
     </row>
     <row r="51" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B51" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B52" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="55" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="23" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="57" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="59" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="23" t="s">
+        <v>284</v>
+      </c>
+      <c r="B59" s="4" t="s">
         <v>285</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="61" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="23" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -7424,22 +7479,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>292</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="221.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -7447,19 +7502,19 @@
         <v>44682</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>294</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>295</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>159</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="F2" s="23" t="s">
         <v>296</v>
-      </c>
-      <c r="F2" s="23" t="s">
-        <v>297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lots of formatting and updates to the primers
</commit_message>
<xml_diff>
--- a/unit stats.xlsx
+++ b/unit stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas\Documents\wargame\wargame-tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9373FB-0E11-48E9-B5D5-55C88CB80458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6140076B-A978-43CF-B7C5-A2F0B5B0ACBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20520" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="units new statlines" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,6 @@
     <sheet name="Notable Locations" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -43,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="355">
   <si>
     <t>Name</t>
   </si>
@@ -102,9 +101,6 @@
     <t>Elite armored melee unit</t>
   </si>
   <si>
-    <t>Longhorn Magus</t>
-  </si>
-  <si>
     <t>Spellcaster unit</t>
   </si>
   <si>
@@ -1105,6 +1101,12 @@
   </si>
   <si>
     <t>Marauder</t>
+  </si>
+  <si>
+    <t>Excavator</t>
+  </si>
+  <si>
+    <t>Royal Emissary</t>
   </si>
 </sst>
 </file>
@@ -1410,7 +1412,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2052,7 +2054,7 @@
                   <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.333333333333333</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2488,7 +2490,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2541,7 +2543,7 @@
         <v>13</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -2579,7 +2581,7 @@
         <v>20</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>16</v>
@@ -2620,7 +2622,7 @@
         <v>50</v>
       </c>
       <c r="L3" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>16</v>
@@ -2628,10 +2630,10 @@
     </row>
     <row r="4" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="C4" s="2">
         <v>0.7</v>
@@ -2661,16 +2663,16 @@
         <v>70</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
@@ -2697,18 +2699,18 @@
         <v>20</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -2735,18 +2737,18 @@
         <v>15</v>
       </c>
       <c r="L6" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C7" s="2">
         <v>0.75</v>
@@ -2773,7 +2775,7 @@
         <v>20</v>
       </c>
       <c r="L7" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2781,7 +2783,7 @@
     </row>
     <row r="9" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
@@ -2805,18 +2807,18 @@
         <v>1</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K9" s="2">
         <v>15</v>
       </c>
       <c r="L9" s="14" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="2">
         <v>0.6</v>
@@ -2840,7 +2842,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K10" s="2">
         <v>15</v>
@@ -2848,7 +2850,7 @@
     </row>
     <row r="11" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
@@ -2875,12 +2877,12 @@
         <v>15</v>
       </c>
       <c r="L11" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="2">
         <v>1.2</v>
@@ -2907,15 +2909,15 @@
         <v>15</v>
       </c>
       <c r="L12" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="C13" s="2">
         <v>1</v>
@@ -2942,36 +2944,36 @@
         <v>30</v>
       </c>
       <c r="L13" s="14" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2">
+        <v>2</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="2">
-        <v>2</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="E14" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K14" s="2">
         <v>20</v>
@@ -2979,31 +2981,31 @@
     </row>
     <row r="15" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="C15" s="2">
         <v>2</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K15" s="2">
         <v>20</v>
@@ -3038,10 +3040,10 @@
     </row>
     <row r="19" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="13" t="s">
         <v>37</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>38</v>
       </c>
       <c r="C19" s="12">
         <v>1</v>
@@ -3071,15 +3073,15 @@
         <v>7</v>
       </c>
       <c r="L19" s="14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="13" t="s">
         <v>39</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>40</v>
       </c>
       <c r="C20" s="12">
         <v>1</v>
@@ -3107,15 +3109,15 @@
         <v>10</v>
       </c>
       <c r="L20" s="14" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C21" s="12">
         <v>1</v>
@@ -3143,15 +3145,15 @@
         <v>9</v>
       </c>
       <c r="L21" s="14" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="B22" s="15" t="s">
         <v>259</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>260</v>
       </c>
       <c r="C22" s="16">
         <v>1</v>
@@ -3179,15 +3181,15 @@
         <v>13</v>
       </c>
       <c r="L22" s="14" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C23" s="16">
         <v>1</v>
@@ -3217,7 +3219,7 @@
         <v>40</v>
       </c>
       <c r="L23" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3225,10 +3227,10 @@
     </row>
     <row r="25" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="C25" s="2">
         <v>1</v>
@@ -3255,15 +3257,18 @@
         <v>10</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G26" s="13"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>350</v>
+      </c>
       <c r="B27" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C27" s="2">
         <v>1.5</v>
@@ -3287,13 +3292,13 @@
         <v>1</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K27" s="2">
         <v>20</v>
       </c>
       <c r="L27" s="14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3301,7 +3306,7 @@
         <v>351</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C28" s="2">
         <v>1.5</v>
@@ -3325,13 +3330,13 @@
         <v>1</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K28" s="2">
         <v>20</v>
       </c>
       <c r="L28" s="14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3339,7 +3344,7 @@
         <v>352</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C29" s="2">
         <v>1.5</v>
@@ -3363,13 +3368,13 @@
         <v>1</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K29" s="2">
         <v>20</v>
       </c>
       <c r="L29" s="14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3377,7 +3382,7 @@
         <v>353</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C30" s="2">
         <v>1.5</v>
@@ -3404,15 +3409,15 @@
         <v>20</v>
       </c>
       <c r="L30" s="14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C31" s="2">
         <v>0.8</v>
@@ -3442,10 +3447,10 @@
     </row>
     <row r="32" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C32" s="2">
         <v>1.5</v>
@@ -3472,15 +3477,15 @@
         <v>10</v>
       </c>
       <c r="L32" s="14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>282</v>
       </c>
       <c r="C33" s="2">
         <v>1.5</v>
@@ -3507,20 +3512,20 @@
         <v>20</v>
       </c>
       <c r="L33" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G34" s="13" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="C35" s="2">
         <v>1.5</v>
@@ -3547,12 +3552,12 @@
         <v>15</v>
       </c>
       <c r="L35" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C36" s="2">
         <v>1.5</v>
@@ -3579,12 +3584,12 @@
         <v>20</v>
       </c>
       <c r="L36" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C37" s="2">
         <v>1.5</v>
@@ -3611,12 +3616,12 @@
         <v>20</v>
       </c>
       <c r="L37" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C38" s="2">
         <v>1.5</v>
@@ -3643,12 +3648,12 @@
         <v>20</v>
       </c>
       <c r="L38" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C39" s="2">
         <v>1.5</v>
@@ -3675,12 +3680,12 @@
         <v>20</v>
       </c>
       <c r="L39" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C40" s="2">
         <v>1.5</v>
@@ -3707,12 +3712,12 @@
         <v>20</v>
       </c>
       <c r="L40" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C41" s="2">
         <v>1.5</v>
@@ -3739,12 +3744,12 @@
         <v>20</v>
       </c>
       <c r="L41" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C42" s="2">
         <v>1.5</v>
@@ -3771,12 +3776,12 @@
         <v>20</v>
       </c>
       <c r="L42" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C43" s="2">
         <v>1</v>
@@ -3803,7 +3808,7 @@
         <v>20</v>
       </c>
       <c r="L43" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3811,16 +3816,16 @@
     </row>
     <row r="45" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="C45" s="2">
         <v>3</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E45" s="2">
         <v>1</v>
@@ -3838,21 +3843,21 @@
         <v>0</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L45" s="14" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="C46" s="2">
         <v>1</v>
@@ -3879,15 +3884,15 @@
         <v>10</v>
       </c>
       <c r="L46" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C47" s="2">
         <v>0.9</v>
@@ -3914,15 +3919,15 @@
         <v>20</v>
       </c>
       <c r="L47" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C48" s="2">
         <v>0.9</v>
@@ -3949,15 +3954,15 @@
         <v>35</v>
       </c>
       <c r="L48" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C49" s="4">
         <v>0.8</v>
@@ -3985,15 +3990,15 @@
         <v>55</v>
       </c>
       <c r="L49" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C50" s="4">
         <v>0.8</v>
@@ -4021,15 +4026,15 @@
         <v>80</v>
       </c>
       <c r="L50" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C51" s="2">
         <v>1</v>
@@ -4056,7 +4061,7 @@
         <v>20</v>
       </c>
       <c r="L51" s="14" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4064,10 +4069,10 @@
     </row>
     <row r="53" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="C53" s="2">
         <v>2</v>
@@ -4095,15 +4100,15 @@
         <v>10</v>
       </c>
       <c r="L53" s="14" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C54" s="2">
         <v>2</v>
@@ -4127,27 +4132,27 @@
         <v>0</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K54" s="2">
         <v>10</v>
       </c>
       <c r="L54" s="14" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B55" s="2" t="s">
-        <v>87</v>
-      </c>
       <c r="C55" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E55" s="2">
         <v>1</v>
@@ -4168,15 +4173,15 @@
         <v>5</v>
       </c>
       <c r="L55" s="14" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="C56" s="2">
         <v>1.5</v>
@@ -4200,21 +4205,21 @@
         <v>3</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K56" s="2">
         <v>50</v>
       </c>
       <c r="L56" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="C57" s="2">
         <v>2</v>
@@ -4238,21 +4243,21 @@
         <v>0</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K57" s="2">
         <v>10</v>
       </c>
       <c r="L57" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="C58" s="2">
         <v>2</v>
@@ -4276,33 +4281,33 @@
         <v>0</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="K58" s="2">
         <v>10</v>
       </c>
       <c r="L58" s="14" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="77.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="C59" s="2">
+        <v>2</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C59" s="2">
-        <v>2</v>
-      </c>
-      <c r="D59" s="2" t="s">
+      <c r="E59" s="2">
+        <v>2</v>
+      </c>
+      <c r="F59" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="E59" s="2">
-        <v>2</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="G59" s="12">
         <v>8</v>
@@ -4314,13 +4319,13 @@
         <v>0</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K59" s="2">
         <v>10</v>
       </c>
       <c r="L59" s="14" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="60" spans="1:12" ht="12.75" x14ac:dyDescent="0.2"/>
@@ -4345,21 +4350,21 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -4386,8 +4391,8 @@
   </sheetPr>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4397,33 +4402,33 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B2" s="2">
         <v>5</v>
@@ -4454,7 +4459,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B3" s="2">
         <v>6</v>
@@ -4485,7 +4490,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B4" s="2">
         <v>4</v>
@@ -4516,7 +4521,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B5" s="2">
         <v>2</v>
@@ -4547,7 +4552,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B6" s="2">
         <v>4</v>
@@ -4578,7 +4583,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B7" s="2">
         <v>1</v>
@@ -4609,10 +4614,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B8" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" s="2">
         <v>4</v>
@@ -4631,16 +4636,16 @@
       </c>
       <c r="H8" s="2">
         <f t="shared" si="0"/>
-        <v>4.333333333333333</v>
+        <v>4.5</v>
       </c>
       <c r="I8" s="2">
         <f t="shared" si="1"/>
-        <v>4.4000000000000004</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -4676,30 +4681,30 @@
         <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>127</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>128</v>
       </c>
       <c r="D2" s="2">
         <v>-1</v>
@@ -4708,7 +4713,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H2" s="2">
         <v>2</v>
@@ -4716,22 +4721,22 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>131</v>
-      </c>
       <c r="C3" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="H3" s="2">
         <v>2</v>
@@ -4739,7 +4744,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B4" s="2">
         <v>4</v>
@@ -4762,7 +4767,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
@@ -4785,7 +4790,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
@@ -4797,7 +4802,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H6" s="2">
         <v>2</v>
@@ -4805,22 +4810,22 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="H7" s="2">
         <v>3</v>
@@ -4828,22 +4833,22 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="B8" s="2">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0</v>
-      </c>
-      <c r="E8" s="6" t="s">
+      <c r="G8" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>139</v>
       </c>
       <c r="H8" s="2">
         <v>4</v>
@@ -4851,25 +4856,25 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>141</v>
       </c>
       <c r="H9" s="2">
         <v>3</v>
@@ -4877,7 +4882,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B10" s="2">
         <v>0</v>
@@ -4889,7 +4894,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H10" s="2">
         <v>2</v>
@@ -4897,19 +4902,19 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>144</v>
       </c>
       <c r="H11" s="2">
         <v>4</v>
@@ -4940,244 +4945,244 @@
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>145</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>148</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>150</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" s="14" t="s">
         <v>152</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>154</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>261</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C10" s="14" t="s">
         <v>157</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C11" s="14" t="s">
         <v>256</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="14" t="s">
         <v>160</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C13" s="14" t="s">
         <v>162</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="14" t="s">
         <v>165</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C15" s="14" t="s">
         <v>167</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C16" s="14" t="s">
         <v>169</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="18" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="19" spans="1:27" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="20" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>172</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="21" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C21" s="14" t="s">
         <v>310</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="22" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C22" s="17" t="s">
         <v>174</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>175</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="3"/>
@@ -5206,35 +5211,35 @@
     </row>
     <row r="23" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C23" s="14" t="s">
         <v>176</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="24" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="25" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -5262,200 +5267,200 @@
   <sheetData>
     <row r="2" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>193</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>314</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>200</v>
-      </c>
       <c r="E24" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>202</v>
       </c>
       <c r="C25" s="2">
         <v>24</v>
@@ -5464,32 +5469,32 @@
         <v>6</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C26" s="2">
         <v>18</v>
       </c>
       <c r="D26" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="E26" s="14" t="s">
         <v>304</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C27" s="2">
         <v>18</v>
@@ -5498,32 +5503,32 @@
         <v>4</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>205</v>
       </c>
       <c r="D28" s="2">
         <v>8</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C29">
         <v>12</v>
@@ -5532,24 +5537,24 @@
         <v>6</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="C30" s="20" t="s">
-        <v>205</v>
-      </c>
-      <c r="D30" s="2" t="s">
+      <c r="E30" s="14" t="s">
         <v>302</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -5576,7 +5581,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B1" s="14">
         <f>6*9</f>
@@ -5589,7 +5594,7 @@
     </row>
     <row r="2" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B2" s="2">
         <f>18*7</f>
@@ -5598,7 +5603,7 @@
     </row>
     <row r="3" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B3" s="2">
         <f>10*2</f>
@@ -5607,7 +5612,7 @@
     </row>
     <row r="6" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B6">
         <v>50</v>
@@ -5615,7 +5620,7 @@
     </row>
     <row r="7" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B7">
         <v>40</v>
@@ -5623,7 +5628,7 @@
     </row>
     <row r="8" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B8">
         <v>40</v>
@@ -5631,7 +5636,7 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B9">
         <v>40</v>
@@ -5639,7 +5644,7 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B10">
         <v>30</v>
@@ -5651,205 +5656,205 @@
     <row r="12" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="71.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="22" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="26" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C29" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>223</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="36" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="44" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B45" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="47" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>234</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="50" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B51" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B52" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="55" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="14" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="57" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="14" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="59" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="61" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -5877,22 +5882,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>249</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="221.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5925,34 +5930,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B1" s="20" t="s">
+        <v>327</v>
+      </c>
+      <c r="C1" s="20" t="s">
         <v>328</v>
       </c>
-      <c r="C1" s="20" t="s">
-        <v>329</v>
-      </c>
       <c r="D1" s="20" t="s">
+        <v>340</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>341</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="F1" s="20" t="s">
         <v>342</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>343</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="H1" s="20" t="s">
         <v>344</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="I1" s="20" t="s">
         <v>345</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="J1" s="20" t="s">
         <v>346</v>
-      </c>
-      <c r="J1" s="20" t="s">
-        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -5977,30 +5982,30 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D1" t="s">
+        <v>333</v>
+      </c>
+      <c r="E1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" t="s">
         <v>334</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>119</v>
-      </c>
-      <c r="F1" t="s">
-        <v>335</v>
-      </c>
-      <c r="G1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="21"/>
@@ -6011,7 +6016,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B3" s="21"/>
       <c r="C3" s="25"/>
@@ -6022,7 +6027,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
@@ -6033,7 +6038,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B5" s="24"/>
       <c r="C5" s="27"/>
@@ -6044,7 +6049,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
@@ -6055,7 +6060,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B7" s="25"/>
       <c r="C7" s="25"/>

</xml_diff>

<commit_message>
Added facion abilities to the primer
</commit_message>
<xml_diff>
--- a/unit stats.xlsx
+++ b/unit stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas\Documents\wargame\wargame-tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6140076B-A978-43CF-B7C5-A2F0B5B0ACBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08AF6AC5-C86E-481B-876D-6264DFD35FF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20520" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20520" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="units new statlines" sheetId="2" r:id="rId1"/>
@@ -842,9 +842,6 @@
     <t>Spore Colony</t>
   </si>
   <si>
-    <t>Releases a cloud of basic spores that fills an area of radius X (2 if not provided) for 3 turns. Each enemy unit that ends its turn within the cloud either becomes infected with the specific Spore type, or adds a counter to an existing Spore infection.  If no enemy units are infected with this cloud after the 3 turns, then return the unit to the battlefield at full Wounds.</t>
-  </si>
-  <si>
     <t>Creates a spore cloud at a location, or adds 3 rounds to an existing cloud while increasing its radius by 2 inches</t>
   </si>
   <si>
@@ -1107,6 +1104,9 @@
   </si>
   <si>
     <t>Royal Emissary</t>
+  </si>
+  <si>
+    <t>Releases a cloud of basic spores that fills an area of radius X (2 if not provided) for 2 turns. Each enemy unit that ends its turn within the cloud either becomes infected with the specific Spore type, or adds a counter to an existing Spore infection.  If no enemy units are infected with this cloud after the 2 turns, then return the unit to the battlefield at full Wounds.</t>
   </si>
 </sst>
 </file>
@@ -2488,7 +2488,7 @@
   </sheetPr>
   <dimension ref="A1:N60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
@@ -2543,7 +2543,7 @@
         <v>13</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -2581,7 +2581,7 @@
         <v>20</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>16</v>
@@ -2669,7 +2669,7 @@
     </row>
     <row r="5" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>19</v>
@@ -2702,7 +2702,7 @@
         <v>96</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -2745,10 +2745,10 @@
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C7" s="2">
         <v>0.75</v>
@@ -2944,7 +2944,7 @@
         <v>30</v>
       </c>
       <c r="L13" s="14" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3073,7 +3073,7 @@
         <v>7</v>
       </c>
       <c r="L19" s="14" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3109,7 +3109,7 @@
         <v>10</v>
       </c>
       <c r="L20" s="14" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -3145,7 +3145,7 @@
         <v>9</v>
       </c>
       <c r="L21" s="14" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3181,7 +3181,7 @@
         <v>13</v>
       </c>
       <c r="L22" s="14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -3265,10 +3265,10 @@
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C27" s="2">
         <v>1.5</v>
@@ -3298,15 +3298,15 @@
         <v>20</v>
       </c>
       <c r="L27" s="14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C28" s="2">
         <v>1.5</v>
@@ -3336,15 +3336,15 @@
         <v>20</v>
       </c>
       <c r="L28" s="14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C29" s="2">
         <v>1.5</v>
@@ -3374,15 +3374,15 @@
         <v>20</v>
       </c>
       <c r="L29" s="14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C30" s="2">
         <v>1.5</v>
@@ -3409,7 +3409,7 @@
         <v>20</v>
       </c>
       <c r="L30" s="14" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3417,7 +3417,7 @@
         <v>45</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C31" s="2">
         <v>0.8</v>
@@ -3447,10 +3447,10 @@
     </row>
     <row r="32" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C32" s="2">
         <v>1.5</v>
@@ -3477,15 +3477,15 @@
         <v>10</v>
       </c>
       <c r="L32" s="14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>280</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>281</v>
       </c>
       <c r="C33" s="2">
         <v>1.5</v>
@@ -3512,12 +3512,12 @@
         <v>20</v>
       </c>
       <c r="L33" s="14" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G34" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3849,7 +3849,7 @@
         <v>33</v>
       </c>
       <c r="L45" s="14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4061,7 +4061,7 @@
         <v>20</v>
       </c>
       <c r="L51" s="14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4100,7 +4100,7 @@
         <v>10</v>
       </c>
       <c r="L53" s="14" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="39" thickBot="1" x14ac:dyDescent="0.25">
@@ -4108,7 +4108,7 @@
         <v>91</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C54" s="2">
         <v>2</v>
@@ -4132,13 +4132,13 @@
         <v>0</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K54" s="2">
         <v>10</v>
       </c>
       <c r="L54" s="14" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4173,7 +4173,7 @@
         <v>5</v>
       </c>
       <c r="L55" s="14" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4243,13 +4243,13 @@
         <v>0</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K57" s="2">
         <v>10</v>
       </c>
       <c r="L57" s="14" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="39" thickBot="1" x14ac:dyDescent="0.25">
@@ -4281,13 +4281,13 @@
         <v>0</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K58" s="2">
         <v>10</v>
       </c>
       <c r="L58" s="14" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="77.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -4325,7 +4325,7 @@
         <v>10</v>
       </c>
       <c r="L59" s="14" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="60" spans="1:12" ht="12.75" x14ac:dyDescent="0.2"/>
@@ -4356,12 +4356,12 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B2" t="s">
         <v>115</v>
@@ -4614,7 +4614,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B8" s="2">
         <v>6</v>
@@ -4932,8 +4932,8 @@
   </sheetPr>
   <dimension ref="A1:AA25"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4962,7 +4962,7 @@
         <v>146</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>266</v>
+        <v>354</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
@@ -5017,7 +5017,7 @@
         <v>155</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
@@ -5028,7 +5028,7 @@
         <v>264</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
@@ -5127,7 +5127,7 @@
         <v>97</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="18" spans="1:27" ht="51" x14ac:dyDescent="0.2">
@@ -5135,10 +5135,10 @@
         <v>158</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="19" spans="1:27" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -5149,7 +5149,7 @@
         <v>170</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="20" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
@@ -5168,10 +5168,10 @@
         <v>158</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C21" s="14" t="s">
         <v>309</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="22" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
@@ -5228,7 +5228,7 @@
         <v>177</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="25" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
@@ -5288,16 +5288,16 @@
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -5315,7 +5315,7 @@
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -5351,7 +5351,7 @@
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -5360,16 +5360,16 @@
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -5378,7 +5378,7 @@
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -5387,7 +5387,7 @@
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
@@ -5400,10 +5400,10 @@
     </row>
     <row r="18" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>313</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
@@ -5421,7 +5421,7 @@
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
@@ -5430,7 +5430,7 @@
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
@@ -5469,7 +5469,7 @@
         <v>6</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
@@ -5483,10 +5483,10 @@
         <v>18</v>
       </c>
       <c r="D26" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="E26" s="14" t="s">
         <v>303</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
@@ -5494,7 +5494,7 @@
         <v>200</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C27" s="2">
         <v>18</v>
@@ -5503,7 +5503,7 @@
         <v>4</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5520,7 +5520,7 @@
         <v>8</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="51" x14ac:dyDescent="0.2">
@@ -5537,24 +5537,24 @@
         <v>6</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>299</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>300</v>
       </c>
       <c r="C30" s="20" t="s">
         <v>204</v>
       </c>
       <c r="D30" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="E30" s="14" t="s">
         <v>301</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -5620,7 +5620,7 @@
     </row>
     <row r="7" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B7">
         <v>40</v>
@@ -5628,7 +5628,7 @@
     </row>
     <row r="8" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B8">
         <v>40</v>
@@ -5636,7 +5636,7 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B9">
         <v>40</v>
@@ -5644,7 +5644,7 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B10">
         <v>30</v>
@@ -5933,31 +5933,31 @@
         <v>107</v>
       </c>
       <c r="B1" s="20" t="s">
+        <v>326</v>
+      </c>
+      <c r="C1" s="20" t="s">
         <v>327</v>
       </c>
-      <c r="C1" s="20" t="s">
-        <v>328</v>
-      </c>
       <c r="D1" s="20" t="s">
+        <v>339</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>340</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="F1" s="20" t="s">
         <v>341</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>342</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="H1" s="20" t="s">
         <v>343</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="I1" s="20" t="s">
         <v>344</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="J1" s="20" t="s">
         <v>345</v>
-      </c>
-      <c r="J1" s="20" t="s">
-        <v>346</v>
       </c>
     </row>
   </sheetData>
@@ -5982,7 +5982,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B1" t="s">
         <v>115</v>
@@ -5991,13 +5991,13 @@
         <v>120</v>
       </c>
       <c r="D1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E1" t="s">
         <v>118</v>
       </c>
       <c r="F1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G1" t="s">
         <v>119</v>
@@ -6027,7 +6027,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
@@ -6049,7 +6049,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>

</xml_diff>

<commit_message>
Revamped equipment table to use basic templates.
</commit_message>
<xml_diff>
--- a/unit stats.xlsx
+++ b/unit stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas\Documents\wargame\wargame-tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Nicholas\Documents\wargame\wargame-tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08AF6AC5-C86E-481B-876D-6264DFD35FF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFBD463F-1CB3-4C32-AC99-78E63F85E19F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20520" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="units new statlines" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="363">
   <si>
     <t>Name</t>
   </si>
@@ -92,9 +92,6 @@
     <t>Basic armored melee unit</t>
   </si>
   <si>
-    <t>May take a Greatsword, Sword/Magic Sword &amp; Shield, or Crushing Claws (Warhammer equivalent) for free</t>
-  </si>
-  <si>
     <t>Hercules Knight</t>
   </si>
   <si>
@@ -422,57 +419,9 @@
     <t>Base Cost</t>
   </si>
   <si>
-    <t>Magic Sword</t>
-  </si>
-  <si>
-    <t>+1</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>Warhammer</t>
-  </si>
-  <si>
-    <t>+2</t>
-  </si>
-  <si>
-    <t>Phase Blaster</t>
-  </si>
-  <si>
-    <t>Rifle</t>
-  </si>
-  <si>
-    <t>Light Armor</t>
-  </si>
-  <si>
-    <t>Medium Armor</t>
-  </si>
-  <si>
-    <t>Movement cost +0.2</t>
-  </si>
-  <si>
-    <t>Heavy Armor</t>
-  </si>
-  <si>
-    <t>+3</t>
-  </si>
-  <si>
-    <t>Movement cost +0.4</t>
-  </si>
-  <si>
-    <t>Speed Amulet</t>
-  </si>
-  <si>
-    <t>Movement cost -0.5 (can't go below 0.75)</t>
-  </si>
-  <si>
     <t>Shield</t>
   </si>
   <si>
-    <t>Greatsword</t>
-  </si>
-  <si>
     <t>Cleave</t>
   </si>
   <si>
@@ -1107,6 +1056,81 @@
   </si>
   <si>
     <t>Releases a cloud of basic spores that fills an area of radius X (2 if not provided) for 2 turns. Each enemy unit that ends its turn within the cloud either becomes infected with the specific Spore type, or adds a counter to an existing Spore infection.  If no enemy units are infected with this cloud after the 2 turns, then return the unit to the battlefield at full Wounds.</t>
+  </si>
+  <si>
+    <t>image loc</t>
+  </si>
+  <si>
+    <t>..\Stag knight.png</t>
+  </si>
+  <si>
+    <t>..\hercules.png</t>
+  </si>
+  <si>
+    <t>Fire</t>
+  </si>
+  <si>
+    <t>Everflame</t>
+  </si>
+  <si>
+    <t>The afflicted unit burns with an unquenchable fire.  At the end of each round, the afflicted unit takes 1 point of damage per stack of Everflame.  If an afflicted unit ends or begins its turn less than 1 inch from another unit, the adjacent unit gains one stack of Everflame.</t>
+  </si>
+  <si>
+    <t>Wall of Flame</t>
+  </si>
+  <si>
+    <t>Blinding Fog</t>
+  </si>
+  <si>
+    <t>Tectonic Rise</t>
+  </si>
+  <si>
+    <t>Wind Tunnel</t>
+  </si>
+  <si>
+    <t>Summons a cloud of haze which obscures vision.  The area counts as difficult terrain, and prevents vision for the purposes of ranged attacks. 20 sq inches max</t>
+  </si>
+  <si>
+    <t>Brings forth a ridge of stone and earth from the ground.  Creates an object up to 30 cubic inches.  Counts as dangerous terrain.  Anything higher than 6 inches counts as impassible.</t>
+  </si>
+  <si>
+    <t>Creates a rectangular area up to 15 square inches.  Pick a direction.  Any unit inside the area moves 1 inch in the specified direction for each inch moved otherwise.  To move against it, the unit must move with two movement penalty levels.</t>
+  </si>
+  <si>
+    <t>Fire/Geomancy</t>
+  </si>
+  <si>
+    <t>Water/Geomancy</t>
+  </si>
+  <si>
+    <t>Earth/Geomancy</t>
+  </si>
+  <si>
+    <t>Air/Geomancy</t>
+  </si>
+  <si>
+    <t>Summons a wall of flame which deals 2 damage to anything crossing through it, and 1 damage to any unit which begins or ends its turn within an inch of it. Up to 6 square inches</t>
+  </si>
+  <si>
+    <t>May take a two-handed weapon, spear, an additional one-handed weapon, or a shield for free</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Offhand weapon</t>
+  </si>
+  <si>
+    <t>Multiattack</t>
+  </si>
+  <si>
+    <t>Two-handed weapon (slashing)</t>
+  </si>
+  <si>
+    <t>Two-handed weapon (crushing)</t>
+  </si>
+  <si>
+    <t>Two-handed weapon (piercing)</t>
   </si>
 </sst>
 </file>
@@ -1116,7 +1140,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmmm\ d\,\ yyyy"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1163,6 +1187,13 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1247,10 +1278,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1299,8 +1331,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2486,11 +2520,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N60"/>
+  <dimension ref="A1:O60"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2502,7 +2536,7 @@
     <col min="12" max="12" width="55.140625" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2543,10 +2577,13 @@
         <v>13</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>318</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -2581,18 +2618,21 @@
         <v>20</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>347</v>
+        <v>330</v>
       </c>
       <c r="M2" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="O2" s="28" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="C3" s="2">
         <v>0.8</v>
@@ -2622,18 +2662,21 @@
         <v>50</v>
       </c>
       <c r="L3" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="O3" s="28" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="C4" s="2">
         <v>0.7</v>
@@ -2663,16 +2706,16 @@
         <v>70</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>353</v>
+        <v>336</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
@@ -2699,18 +2742,18 @@
         <v>20</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -2737,18 +2780,18 @@
         <v>15</v>
       </c>
       <c r="L6" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>274</v>
+        <v>257</v>
       </c>
       <c r="C7" s="2">
         <v>0.75</v>
@@ -2775,15 +2818,15 @@
         <v>20</v>
       </c>
       <c r="L7" s="14" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G8" s="13"/>
     </row>
-    <row r="9" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
@@ -2807,18 +2850,18 @@
         <v>1</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K9" s="2">
         <v>15</v>
       </c>
       <c r="L9" s="14" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="2">
         <v>0.6</v>
@@ -2842,15 +2885,15 @@
         <v>1</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K10" s="2">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
@@ -2877,12 +2920,12 @@
         <v>15</v>
       </c>
       <c r="L11" s="18" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="2">
         <v>1.2</v>
@@ -2909,15 +2952,15 @@
         <v>15</v>
       </c>
       <c r="L12" s="18" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="C13" s="2">
         <v>1</v>
@@ -2944,74 +2987,74 @@
         <v>30</v>
       </c>
       <c r="L13" s="14" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2">
+        <v>2</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="2">
-        <v>2</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="E14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K14" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="C15" s="2">
         <v>2</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K15" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -3040,10 +3083,10 @@
     </row>
     <row r="19" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="13" t="s">
         <v>36</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>37</v>
       </c>
       <c r="C19" s="12">
         <v>1</v>
@@ -3073,15 +3116,15 @@
         <v>7</v>
       </c>
       <c r="L19" s="14" t="s">
-        <v>322</v>
+        <v>305</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="13" t="s">
         <v>38</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>39</v>
       </c>
       <c r="C20" s="12">
         <v>1</v>
@@ -3109,15 +3152,15 @@
         <v>10</v>
       </c>
       <c r="L20" s="14" t="s">
-        <v>325</v>
+        <v>308</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C21" s="12">
         <v>1</v>
@@ -3145,15 +3188,15 @@
         <v>9</v>
       </c>
       <c r="L21" s="14" t="s">
-        <v>324</v>
+        <v>307</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="C22" s="16">
         <v>1</v>
@@ -3181,15 +3224,15 @@
         <v>13</v>
       </c>
       <c r="L22" s="14" t="s">
-        <v>323</v>
+        <v>306</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>265</v>
+        <v>248</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
       <c r="C23" s="16">
         <v>1</v>
@@ -3219,7 +3262,7 @@
         <v>40</v>
       </c>
       <c r="L23" s="14" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3227,10 +3270,10 @@
     </row>
     <row r="25" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="C25" s="2">
         <v>1</v>
@@ -3257,7 +3300,7 @@
         <v>10</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3265,10 +3308,10 @@
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>349</v>
+        <v>332</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>338</v>
+        <v>321</v>
       </c>
       <c r="C27" s="2">
         <v>1.5</v>
@@ -3292,21 +3335,21 @@
         <v>1</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K27" s="2">
         <v>20</v>
       </c>
       <c r="L27" s="14" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>350</v>
+        <v>333</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>338</v>
+        <v>321</v>
       </c>
       <c r="C28" s="2">
         <v>1.5</v>
@@ -3330,21 +3373,21 @@
         <v>1</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K28" s="2">
         <v>20</v>
       </c>
       <c r="L28" s="14" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>351</v>
+        <v>334</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>338</v>
+        <v>321</v>
       </c>
       <c r="C29" s="2">
         <v>1.5</v>
@@ -3368,21 +3411,21 @@
         <v>1</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K29" s="2">
         <v>20</v>
       </c>
       <c r="L29" s="14" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>352</v>
+        <v>335</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>337</v>
+        <v>320</v>
       </c>
       <c r="C30" s="2">
         <v>1.5</v>
@@ -3409,15 +3452,15 @@
         <v>20</v>
       </c>
       <c r="L30" s="14" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
       <c r="C31" s="2">
         <v>0.8</v>
@@ -3447,10 +3490,10 @@
     </row>
     <row r="32" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>348</v>
+        <v>331</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="C32" s="2">
         <v>1.5</v>
@@ -3477,15 +3520,15 @@
         <v>10</v>
       </c>
       <c r="L32" s="14" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
       <c r="C33" s="2">
         <v>1.5</v>
@@ -3512,20 +3555,20 @@
         <v>20</v>
       </c>
       <c r="L33" s="14" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G34" s="13" t="s">
-        <v>282</v>
+        <v>265</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="C35" s="2">
         <v>1.5</v>
@@ -3552,12 +3595,12 @@
         <v>15</v>
       </c>
       <c r="L35" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C36" s="2">
         <v>1.5</v>
@@ -3584,12 +3627,12 @@
         <v>20</v>
       </c>
       <c r="L36" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C37" s="2">
         <v>1.5</v>
@@ -3616,12 +3659,12 @@
         <v>20</v>
       </c>
       <c r="L37" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C38" s="2">
         <v>1.5</v>
@@ -3648,12 +3691,12 @@
         <v>20</v>
       </c>
       <c r="L38" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C39" s="2">
         <v>1.5</v>
@@ -3680,12 +3723,12 @@
         <v>20</v>
       </c>
       <c r="L39" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C40" s="2">
         <v>1.5</v>
@@ -3712,12 +3755,12 @@
         <v>20</v>
       </c>
       <c r="L40" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C41" s="2">
         <v>1.5</v>
@@ -3744,12 +3787,12 @@
         <v>20</v>
       </c>
       <c r="L41" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C42" s="2">
         <v>1.5</v>
@@ -3776,12 +3819,12 @@
         <v>20</v>
       </c>
       <c r="L42" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C43" s="2">
         <v>1</v>
@@ -3808,7 +3851,7 @@
         <v>20</v>
       </c>
       <c r="L43" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3816,16 +3859,16 @@
     </row>
     <row r="45" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="C45" s="2">
         <v>3</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E45" s="2">
         <v>1</v>
@@ -3843,21 +3886,21 @@
         <v>0</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L45" s="14" t="s">
-        <v>318</v>
+        <v>301</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="C46" s="2">
         <v>1</v>
@@ -3884,15 +3927,15 @@
         <v>10</v>
       </c>
       <c r="L46" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C47" s="2">
         <v>0.9</v>
@@ -3919,15 +3962,15 @@
         <v>20</v>
       </c>
       <c r="L47" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C48" s="2">
         <v>0.9</v>
@@ -3954,15 +3997,15 @@
         <v>35</v>
       </c>
       <c r="L48" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C49" s="4">
         <v>0.8</v>
@@ -3990,15 +4033,15 @@
         <v>55</v>
       </c>
       <c r="L49" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C50" s="4">
         <v>0.8</v>
@@ -4026,15 +4069,15 @@
         <v>80</v>
       </c>
       <c r="L50" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C51" s="2">
         <v>1</v>
@@ -4061,7 +4104,7 @@
         <v>20</v>
       </c>
       <c r="L51" s="14" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4069,10 +4112,10 @@
     </row>
     <row r="53" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="C53" s="2">
         <v>2</v>
@@ -4100,15 +4143,15 @@
         <v>10</v>
       </c>
       <c r="L53" s="14" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>295</v>
+        <v>278</v>
       </c>
       <c r="C54" s="2">
         <v>2</v>
@@ -4132,27 +4175,27 @@
         <v>0</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>294</v>
+        <v>277</v>
       </c>
       <c r="K54" s="2">
         <v>10</v>
       </c>
       <c r="L54" s="14" t="s">
-        <v>296</v>
+        <v>279</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B55" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="C55" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E55" s="2">
         <v>1</v>
@@ -4173,15 +4216,15 @@
         <v>5</v>
       </c>
       <c r="L55" s="14" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="C56" s="2">
         <v>1.5</v>
@@ -4205,21 +4248,21 @@
         <v>3</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K56" s="2">
         <v>50</v>
       </c>
       <c r="L56" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="C57" s="2">
         <v>2</v>
@@ -4243,21 +4286,21 @@
         <v>0</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>293</v>
+        <v>276</v>
       </c>
       <c r="K57" s="2">
         <v>10</v>
       </c>
       <c r="L57" s="14" t="s">
-        <v>292</v>
+        <v>275</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="C58" s="2">
         <v>2</v>
@@ -4281,33 +4324,33 @@
         <v>0</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>291</v>
+        <v>274</v>
       </c>
       <c r="K58" s="2">
         <v>10</v>
       </c>
       <c r="L58" s="14" t="s">
-        <v>290</v>
+        <v>273</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="77.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="C59" s="2">
+        <v>2</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C59" s="2">
-        <v>2</v>
-      </c>
-      <c r="D59" s="2" t="s">
+      <c r="E59" s="2">
+        <v>2</v>
+      </c>
+      <c r="F59" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="E59" s="2">
-        <v>2</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="G59" s="12">
         <v>8</v>
@@ -4319,19 +4362,23 @@
         <v>0</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K59" s="2">
         <v>10</v>
       </c>
       <c r="L59" s="14" t="s">
-        <v>285</v>
+        <v>268</v>
       </c>
     </row>
     <row r="60" spans="1:12" ht="12.75" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="O2" r:id="rId1" display="..\Stag knight.jpg" xr:uid="{051090D8-9F0F-4C9A-A707-1EB36D88B061}"/>
+    <hyperlink ref="O3" r:id="rId2" display="..\hercules.jpg" xr:uid="{B10553E2-CAEF-42FE-8070-D95757733EDB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -4350,21 +4397,21 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>344</v>
+        <v>327</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>346</v>
+        <v>329</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -4402,33 +4449,33 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B2" s="2">
         <v>5</v>
@@ -4459,7 +4506,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" s="2">
         <v>6</v>
@@ -4490,7 +4537,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B4" s="2">
         <v>4</v>
@@ -4521,7 +4568,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B5" s="2">
         <v>2</v>
@@ -4552,7 +4599,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B6" s="2">
         <v>4</v>
@@ -4583,7 +4630,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B7" s="2">
         <v>1</v>
@@ -4614,7 +4661,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>332</v>
+        <v>315</v>
       </c>
       <c r="B8" s="2">
         <v>6</v>
@@ -4645,7 +4692,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -4661,11 +4708,13 @@
   </sheetPr>
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.85546875" customWidth="1"/>
     <col min="7" max="7" width="31.42578125" customWidth="1"/>
   </cols>
@@ -4681,244 +4730,138 @@
         <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>126</v>
+        <v>362</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>127</v>
+        <v>357</v>
       </c>
       <c r="D2" s="2">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="2">
         <v>0</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H2" s="2">
-        <v>2</v>
-      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H3" s="2">
-        <v>2</v>
-      </c>
+        <v>358</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" t="s">
+        <v>359</v>
+      </c>
+      <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B4" s="2">
-        <v>4</v>
-      </c>
-      <c r="C4" s="2">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2">
-        <v>-3</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2">
-        <v>8</v>
-      </c>
-      <c r="H4" s="2">
-        <v>10</v>
-      </c>
+        <v>360</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B5" s="2">
-        <v>4</v>
-      </c>
-      <c r="C5" s="2">
-        <v>4</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
       <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>16</v>
-      </c>
-      <c r="H5" s="2">
-        <v>4</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B6" s="2">
-        <v>0</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0</v>
-      </c>
+        <v>361</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
       <c r="D6" s="2">
-        <v>0</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="H6" s="2">
-        <v>2</v>
-      </c>
+        <v>-2</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="H7" s="2">
-        <v>3</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="6"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B8" s="2">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="H8" s="2">
-        <v>4</v>
-      </c>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="6"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="H9" s="2">
-        <v>3</v>
-      </c>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="H10" s="2">
-        <v>2</v>
-      </c>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="6"/>
+      <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="H11" s="2">
-        <v>4</v>
-      </c>
+      <c r="A11" s="2"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4932,7 +4875,7 @@
   </sheetPr>
   <dimension ref="A1:AA25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -4945,244 +4888,244 @@
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>354</v>
+        <v>337</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>264</v>
+        <v>247</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>328</v>
+        <v>311</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>260</v>
+        <v>243</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>261</v>
+        <v>244</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>256</v>
+        <v>239</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>330</v>
+        <v>313</v>
       </c>
     </row>
     <row r="18" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>336</v>
+        <v>319</v>
       </c>
     </row>
     <row r="19" spans="1:27" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>329</v>
+        <v>312</v>
       </c>
     </row>
     <row r="20" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>308</v>
+        <v>291</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>309</v>
+        <v>292</v>
       </c>
     </row>
     <row r="22" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="3"/>
@@ -5211,35 +5154,35 @@
     </row>
     <row r="23" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>175</v>
-      </c>
       <c r="C23" s="14" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>331</v>
+        <v>314</v>
       </c>
     </row>
     <row r="25" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -5252,14 +5195,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:E30"/>
+  <dimension ref="A2:E35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
     <col min="5" max="5" width="71.140625" style="18" customWidth="1"/>
@@ -5267,200 +5211,200 @@
   <sheetData>
     <row r="2" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="6" t="s">
-        <v>270</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="6" t="s">
-        <v>269</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="6" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="6" t="s">
-        <v>311</v>
+        <v>294</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="6" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>253</v>
+        <v>236</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
-        <v>188</v>
+        <v>171</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>306</v>
+        <v>289</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>307</v>
+        <v>290</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
-        <v>317</v>
+        <v>300</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>321</v>
+        <v>304</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="6" t="s">
-        <v>310</v>
+        <v>293</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>304</v>
+        <v>287</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
-        <v>312</v>
+        <v>295</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>313</v>
+        <v>296</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
-        <v>254</v>
+        <v>237</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="6" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>201</v>
+        <v>184</v>
       </c>
       <c r="C25" s="2">
         <v>24</v>
@@ -5469,32 +5413,32 @@
         <v>6</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>319</v>
+        <v>302</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>202</v>
+        <v>185</v>
       </c>
       <c r="C26" s="2">
         <v>18</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>302</v>
+        <v>285</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>303</v>
+        <v>286</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>315</v>
+        <v>298</v>
       </c>
       <c r="C27" s="2">
         <v>18</v>
@@ -5503,32 +5447,32 @@
         <v>4</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>316</v>
+        <v>299</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>203</v>
+        <v>186</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
       <c r="D28" s="2">
         <v>8</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>314</v>
+        <v>297</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
       <c r="C29">
         <v>12</v>
@@ -5537,24 +5481,85 @@
         <v>6</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>320</v>
+        <v>303</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>298</v>
+        <v>281</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>299</v>
+        <v>282</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>300</v>
+        <v>283</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>301</v>
+        <v>284</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C31" s="2">
+        <v>6</v>
+      </c>
+      <c r="D31" s="2">
+        <v>6</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -5581,7 +5586,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>206</v>
+        <v>189</v>
       </c>
       <c r="B1" s="14">
         <f>6*9</f>
@@ -5594,7 +5599,7 @@
     </row>
     <row r="2" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>207</v>
+        <v>190</v>
       </c>
       <c r="B2" s="2">
         <f>18*7</f>
@@ -5603,7 +5608,7 @@
     </row>
     <row r="3" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>208</v>
+        <v>191</v>
       </c>
       <c r="B3" s="2">
         <f>10*2</f>
@@ -5612,7 +5617,7 @@
     </row>
     <row r="6" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>209</v>
+        <v>192</v>
       </c>
       <c r="B6">
         <v>50</v>
@@ -5620,7 +5625,7 @@
     </row>
     <row r="7" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>288</v>
+        <v>271</v>
       </c>
       <c r="B7">
         <v>40</v>
@@ -5628,7 +5633,7 @@
     </row>
     <row r="8" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>286</v>
+        <v>269</v>
       </c>
       <c r="B8">
         <v>40</v>
@@ -5636,7 +5641,7 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>289</v>
+        <v>272</v>
       </c>
       <c r="B9">
         <v>40</v>
@@ -5644,7 +5649,7 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>287</v>
+        <v>270</v>
       </c>
       <c r="B10">
         <v>30</v>
@@ -5656,205 +5661,205 @@
     <row r="12" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="71.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="22" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="26" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C29" s="2" t="s">
-        <v>219</v>
+        <v>202</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
-        <v>219</v>
+        <v>202</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>221</v>
+        <v>204</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>222</v>
+        <v>205</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
-        <v>222</v>
+        <v>205</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="14" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="36" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="14" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="14" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="14" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="44" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="14" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B45" s="2" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="47" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="14" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
-        <v>235</v>
+        <v>218</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="50" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="14" t="s">
-        <v>236</v>
+        <v>219</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B51" s="2" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B52" s="2" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="55" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="14" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="57" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="14" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="59" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="14" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="61" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="14" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -5882,22 +5887,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>244</v>
+        <v>227</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>247</v>
+        <v>230</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>248</v>
+        <v>231</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="221.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5930,34 +5935,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B1" s="20" t="s">
+        <v>309</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>310</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>322</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>323</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>324</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>325</v>
+      </c>
+      <c r="H1" s="20" t="s">
         <v>326</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="I1" s="20" t="s">
         <v>327</v>
       </c>
-      <c r="D1" s="20" t="s">
-        <v>339</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>340</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>341</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>342</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>343</v>
-      </c>
-      <c r="I1" s="20" t="s">
-        <v>344</v>
-      </c>
       <c r="J1" s="20" t="s">
-        <v>345</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -5982,30 +5987,30 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>334</v>
+        <v>317</v>
       </c>
       <c r="B1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D1" t="s">
-        <v>332</v>
+        <v>315</v>
       </c>
       <c r="E1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" t="s">
+        <v>316</v>
+      </c>
+      <c r="G1" t="s">
         <v>118</v>
-      </c>
-      <c r="F1" t="s">
-        <v>333</v>
-      </c>
-      <c r="G1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="21"/>
@@ -6016,7 +6021,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B3" s="21"/>
       <c r="C3" s="25"/>
@@ -6027,7 +6032,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>332</v>
+        <v>315</v>
       </c>
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
@@ -6038,7 +6043,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B5" s="24"/>
       <c r="C5" s="27"/>
@@ -6049,7 +6054,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>333</v>
+        <v>316</v>
       </c>
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
@@ -6060,7 +6065,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B7" s="25"/>
       <c r="C7" s="25"/>

</xml_diff>

<commit_message>
Added Defy Death ability and updated Mine Plant damage
</commit_message>
<xml_diff>
--- a/unit stats.xlsx
+++ b/unit stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Nicholas\Documents\wargame\wargame-tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFBD463F-1CB3-4C32-AC99-78E63F85E19F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F42B44-140B-440B-BC65-E03C8FC64942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="units new statlines" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="365">
   <si>
     <t>Name</t>
   </si>
@@ -356,9 +356,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>6-R</t>
-  </si>
-  <si>
     <t>3R</t>
   </si>
   <si>
@@ -842,15 +839,9 @@
     <t>.</t>
   </si>
   <si>
-    <t>Root, Seed 12</t>
-  </si>
-  <si>
     <t>You may take one Root Cluster for free.  Starts rooted.  Seed 8</t>
   </si>
   <si>
-    <t>Root, Seed 12, True Damage 2, When an enemy unit is within 3 inches of this, it triggers a free Opportunity Attack from this unit.  This can be avoided with a penalty level; otherwise this unit automatically explodes, leaving behind a Root Cluster and damaging all enemy units within Range.  The Root Cluster share's this unit's Seed ability</t>
-  </si>
-  <si>
     <t>Tunnel Sapper x2</t>
   </si>
   <si>
@@ -1131,6 +1122,21 @@
   </si>
   <si>
     <t>Two-handed weapon (piercing)</t>
+  </si>
+  <si>
+    <t>Defy Death</t>
+  </si>
+  <si>
+    <t>If this model has more than 1 Wound remaining as an Attack against it begins, that Attack cannot reduce it to less than 1 Wound.  All excess damage is prevented.</t>
+  </si>
+  <si>
+    <t>Root, Seed 12, Defy Death</t>
+  </si>
+  <si>
+    <t>6-R ( 3 to 5 damage)</t>
+  </si>
+  <si>
+    <t>Root, Seed 12, True Damage 2</t>
   </si>
 </sst>
 </file>
@@ -2522,9 +2528,9 @@
   </sheetPr>
   <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2577,10 +2583,10 @@
         <v>13</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -2618,13 +2624,13 @@
         <v>20</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="O2" s="28" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -2665,10 +2671,10 @@
         <v>91</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="O3" s="28" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -2712,7 +2718,7 @@
     </row>
     <row r="5" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>18</v>
@@ -2745,7 +2751,7 @@
         <v>95</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -2788,10 +2794,10 @@
     </row>
     <row r="7" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C7" s="2">
         <v>0.75</v>
@@ -2856,7 +2862,7 @@
         <v>15</v>
       </c>
       <c r="L9" s="14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -2920,7 +2926,7 @@
         <v>15</v>
       </c>
       <c r="L11" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -2952,7 +2958,7 @@
         <v>15</v>
       </c>
       <c r="L12" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -2987,7 +2993,7 @@
         <v>30</v>
       </c>
       <c r="L13" s="14" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3116,7 +3122,7 @@
         <v>7</v>
       </c>
       <c r="L19" s="14" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3152,7 +3158,7 @@
         <v>10</v>
       </c>
       <c r="L20" s="14" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -3188,15 +3194,15 @@
         <v>9</v>
       </c>
       <c r="L21" s="14" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="B22" s="15" t="s">
         <v>241</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>242</v>
       </c>
       <c r="C22" s="16">
         <v>1</v>
@@ -3224,15 +3230,15 @@
         <v>13</v>
       </c>
       <c r="L22" s="14" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C23" s="16">
         <v>1</v>
@@ -3262,7 +3268,7 @@
         <v>40</v>
       </c>
       <c r="L23" s="14" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3308,10 +3314,10 @@
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C27" s="2">
         <v>1.5</v>
@@ -3341,15 +3347,15 @@
         <v>20</v>
       </c>
       <c r="L27" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C28" s="2">
         <v>1.5</v>
@@ -3379,15 +3385,15 @@
         <v>20</v>
       </c>
       <c r="L28" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C29" s="2">
         <v>1.5</v>
@@ -3417,15 +3423,15 @@
         <v>20</v>
       </c>
       <c r="L29" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C30" s="2">
         <v>1.5</v>
@@ -3452,7 +3458,7 @@
         <v>20</v>
       </c>
       <c r="L30" s="14" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3460,7 +3466,7 @@
         <v>44</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C31" s="2">
         <v>0.8</v>
@@ -3490,10 +3496,10 @@
     </row>
     <row r="32" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C32" s="2">
         <v>1.5</v>
@@ -3520,15 +3526,15 @@
         <v>10</v>
       </c>
       <c r="L32" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>263</v>
       </c>
       <c r="C33" s="2">
         <v>1.5</v>
@@ -3555,12 +3561,12 @@
         <v>20</v>
       </c>
       <c r="L33" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G34" s="13" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3892,7 +3898,7 @@
         <v>32</v>
       </c>
       <c r="L45" s="14" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4002,7 +4008,7 @@
     </row>
     <row r="49" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>75</v>
@@ -4104,7 +4110,7 @@
         <v>20</v>
       </c>
       <c r="L51" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4143,7 +4149,7 @@
         <v>10</v>
       </c>
       <c r="L53" s="14" t="s">
-        <v>266</v>
+        <v>362</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="39" thickBot="1" x14ac:dyDescent="0.25">
@@ -4151,7 +4157,7 @@
         <v>90</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C54" s="2">
         <v>2</v>
@@ -4175,13 +4181,13 @@
         <v>0</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="K54" s="2">
         <v>10</v>
       </c>
       <c r="L54" s="14" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4216,7 +4222,7 @@
         <v>5</v>
       </c>
       <c r="L55" s="14" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4239,7 +4245,7 @@
         <v>7</v>
       </c>
       <c r="G56" s="12">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="H56" s="2">
         <v>2</v>
@@ -4286,13 +4292,13 @@
         <v>0</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="K57" s="2">
         <v>10</v>
       </c>
       <c r="L57" s="14" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="39" thickBot="1" x14ac:dyDescent="0.25">
@@ -4324,16 +4330,16 @@
         <v>0</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="K58" s="2">
         <v>10</v>
       </c>
       <c r="L58" s="14" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" ht="77.25" thickBot="1" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>101</v>
       </c>
@@ -4350,7 +4356,7 @@
         <v>2</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>104</v>
+        <v>363</v>
       </c>
       <c r="G59" s="12">
         <v>8</v>
@@ -4362,13 +4368,13 @@
         <v>0</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K59" s="2">
         <v>10</v>
       </c>
       <c r="L59" s="14" t="s">
-        <v>268</v>
+        <v>364</v>
       </c>
     </row>
     <row r="60" spans="1:12" ht="12.75" x14ac:dyDescent="0.2"/>
@@ -4397,21 +4403,21 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -4449,33 +4455,33 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B2" s="2">
         <v>5</v>
@@ -4506,7 +4512,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B3" s="2">
         <v>6</v>
@@ -4537,7 +4543,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B4" s="2">
         <v>4</v>
@@ -4568,7 +4574,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B5" s="2">
         <v>2</v>
@@ -4599,7 +4605,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B6" s="2">
         <v>4</v>
@@ -4630,7 +4636,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B7" s="2">
         <v>1</v>
@@ -4661,7 +4667,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B8" s="2">
         <v>6</v>
@@ -4692,7 +4698,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -4708,7 +4714,7 @@
   </sheetPr>
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -4730,30 +4736,30 @@
         <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
@@ -4768,7 +4774,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -4776,13 +4782,13 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -4790,13 +4796,13 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -4809,7 +4815,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -4873,10 +4879,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA25"/>
+  <dimension ref="A1:AA26"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4888,244 +4894,244 @@
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>130</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>132</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" s="14" t="s">
         <v>134</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>136</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>243</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C10" s="14" t="s">
         <v>139</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C11" s="14" t="s">
         <v>238</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="14" t="s">
         <v>142</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C13" s="14" t="s">
         <v>144</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="14" t="s">
         <v>147</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C15" s="14" t="s">
         <v>149</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C16" s="14" t="s">
         <v>151</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="18" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="19" spans="1:27" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="20" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>154</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="22" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C22" s="17" t="s">
         <v>156</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>157</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="3"/>
@@ -5152,37 +5158,72 @@
       <c r="Z22" s="3"/>
       <c r="AA22" s="3"/>
     </row>
-    <row r="23" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B23" s="2" t="s">
+    <row r="23" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>361</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+      <c r="V23" s="3"/>
+      <c r="W23" s="3"/>
+      <c r="X23" s="3"/>
+      <c r="Y23" s="3"/>
+      <c r="Z23" s="3"/>
+      <c r="AA23" s="3"/>
+    </row>
+    <row r="24" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C24" s="14" t="s">
         <v>158</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="24" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="25" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C25" s="14" t="s">
-        <v>161</v>
+      <c r="C26" s="14" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -5211,200 +5252,200 @@
   <sheetData>
     <row r="2" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="6" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="6" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>184</v>
       </c>
       <c r="C25" s="2">
         <v>24</v>
@@ -5413,32 +5454,32 @@
         <v>6</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C26" s="2">
         <v>18</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C27" s="2">
         <v>18</v>
@@ -5447,32 +5488,32 @@
         <v>4</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>186</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>187</v>
       </c>
       <c r="D28" s="2">
         <v>8</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C29">
         <v>12</v>
@@ -5481,32 +5522,32 @@
         <v>6</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="E30" s="14" t="s">
         <v>281</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="C30" s="20" t="s">
-        <v>187</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C31" s="2">
         <v>6</v>
@@ -5515,51 +5556,51 @@
         <v>6</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="E33" s="18" t="s">
         <v>345</v>
-      </c>
-      <c r="E33" s="18" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E34" s="18" t="s">
         <v>346</v>
-      </c>
-      <c r="E34" s="18" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="E35" s="18" t="s">
         <v>347</v>
-      </c>
-      <c r="E35" s="18" t="s">
-        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -5586,7 +5627,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B1" s="14">
         <f>6*9</f>
@@ -5599,7 +5640,7 @@
     </row>
     <row r="2" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B2" s="2">
         <f>18*7</f>
@@ -5608,7 +5649,7 @@
     </row>
     <row r="3" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B3" s="2">
         <f>10*2</f>
@@ -5617,7 +5658,7 @@
     </row>
     <row r="6" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B6">
         <v>50</v>
@@ -5625,7 +5666,7 @@
     </row>
     <row r="7" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B7">
         <v>40</v>
@@ -5633,7 +5674,7 @@
     </row>
     <row r="8" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B8">
         <v>40</v>
@@ -5641,7 +5682,7 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B9">
         <v>40</v>
@@ -5649,7 +5690,7 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B10">
         <v>30</v>
@@ -5661,162 +5702,162 @@
     <row r="12" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="71.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="22" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="26" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C29" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>207</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="36" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="44" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B45" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="47" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>216</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="50" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>96</v>
@@ -5824,42 +5865,42 @@
     </row>
     <row r="51" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B51" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B52" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="55" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="57" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="59" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="61" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -5887,22 +5928,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>231</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="221.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5935,34 +5976,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D1" s="20" t="s">
+        <v>319</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>320</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>321</v>
+      </c>
+      <c r="G1" s="20" t="s">
         <v>322</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="H1" s="20" t="s">
         <v>323</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="I1" s="20" t="s">
         <v>324</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="J1" s="20" t="s">
         <v>325</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>326</v>
-      </c>
-      <c r="I1" s="20" t="s">
-        <v>327</v>
-      </c>
-      <c r="J1" s="20" t="s">
-        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -5987,30 +6028,30 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="E1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" t="s">
+        <v>313</v>
+      </c>
+      <c r="G1" t="s">
         <v>117</v>
-      </c>
-      <c r="F1" t="s">
-        <v>316</v>
-      </c>
-      <c r="G1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="21"/>
@@ -6021,7 +6062,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B3" s="21"/>
       <c r="C3" s="25"/>
@@ -6032,7 +6073,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
@@ -6043,7 +6084,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B5" s="24"/>
       <c r="C5" s="27"/>
@@ -6054,7 +6095,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
@@ -6065,7 +6106,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B7" s="25"/>
       <c r="C7" s="25"/>

</xml_diff>

<commit_message>
Added traits.  Keyworded some abilities
</commit_message>
<xml_diff>
--- a/unit stats.xlsx
+++ b/unit stats.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Nicholas\Documents\wargame\wargame-tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F42B44-140B-440B-BC65-E03C8FC64942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07DC9422-0F47-48D4-B0C6-2C2327332F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="units new statlines" sheetId="2" r:id="rId1"/>
     <sheet name="Faction breakdown" sheetId="3" r:id="rId2"/>
     <sheet name="Equipment" sheetId="4" r:id="rId3"/>
-    <sheet name="Abilities" sheetId="5" r:id="rId4"/>
-    <sheet name="Faction info" sheetId="6" r:id="rId5"/>
-    <sheet name="Sample lists" sheetId="7" r:id="rId6"/>
-    <sheet name="Game notes" sheetId="8" r:id="rId7"/>
-    <sheet name="Lore" sheetId="9" r:id="rId8"/>
-    <sheet name="Relationships" sheetId="10" r:id="rId9"/>
-    <sheet name="Notable figures" sheetId="11" r:id="rId10"/>
-    <sheet name="Notable Locations" sheetId="12" r:id="rId11"/>
+    <sheet name="Traits" sheetId="13" r:id="rId4"/>
+    <sheet name="Abilities" sheetId="5" r:id="rId5"/>
+    <sheet name="Faction info" sheetId="6" r:id="rId6"/>
+    <sheet name="Sample lists" sheetId="7" r:id="rId7"/>
+    <sheet name="Game notes" sheetId="8" r:id="rId8"/>
+    <sheet name="Lore" sheetId="9" r:id="rId9"/>
+    <sheet name="Relationships" sheetId="10" r:id="rId10"/>
+    <sheet name="Notable figures" sheetId="11" r:id="rId11"/>
+    <sheet name="Notable Locations" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="431">
   <si>
     <t>Name</t>
   </si>
@@ -1046,9 +1047,6 @@
     <t>Royal Emissary</t>
   </si>
   <si>
-    <t>Releases a cloud of basic spores that fills an area of radius X (2 if not provided) for 2 turns. Each enemy unit that ends its turn within the cloud either becomes infected with the specific Spore type, or adds a counter to an existing Spore infection.  If no enemy units are infected with this cloud after the 2 turns, then return the unit to the battlefield at full Wounds.</t>
-  </si>
-  <si>
     <t>image loc</t>
   </si>
   <si>
@@ -1130,13 +1128,214 @@
     <t>If this model has more than 1 Wound remaining as an Attack against it begins, that Attack cannot reduce it to less than 1 Wound.  All excess damage is prevented.</t>
   </si>
   <si>
-    <t>Root, Seed 12, Defy Death</t>
-  </si>
-  <si>
     <t>6-R ( 3 to 5 damage)</t>
   </si>
   <si>
     <t>Root, Seed 12, True Damage 2</t>
+  </si>
+  <si>
+    <t>Oathsworn Stag Knight</t>
+  </si>
+  <si>
+    <t>Relentless 1, Dauntless 1, Flying, Gains +1A, Defy Death, +1P, +1T, +6W or -0.25 AC</t>
+  </si>
+  <si>
+    <t>Root, Seed 12, Defy Death, Ensnare</t>
+  </si>
+  <si>
+    <t>Ensnare</t>
+  </si>
+  <si>
+    <t>An enemy unit within 1 inch of this unit cannot move unless it takes 2 penalty levels to Movement for the entire Move action.</t>
+  </si>
+  <si>
+    <t>ss</t>
+  </si>
+  <si>
+    <t>Releases a cloud of basic spores that fills an area of radius X (2 if not provided) for 2 turns. Each enemy unit that ends its turn within the cloud either becomes infected with the specific Spore type, or adds a counter to an existing Spore infection.  If no enemy units are infected with this cloud after the 2 turns, then return the unit to the battlefield at full Wounds.  A unit with Spore Cloud may also spend 6 Activation Points to create a cloud until the end of the round centered on their location.  This cloud may be any type of spore the unit may normally make.  Upon dispersal, this cloud does not create a Grunt</t>
+  </si>
+  <si>
+    <t>Phase Out</t>
+  </si>
+  <si>
+    <t>You may skip activation this turn.</t>
+  </si>
+  <si>
+    <t>Synchronize</t>
+  </si>
+  <si>
+    <t>You may spread your Activations across multiple units this turn.  You may only spend 12 points this way, and each unit is still limited to a single type of each Action.</t>
+  </si>
+  <si>
+    <t>Parallelize</t>
+  </si>
+  <si>
+    <t>You may activate up to three different units this turn.  You may only spend up to 12 Activation Points per unit, and you are limited to only one of each Action type, across all selected units.</t>
+  </si>
+  <si>
+    <t>Each turn you may choose Parallelize, Synchronize, or Phase out and gain its effects.  You may not use the same ability two turns in a row.</t>
+  </si>
+  <si>
+    <t>Ranged weapon</t>
+  </si>
+  <si>
+    <t>Heavy Ranged Weapon</t>
+  </si>
+  <si>
+    <t>+1</t>
+  </si>
+  <si>
+    <t>Hograx</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>Hardy</t>
+  </si>
+  <si>
+    <t>+1T</t>
+  </si>
+  <si>
+    <t>Sure-Footed</t>
+  </si>
+  <si>
+    <t>Ignores diff terrain</t>
+  </si>
+  <si>
+    <t>Quick</t>
+  </si>
+  <si>
+    <t>+1 inch when moving 6+ inches</t>
+  </si>
+  <si>
+    <t>Brutish</t>
+  </si>
+  <si>
+    <t>+1S</t>
+  </si>
+  <si>
+    <t>Precise</t>
+  </si>
+  <si>
+    <t>When attacking, disregard enemy's Toughness</t>
+  </si>
+  <si>
+    <t>Heroic</t>
+  </si>
+  <si>
+    <t>When this unit contests an Objective, if no other contesting unit has Heroic, you control the objective</t>
+  </si>
+  <si>
+    <t>Counts as charging +3 inches</t>
+  </si>
+  <si>
+    <t>Tackler</t>
+  </si>
+  <si>
+    <t>Slippery</t>
+  </si>
+  <si>
+    <t>Immune to Opportunity Attacks and Ensnare</t>
+  </si>
+  <si>
+    <t>Professional</t>
+  </si>
+  <si>
+    <t>+1 AP</t>
+  </si>
+  <si>
+    <t>Battle-hardened</t>
+  </si>
+  <si>
+    <t>+10% Wounds</t>
+  </si>
+  <si>
+    <t>Vanguard</t>
+  </si>
+  <si>
+    <t>May deploy up to 6" outside your deployment zone. May not deploy in opponent's deployment zone</t>
+  </si>
+  <si>
+    <t>Grit</t>
+  </si>
+  <si>
+    <t>Grants the Grit ability</t>
+  </si>
+  <si>
+    <t>Tough</t>
+  </si>
+  <si>
+    <t>Defense</t>
+  </si>
+  <si>
+    <t>Movement</t>
+  </si>
+  <si>
+    <t>Logistics</t>
+  </si>
+  <si>
+    <t>Frail</t>
+  </si>
+  <si>
+    <t>-1T</t>
+  </si>
+  <si>
+    <t>This unit does not suffer the usual penalties for being Wounded.</t>
+  </si>
+  <si>
+    <t>Difficult Terrain counts as Dangerous Terrain, and Dangerous becomes Impassible</t>
+  </si>
+  <si>
+    <t>Wounded threshold increases from 25% to 50%</t>
+  </si>
+  <si>
+    <t>When this unit takes damage for the first time each round, increase the amount by 1</t>
+  </si>
+  <si>
+    <t>-2 AP</t>
+  </si>
+  <si>
+    <t>Lazy</t>
+  </si>
+  <si>
+    <t>Late</t>
+  </si>
+  <si>
+    <t>Enters from your table edge at the beginning of Round 2</t>
+  </si>
+  <si>
+    <t>-1 Armor Penetration</t>
+  </si>
+  <si>
+    <t>Butterfingers</t>
+  </si>
+  <si>
+    <t>Bad Eyes</t>
+  </si>
+  <si>
+    <t>Counts as -2S when opposing Toughness (minimum 1)</t>
+  </si>
+  <si>
+    <t>-1R (minimum 0)</t>
+  </si>
+  <si>
+    <t>Enemy Opportunity Attacks and Ensnare range is increased by 1 inch</t>
+  </si>
+  <si>
+    <t>Objective Control Range is reduced by 1 inch</t>
+  </si>
+  <si>
+    <t>Old Wounds</t>
+  </si>
+  <si>
+    <t>Nervous</t>
+  </si>
+  <si>
+    <t>Inattentive</t>
+  </si>
+  <si>
+    <t>When getting the cost for this unit's Movement, it counts as moving one more inch</t>
   </si>
 </sst>
 </file>
@@ -1203,7 +1402,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1252,6 +1451,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1288,7 +1511,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1338,6 +1561,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2526,11 +2755,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:O60"/>
+  <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B63" sqref="B63"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2586,7 +2815,7 @@
         <v>315</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -2627,139 +2856,145 @@
         <v>327</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="O2" s="28" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="2" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
         <v>2</v>
       </c>
-      <c r="E3" s="2">
-        <v>7</v>
-      </c>
-      <c r="F3" s="2">
-        <v>7</v>
-      </c>
-      <c r="G3" s="12">
-        <v>40</v>
+      <c r="E3" s="1">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1">
+        <v>5</v>
+      </c>
+      <c r="G3" s="11">
+        <v>24</v>
       </c>
       <c r="H3" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I3" s="2">
         <v>0</v>
       </c>
       <c r="J3" s="2">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="K3" s="2">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="L3" s="14" t="s">
-        <v>91</v>
+        <v>364</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="O3" s="28" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>93</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="D4" s="2">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="E4" s="2">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F4" s="2">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G4" s="12">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="H4" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I4" s="2">
         <v>0</v>
       </c>
       <c r="J4" s="2">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="K4" s="2">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="M4" s="2"/>
+        <v>91</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="O4" s="28" t="s">
+        <v>336</v>
+      </c>
     </row>
     <row r="5" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>333</v>
+        <v>92</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>93</v>
       </c>
       <c r="C5" s="2">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="D5" s="2">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="E5" s="2">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F5" s="2">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G5" s="12">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="H5" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
         <v>2</v>
       </c>
       <c r="K5" s="2">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>255</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="M5" s="2"/>
     </row>
     <row r="6" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>19</v>
+        <v>333</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -2774,33 +3009,33 @@
         <v>4</v>
       </c>
       <c r="G6" s="12">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K6" s="2">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="L6" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>254</v>
+        <v>19</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>256</v>
+        <v>20</v>
       </c>
       <c r="C7" s="2">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="D7" s="2">
         <v>3</v>
@@ -2811,75 +3046,78 @@
       <c r="F7" s="2">
         <v>4</v>
       </c>
-      <c r="G7" s="13">
-        <v>16</v>
+      <c r="G7" s="12">
+        <v>12</v>
       </c>
       <c r="H7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7" s="2">
         <v>0</v>
       </c>
       <c r="K7" s="2">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L7" s="14" t="s">
         <v>96</v>
       </c>
+      <c r="M7" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G8" s="13"/>
-    </row>
-    <row r="9" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="2">
+      <c r="A8" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D8" s="2">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2">
+        <v>4</v>
+      </c>
+      <c r="F8" s="2">
+        <v>4</v>
+      </c>
+      <c r="G8" s="13">
+        <v>16</v>
+      </c>
+      <c r="H8" s="2">
         <v>1</v>
       </c>
-      <c r="D9" s="2">
-        <v>3</v>
-      </c>
-      <c r="E9" s="2">
-        <v>2</v>
-      </c>
-      <c r="F9" s="2">
-        <v>3</v>
-      </c>
-      <c r="G9" s="12">
-        <v>8</v>
-      </c>
-      <c r="H9" s="2">
+      <c r="I8" s="2">
         <v>0</v>
       </c>
-      <c r="I9" s="2">
-        <v>1</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K9" s="2">
-        <v>15</v>
-      </c>
-      <c r="L9" s="14" t="s">
-        <v>232</v>
-      </c>
+      <c r="K8" s="2">
+        <v>20</v>
+      </c>
+      <c r="L8" s="14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C10" s="2">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="D10" s="2">
-        <v>0.8</v>
+        <v>3</v>
       </c>
       <c r="E10" s="2">
         <v>2</v>
       </c>
       <c r="F10" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G10" s="12">
         <v>8</v>
@@ -2891,65 +3129,68 @@
         <v>1</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K10" s="2">
         <v>15</v>
       </c>
+      <c r="L10" s="14" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="11" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C11" s="2">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="D11" s="2">
-        <v>2.5</v>
+        <v>0.8</v>
       </c>
       <c r="E11" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G11" s="12">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H11" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" s="2">
         <v>1</v>
       </c>
+      <c r="J11" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="K11" s="2">
         <v>15</v>
       </c>
-      <c r="L11" s="18" t="s">
-        <v>233</v>
-      </c>
     </row>
     <row r="12" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="2">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="D12" s="2">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="E12" s="2">
+        <v>3</v>
+      </c>
+      <c r="F12" s="2">
         <v>4</v>
       </c>
-      <c r="F12" s="2">
-        <v>3</v>
-      </c>
       <c r="G12" s="12">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H12" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I12" s="2">
         <v>1</v>
@@ -2958,82 +3199,82 @@
         <v>15</v>
       </c>
       <c r="L12" s="18" t="s">
-        <v>152</v>
+        <v>233</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C13" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="D13" s="2">
+        <v>3</v>
+      </c>
+      <c r="E13" s="2">
+        <v>4</v>
+      </c>
+      <c r="F13" s="2">
+        <v>3</v>
+      </c>
+      <c r="G13" s="12">
+        <v>14</v>
+      </c>
+      <c r="H13" s="2">
+        <v>2</v>
+      </c>
+      <c r="I13" s="2">
         <v>1</v>
       </c>
-      <c r="D13" s="2">
-        <v>3</v>
-      </c>
-      <c r="E13" s="2">
-        <v>3</v>
-      </c>
-      <c r="F13" s="2">
-        <v>3</v>
-      </c>
-      <c r="G13" s="12">
-        <v>24</v>
-      </c>
-      <c r="H13" s="2">
-        <v>1</v>
-      </c>
-      <c r="I13" s="2">
-        <v>3</v>
-      </c>
       <c r="K13" s="2">
-        <v>30</v>
-      </c>
-      <c r="L13" s="14" t="s">
-        <v>277</v>
+        <v>15</v>
+      </c>
+      <c r="L13" s="18" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2">
+        <v>3</v>
+      </c>
+      <c r="E14" s="2">
+        <v>3</v>
+      </c>
+      <c r="F14" s="2">
+        <v>3</v>
+      </c>
+      <c r="G14" s="12">
+        <v>24</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1</v>
+      </c>
+      <c r="I14" s="2">
+        <v>3</v>
+      </c>
+      <c r="K14" s="2">
         <v>30</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="2">
-        <v>2</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K14" s="2">
-        <v>20</v>
+      <c r="L14" s="14" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C15" s="2">
         <v>2</v>
@@ -3061,16 +3302,36 @@
       </c>
     </row>
     <row r="16" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="K16" s="2"/>
+      <c r="A16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K16" s="2">
+        <v>20</v>
+      </c>
     </row>
     <row r="17" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
@@ -3084,53 +3345,27 @@
       <c r="I17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
       <c r="G18" s="13"/>
-    </row>
-    <row r="19" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="12">
-        <v>1</v>
-      </c>
-      <c r="D19" s="12">
-        <v>3</v>
-      </c>
-      <c r="E19" s="12">
-        <v>2</v>
-      </c>
-      <c r="F19" s="12">
-        <v>2</v>
-      </c>
-      <c r="G19" s="12">
-        <v>6</v>
-      </c>
-      <c r="H19" s="12">
-        <v>0</v>
-      </c>
-      <c r="I19" s="12">
-        <v>2</v>
-      </c>
-      <c r="J19" s="12">
-        <v>1</v>
-      </c>
-      <c r="K19" s="12">
-        <v>7</v>
-      </c>
-      <c r="L19" s="14" t="s">
-        <v>302</v>
-      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C20" s="12">
         <v>1</v>
@@ -3145,7 +3380,7 @@
         <v>2</v>
       </c>
       <c r="G20" s="12">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H20" s="12">
         <v>0</v>
@@ -3153,20 +3388,22 @@
       <c r="I20" s="12">
         <v>2</v>
       </c>
-      <c r="J20" s="13"/>
+      <c r="J20" s="12">
+        <v>1</v>
+      </c>
       <c r="K20" s="12">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="L20" s="14" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>97</v>
+        <v>37</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C21" s="12">
         <v>1</v>
@@ -3181,7 +3418,7 @@
         <v>2</v>
       </c>
       <c r="G21" s="12">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H21" s="12">
         <v>0</v>
@@ -3191,54 +3428,54 @@
       </c>
       <c r="J21" s="13"/>
       <c r="K21" s="12">
+        <v>10</v>
+      </c>
+      <c r="L21" s="14" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="12">
+        <v>1</v>
+      </c>
+      <c r="D22" s="12">
+        <v>3</v>
+      </c>
+      <c r="E22" s="12">
+        <v>2</v>
+      </c>
+      <c r="F22" s="12">
+        <v>2</v>
+      </c>
+      <c r="G22" s="12">
+        <v>6</v>
+      </c>
+      <c r="H22" s="12">
+        <v>0</v>
+      </c>
+      <c r="I22" s="12">
+        <v>2</v>
+      </c>
+      <c r="J22" s="13"/>
+      <c r="K22" s="12">
         <v>9</v>
       </c>
-      <c r="L21" s="14" t="s">
+      <c r="L22" s="14" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
+    <row r="23" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B23" s="15" t="s">
         <v>241</v>
-      </c>
-      <c r="C22" s="16">
-        <v>1</v>
-      </c>
-      <c r="D22" s="16">
-        <v>3</v>
-      </c>
-      <c r="E22" s="16">
-        <v>2</v>
-      </c>
-      <c r="F22" s="16">
-        <v>2</v>
-      </c>
-      <c r="G22" s="12">
-        <v>14</v>
-      </c>
-      <c r="H22" s="16">
-        <v>0</v>
-      </c>
-      <c r="I22" s="16">
-        <v>2</v>
-      </c>
-      <c r="J22" s="15"/>
-      <c r="K22" s="16">
-        <v>13</v>
-      </c>
-      <c r="L22" s="14" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
-        <v>247</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>244</v>
       </c>
       <c r="C23" s="16">
         <v>1</v>
@@ -3247,13 +3484,13 @@
         <v>3</v>
       </c>
       <c r="E23" s="16">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F23" s="16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G23" s="12">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="H23" s="16">
         <v>0</v>
@@ -3261,98 +3498,99 @@
       <c r="I23" s="16">
         <v>2</v>
       </c>
-      <c r="J23" s="15">
+      <c r="J23" s="15"/>
+      <c r="K23" s="16">
+        <v>13</v>
+      </c>
+      <c r="L23" s="14" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="C24" s="16">
+        <v>1</v>
+      </c>
+      <c r="D24" s="16">
+        <v>3</v>
+      </c>
+      <c r="E24" s="16">
+        <v>5</v>
+      </c>
+      <c r="F24" s="16">
+        <v>3</v>
+      </c>
+      <c r="G24" s="12">
+        <v>60</v>
+      </c>
+      <c r="H24" s="16">
+        <v>0</v>
+      </c>
+      <c r="I24" s="16">
         <v>2</v>
       </c>
-      <c r="K23" s="16">
+      <c r="J24" s="15">
+        <v>2</v>
+      </c>
+      <c r="K24" s="16">
         <v>40</v>
       </c>
-      <c r="L23" s="14" t="s">
+      <c r="L24" s="14" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G24" s="13"/>
-    </row>
-    <row r="25" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+    <row r="25" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G25" s="13"/>
+    </row>
+    <row r="26" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C26" s="2">
         <v>1</v>
       </c>
-      <c r="D25" s="2">
-        <v>3</v>
-      </c>
-      <c r="E25" s="2">
-        <v>3</v>
-      </c>
-      <c r="F25" s="2">
-        <v>3</v>
-      </c>
-      <c r="G25" s="12">
+      <c r="D26" s="2">
+        <v>3</v>
+      </c>
+      <c r="E26" s="2">
+        <v>3</v>
+      </c>
+      <c r="F26" s="2">
+        <v>3</v>
+      </c>
+      <c r="G26" s="12">
         <v>7</v>
       </c>
-      <c r="H25" s="2">
+      <c r="H26" s="2">
         <v>1</v>
       </c>
-      <c r="I25" s="2">
+      <c r="I26" s="2">
         <v>2</v>
       </c>
-      <c r="K25" s="2">
+      <c r="K26" s="2">
         <v>10</v>
       </c>
-      <c r="M25" s="2" t="s">
+      <c r="L26" s="18" t="s">
+        <v>376</v>
+      </c>
+      <c r="M26" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G26" s="13"/>
-    </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="G27" s="13"/>
+    </row>
+    <row r="28" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>329</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="C27" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="D27" s="2">
-        <v>2</v>
-      </c>
-      <c r="E27" s="2">
-        <v>2</v>
-      </c>
-      <c r="F27" s="2">
-        <v>5</v>
-      </c>
-      <c r="G27" s="12">
-        <v>16</v>
-      </c>
-      <c r="H27" s="2">
-        <v>1</v>
-      </c>
-      <c r="I27" s="2">
-        <v>1</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="K27" s="2">
-        <v>20</v>
-      </c>
-      <c r="L27" s="14" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>330</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>318</v>
@@ -3361,13 +3599,13 @@
         <v>1.5</v>
       </c>
       <c r="D28" s="2">
-        <v>2.4</v>
+        <v>2</v>
       </c>
       <c r="E28" s="2">
         <v>2</v>
       </c>
       <c r="F28" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G28" s="12">
         <v>16</v>
@@ -3390,7 +3628,7 @@
     </row>
     <row r="29" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>318</v>
@@ -3405,13 +3643,13 @@
         <v>2</v>
       </c>
       <c r="F29" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G29" s="12">
         <v>16</v>
       </c>
       <c r="H29" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I29" s="2">
         <v>1</v>
@@ -3428,48 +3666,51 @@
     </row>
     <row r="30" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C30" s="2">
         <v>1.5</v>
       </c>
       <c r="D30" s="2">
-        <v>3</v>
+        <v>2.4</v>
       </c>
       <c r="E30" s="2">
         <v>2</v>
       </c>
       <c r="F30" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G30" s="12">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="H30" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I30" s="2">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="K30" s="2">
         <v>20</v>
       </c>
       <c r="L30" s="14" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>44</v>
+        <v>332</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>258</v>
+        <v>317</v>
       </c>
       <c r="C31" s="2">
-        <v>0.8</v>
+        <v>1.5</v>
       </c>
       <c r="D31" s="2">
         <v>3</v>
@@ -3478,31 +3719,33 @@
         <v>2</v>
       </c>
       <c r="F31" s="2">
+        <v>4</v>
+      </c>
+      <c r="G31" s="12">
+        <v>20</v>
+      </c>
+      <c r="H31" s="2">
+        <v>3</v>
+      </c>
+      <c r="I31" s="2">
         <v>2</v>
       </c>
-      <c r="G31" s="12">
-        <v>4</v>
-      </c>
-      <c r="H31" s="2">
-        <v>1</v>
-      </c>
-      <c r="I31" s="2">
-        <v>0</v>
-      </c>
       <c r="K31" s="2">
-        <v>5</v>
-      </c>
-      <c r="L31" s="14"/>
+        <v>20</v>
+      </c>
+      <c r="L31" s="14" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="32" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>328</v>
+        <v>44</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C32" s="2">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="D32" s="2">
         <v>3</v>
@@ -3511,30 +3754,28 @@
         <v>2</v>
       </c>
       <c r="F32" s="2">
+        <v>2</v>
+      </c>
+      <c r="G32" s="12">
         <v>4</v>
-      </c>
-      <c r="G32" s="12">
-        <v>8</v>
       </c>
       <c r="H32" s="2">
         <v>1</v>
       </c>
       <c r="I32" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K32" s="2">
-        <v>10</v>
-      </c>
-      <c r="L32" s="14" t="s">
-        <v>259</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="L32" s="14"/>
     </row>
     <row r="33" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>261</v>
+        <v>328</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C33" s="2">
         <v>1.5</v>
@@ -3549,64 +3790,67 @@
         <v>4</v>
       </c>
       <c r="G33" s="12">
+        <v>8</v>
+      </c>
+      <c r="H33" s="2">
+        <v>1</v>
+      </c>
+      <c r="I33" s="2">
+        <v>1</v>
+      </c>
+      <c r="K33" s="2">
+        <v>10</v>
+      </c>
+      <c r="L33" s="14" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C34" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="D34" s="2">
+        <v>3</v>
+      </c>
+      <c r="E34" s="2">
+        <v>2</v>
+      </c>
+      <c r="F34" s="2">
+        <v>4</v>
+      </c>
+      <c r="G34" s="12">
         <v>12</v>
       </c>
-      <c r="H33" s="2">
+      <c r="H34" s="2">
         <v>2</v>
       </c>
-      <c r="I33" s="2">
+      <c r="I34" s="2">
         <v>4</v>
       </c>
-      <c r="K33" s="2">
+      <c r="K34" s="2">
         <v>20</v>
       </c>
-      <c r="L33" s="14" t="s">
+      <c r="L34" s="14" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G34" s="13" t="s">
+    <row r="35" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G35" s="13" t="s">
         <v>264</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C35" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="D35" s="2">
-        <v>3</v>
-      </c>
-      <c r="E35" s="2">
-        <v>3</v>
-      </c>
-      <c r="F35" s="2">
-        <v>3</v>
-      </c>
-      <c r="G35" s="12">
-        <v>12</v>
-      </c>
-      <c r="H35" s="2">
-        <v>0</v>
-      </c>
-      <c r="I35" s="2">
-        <v>2</v>
-      </c>
-      <c r="K35" s="2">
-        <v>15</v>
-      </c>
-      <c r="L35" s="14" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="C36" s="2">
         <v>1.5</v>
@@ -3621,7 +3865,7 @@
         <v>3</v>
       </c>
       <c r="G36" s="12">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H36" s="2">
         <v>0</v>
@@ -3630,15 +3874,15 @@
         <v>2</v>
       </c>
       <c r="K36" s="2">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L36" s="14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C37" s="2">
         <v>1.5</v>
@@ -3665,12 +3909,12 @@
         <v>20</v>
       </c>
       <c r="L37" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C38" s="2">
         <v>1.5</v>
@@ -3697,12 +3941,12 @@
         <v>20</v>
       </c>
       <c r="L38" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C39" s="2">
         <v>1.5</v>
@@ -3729,12 +3973,12 @@
         <v>20</v>
       </c>
       <c r="L39" s="14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C40" s="2">
         <v>1.5</v>
@@ -3761,12 +4005,12 @@
         <v>20</v>
       </c>
       <c r="L40" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C41" s="2">
         <v>1.5</v>
@@ -3793,12 +4037,12 @@
         <v>20</v>
       </c>
       <c r="L41" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C42" s="2">
         <v>1.5</v>
@@ -3825,15 +4069,15 @@
         <v>20</v>
       </c>
       <c r="L42" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C43" s="2">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D43" s="2">
         <v>3</v>
@@ -3857,194 +4101,190 @@
         <v>20</v>
       </c>
       <c r="L43" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" s="2">
+        <v>1</v>
+      </c>
+      <c r="D44" s="2">
+        <v>3</v>
+      </c>
+      <c r="E44" s="2">
+        <v>3</v>
+      </c>
+      <c r="F44" s="2">
+        <v>3</v>
+      </c>
+      <c r="G44" s="12">
+        <v>15</v>
+      </c>
+      <c r="H44" s="2">
+        <v>0</v>
+      </c>
+      <c r="I44" s="2">
+        <v>2</v>
+      </c>
+      <c r="K44" s="2">
+        <v>20</v>
+      </c>
+      <c r="L44" s="14" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G44" s="13"/>
-    </row>
-    <row r="45" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C45" s="2">
-        <v>3</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E45" s="2">
-        <v>1</v>
-      </c>
-      <c r="F45" s="2">
-        <v>0</v>
-      </c>
-      <c r="G45" s="12">
-        <v>1</v>
-      </c>
-      <c r="H45" s="2">
-        <v>0</v>
-      </c>
-      <c r="I45" s="2">
-        <v>0</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K45" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L45" s="14" t="s">
-        <v>298</v>
-      </c>
+    <row r="45" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G45" s="13"/>
     </row>
     <row r="46" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C46" s="2">
+        <v>3</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E46" s="2">
         <v>1</v>
       </c>
-      <c r="D46" s="2">
-        <v>3</v>
-      </c>
-      <c r="E46" s="2">
-        <v>3</v>
-      </c>
       <c r="F46" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G46" s="12">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H46" s="2">
         <v>0</v>
       </c>
       <c r="I46" s="2">
-        <v>1</v>
-      </c>
-      <c r="K46" s="2">
-        <v>10</v>
+        <v>0</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="L46" s="14" t="s">
-        <v>68</v>
+        <v>298</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C47" s="2">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="D47" s="2">
-        <v>2.9</v>
+        <v>3</v>
       </c>
       <c r="E47" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F47" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G47" s="12">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="H47" s="2">
         <v>0</v>
       </c>
       <c r="I47" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K47" s="2">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="L47" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C48" s="2">
         <v>0.9</v>
       </c>
       <c r="D48" s="2">
+        <v>2.9</v>
+      </c>
+      <c r="E48" s="2">
+        <v>4</v>
+      </c>
+      <c r="F48" s="2">
+        <v>4</v>
+      </c>
+      <c r="G48" s="12">
+        <v>16</v>
+      </c>
+      <c r="H48" s="2">
+        <v>0</v>
+      </c>
+      <c r="I48" s="2">
+        <v>2</v>
+      </c>
+      <c r="K48" s="2">
+        <v>20</v>
+      </c>
+      <c r="L48" s="14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C49" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="D49" s="2">
         <v>2.8</v>
       </c>
-      <c r="E48" s="2">
+      <c r="E49" s="2">
         <v>5</v>
       </c>
-      <c r="F48" s="2">
+      <c r="F49" s="2">
         <v>5</v>
       </c>
-      <c r="G48" s="12">
+      <c r="G49" s="12">
         <v>28</v>
       </c>
-      <c r="H48" s="2">
+      <c r="H49" s="2">
         <v>1</v>
       </c>
-      <c r="I48" s="2">
-        <v>3</v>
-      </c>
-      <c r="K48" s="2">
+      <c r="I49" s="2">
+        <v>3</v>
+      </c>
+      <c r="K49" s="2">
         <v>35</v>
       </c>
-      <c r="L48" s="14" t="s">
+      <c r="L49" s="14" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C49" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="D49" s="4">
-        <v>2.7</v>
-      </c>
-      <c r="E49" s="4">
-        <v>6</v>
-      </c>
-      <c r="F49" s="4">
-        <v>6</v>
-      </c>
-      <c r="G49" s="12">
-        <v>44</v>
-      </c>
-      <c r="H49" s="4">
-        <v>1</v>
-      </c>
-      <c r="I49" s="4">
-        <v>4</v>
-      </c>
-      <c r="J49" s="3"/>
-      <c r="K49" s="4">
-        <v>55</v>
-      </c>
-      <c r="L49" s="17" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>77</v>
+        <v>239</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>75</v>
@@ -4053,123 +4293,123 @@
         <v>0.8</v>
       </c>
       <c r="D50" s="4">
-        <v>2.6</v>
+        <v>2.7</v>
       </c>
       <c r="E50" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F50" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G50" s="12">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="H50" s="4">
         <v>1</v>
       </c>
       <c r="I50" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J50" s="3"/>
       <c r="K50" s="4">
+        <v>55</v>
+      </c>
+      <c r="L50" s="17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C51" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="D51" s="4">
+        <v>2.6</v>
+      </c>
+      <c r="E51" s="4">
+        <v>7</v>
+      </c>
+      <c r="F51" s="4">
+        <v>7</v>
+      </c>
+      <c r="G51" s="12">
+        <v>64</v>
+      </c>
+      <c r="H51" s="4">
+        <v>1</v>
+      </c>
+      <c r="I51" s="4">
+        <v>5</v>
+      </c>
+      <c r="J51" s="3"/>
+      <c r="K51" s="4">
         <v>80</v>
       </c>
-      <c r="L50" s="17" t="s">
+      <c r="L51" s="17" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+    <row r="52" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B52" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C52" s="2">
         <v>1</v>
       </c>
-      <c r="D51" s="2">
-        <v>3</v>
-      </c>
-      <c r="E51" s="2">
+      <c r="D52" s="2">
+        <v>3</v>
+      </c>
+      <c r="E52" s="2">
         <v>4</v>
       </c>
-      <c r="F51" s="2">
+      <c r="F52" s="2">
         <v>4</v>
       </c>
-      <c r="G51" s="12">
+      <c r="G52" s="12">
         <v>20</v>
       </c>
-      <c r="H51" s="2">
+      <c r="H52" s="2">
         <v>0</v>
       </c>
-      <c r="I51" s="2">
+      <c r="I52" s="2">
         <v>4</v>
       </c>
-      <c r="K51" s="2">
+      <c r="K52" s="2">
         <v>20</v>
       </c>
-      <c r="L51" s="14" t="s">
+      <c r="L52" s="14" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G52" s="13"/>
-    </row>
-    <row r="53" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+    <row r="53" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G53" s="13"/>
+    </row>
+    <row r="54" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="C53" s="2">
-        <v>2</v>
-      </c>
-      <c r="D53" s="2">
-        <v>3</v>
-      </c>
-      <c r="E53" s="2">
-        <v>2</v>
-      </c>
-      <c r="F53" s="2">
-        <v>3</v>
-      </c>
-      <c r="G53" s="12">
-        <v>8</v>
-      </c>
-      <c r="H53" s="2">
-        <v>0</v>
-      </c>
-      <c r="I53" s="2">
-        <v>0</v>
-      </c>
-      <c r="J53" s="2"/>
-      <c r="K53" s="2">
-        <v>10</v>
-      </c>
-      <c r="L53" s="14" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>275</v>
       </c>
       <c r="C54" s="2">
         <v>2</v>
       </c>
       <c r="D54" s="2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E54" s="2">
         <v>2</v>
       </c>
       <c r="F54" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G54" s="12">
         <v>8</v>
@@ -4180,145 +4420,143 @@
       <c r="I54" s="2">
         <v>0</v>
       </c>
-      <c r="J54" s="2" t="s">
-        <v>274</v>
-      </c>
+      <c r="J54" s="2"/>
       <c r="K54" s="2">
         <v>10</v>
       </c>
       <c r="L54" s="14" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>32</v>
+        <v>275</v>
+      </c>
+      <c r="C55" s="2">
+        <v>2</v>
+      </c>
+      <c r="D55" s="2">
+        <v>8</v>
       </c>
       <c r="E55" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F55" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G55" s="12">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H55" s="2">
         <v>0</v>
       </c>
       <c r="I55" s="2">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>274</v>
       </c>
       <c r="K55" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="L55" s="14" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E56" s="2">
+        <v>1</v>
+      </c>
+      <c r="F56" s="2">
+        <v>0</v>
+      </c>
+      <c r="G56" s="12">
+        <v>1</v>
+      </c>
+      <c r="H56" s="2">
+        <v>0</v>
+      </c>
+      <c r="I56" s="2">
+        <v>1</v>
+      </c>
+      <c r="K56" s="2">
+        <v>5</v>
+      </c>
+      <c r="L56" s="14" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C57" s="2">
         <v>1.5</v>
       </c>
-      <c r="D56" s="2">
-        <v>3</v>
-      </c>
-      <c r="E56" s="2">
+      <c r="D57" s="2">
+        <v>3</v>
+      </c>
+      <c r="E57" s="2">
         <v>7</v>
       </c>
-      <c r="F56" s="2">
+      <c r="F57" s="2">
         <v>7</v>
       </c>
-      <c r="G56" s="12">
+      <c r="G57" s="12">
         <v>40</v>
       </c>
-      <c r="H56" s="2">
+      <c r="H57" s="2">
         <v>2</v>
       </c>
-      <c r="I56" s="2">
-        <v>3</v>
-      </c>
-      <c r="J56" s="2" t="s">
+      <c r="I57" s="2">
+        <v>3</v>
+      </c>
+      <c r="J57" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="K56" s="2">
+      <c r="K57" s="2">
         <v>50</v>
       </c>
-      <c r="L56" s="14" t="s">
+      <c r="L57" s="14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
+    <row r="58" spans="1:12" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B58" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="C57" s="2">
-        <v>2</v>
-      </c>
-      <c r="D57" s="2">
-        <v>6</v>
-      </c>
-      <c r="E57" s="2">
-        <v>2</v>
-      </c>
-      <c r="F57" s="2">
-        <v>0</v>
-      </c>
-      <c r="G57" s="12">
-        <v>8</v>
-      </c>
-      <c r="H57" s="2">
-        <v>0</v>
-      </c>
-      <c r="I57" s="2">
-        <v>0</v>
-      </c>
-      <c r="J57" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="K57" s="2">
-        <v>10</v>
-      </c>
-      <c r="L57" s="14" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="C58" s="2">
         <v>2</v>
       </c>
       <c r="D58" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E58" s="2">
         <v>2</v>
       </c>
       <c r="F58" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G58" s="12">
         <v>8</v>
@@ -4330,33 +4568,33 @@
         <v>0</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="K58" s="2">
         <v>10</v>
       </c>
       <c r="L58" s="14" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="C59" s="2">
         <v>2</v>
       </c>
-      <c r="D59" s="2" t="s">
-        <v>103</v>
+      <c r="D59" s="2">
+        <v>8</v>
       </c>
       <c r="E59" s="2">
         <v>2</v>
       </c>
-      <c r="F59" s="2" t="s">
-        <v>363</v>
+      <c r="F59" s="2">
+        <v>4</v>
       </c>
       <c r="G59" s="12">
         <v>8</v>
@@ -4368,32 +4606,180 @@
         <v>0</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>104</v>
+        <v>271</v>
       </c>
       <c r="K59" s="2">
         <v>10</v>
       </c>
       <c r="L59" s="14" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" ht="12.75" x14ac:dyDescent="0.2"/>
+        <v>270</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C60" s="2">
+        <v>2</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E60" s="2">
+        <v>2</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="G60" s="12">
+        <v>8</v>
+      </c>
+      <c r="H60" s="2">
+        <v>0</v>
+      </c>
+      <c r="I60" s="2">
+        <v>0</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K60" s="2">
+        <v>10</v>
+      </c>
+      <c r="L60" s="14" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="12.75" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O2" r:id="rId1" display="..\Stag knight.jpg" xr:uid="{051090D8-9F0F-4C9A-A707-1EB36D88B061}"/>
-    <hyperlink ref="O3" r:id="rId2" display="..\hercules.jpg" xr:uid="{B10553E2-CAEF-42FE-8070-D95757733EDB}"/>
+    <hyperlink ref="O3" r:id="rId1" display="..\Stag knight.jpg" xr:uid="{051090D8-9F0F-4C9A-A707-1EB36D88B061}"/>
+    <hyperlink ref="O4" r:id="rId2" display="..\hercules.jpg" xr:uid="{B10553E2-CAEF-42FE-8070-D95757733EDB}"/>
+    <hyperlink ref="O2" r:id="rId3" display="..\Stag knight.jpg" xr:uid="{E8FD10AB-00D1-444C-9DC5-62094B5166F7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD5C00C2-713F-455F-AB32-F63C45BE2971}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12640ACA-EB68-4BDC-8A72-44760D4BEB7C}">
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" t="s">
+        <v>312</v>
+      </c>
+      <c r="E1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" t="s">
+        <v>313</v>
+      </c>
+      <c r="G1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="21"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" s="21"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="25"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" s="24"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="21"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>313</v>
+      </c>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="25"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="22"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD5C00C2-713F-455F-AB32-F63C45BE2971}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4420,12 +4806,20 @@
         <v>113</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>380</v>
+      </c>
+      <c r="B3" t="s">
+        <v>381</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD829293-CBE6-47ED-83AB-F98F4FF7F124}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -4715,12 +5109,12 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.28515625" customWidth="1"/>
     <col min="6" max="6" width="5.85546875" customWidth="1"/>
     <col min="7" max="7" width="31.42578125" customWidth="1"/>
   </cols>
@@ -4753,13 +5147,13 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
@@ -4767,14 +5161,14 @@
       <c r="E2" s="2">
         <v>0</v>
       </c>
-      <c r="F2" s="2">
-        <v>1</v>
+      <c r="F2" s="6" t="s">
+        <v>379</v>
       </c>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -4782,13 +5176,13 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -4807,15 +5201,15 @@
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="2">
-        <v>1</v>
+      <c r="E5" s="6" t="s">
+        <v>379</v>
       </c>
       <c r="F5" s="2"/>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -4826,20 +5220,36 @@
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
+      <c r="A7" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="6"/>
+      <c r="F7">
+        <v>8</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
+      <c r="A8" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="B8" s="2">
+        <v>4</v>
+      </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="D8" s="2">
+        <v>2</v>
+      </c>
       <c r="E8" s="6"/>
+      <c r="F8">
+        <v>12</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
@@ -4875,14 +5285,232 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAD14A1E-99DD-48DF-BC26-F61D5FC7F987}">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="86.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="71.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>406</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>383</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="D2" t="s">
+        <v>407</v>
+      </c>
+      <c r="E2" t="s">
+        <v>410</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>382</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>401</v>
+      </c>
+      <c r="C3" s="27"/>
+      <c r="E3" t="s">
+        <v>427</v>
+      </c>
+      <c r="F3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>400</v>
+      </c>
+      <c r="B4" t="s">
+        <v>405</v>
+      </c>
+      <c r="C4" s="27"/>
+      <c r="F4" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>396</v>
+      </c>
+      <c r="B5" t="s">
+        <v>397</v>
+      </c>
+      <c r="C5" s="30"/>
+      <c r="D5" t="s">
+        <v>408</v>
+      </c>
+      <c r="F5" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>384</v>
+      </c>
+      <c r="B6" t="s">
+        <v>385</v>
+      </c>
+      <c r="C6" s="30"/>
+      <c r="F6" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>386</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>387</v>
+      </c>
+      <c r="C7" s="30"/>
+      <c r="F7" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>395</v>
+      </c>
+      <c r="B8" t="s">
+        <v>394</v>
+      </c>
+      <c r="C8" s="31"/>
+      <c r="D8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E8" t="s">
+        <v>422</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>388</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>389</v>
+      </c>
+      <c r="C9" s="31"/>
+      <c r="E9" t="s">
+        <v>421</v>
+      </c>
+      <c r="F9" s="29" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>390</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>391</v>
+      </c>
+      <c r="C10" s="31"/>
+      <c r="E10" t="s">
+        <v>428</v>
+      </c>
+      <c r="F10" s="29" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>392</v>
+      </c>
+      <c r="B11" t="s">
+        <v>393</v>
+      </c>
+      <c r="C11" s="32"/>
+      <c r="D11" t="s">
+        <v>409</v>
+      </c>
+      <c r="E11" t="s">
+        <v>429</v>
+      </c>
+      <c r="F11" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>398</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>399</v>
+      </c>
+      <c r="C12" s="32"/>
+      <c r="E12" t="s">
+        <v>417</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>402</v>
+      </c>
+      <c r="B13" t="s">
+        <v>403</v>
+      </c>
+      <c r="C13" s="32"/>
+      <c r="E13" t="s">
+        <v>418</v>
+      </c>
+      <c r="F13" t="s">
+        <v>419</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA26"/>
+  <dimension ref="A1:AA31"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4903,7 +5531,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>116</v>
       </c>
@@ -4911,7 +5539,7 @@
         <v>128</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>334</v>
+        <v>369</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
@@ -4971,7 +5599,7 @@
     </row>
     <row r="8" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>116</v>
+        <v>368</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>246</v>
@@ -5101,15 +5729,15 @@
         <v>309</v>
       </c>
     </row>
-    <row r="20" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:27" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>140</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>153</v>
+        <v>366</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>154</v>
+        <v>367</v>
       </c>
     </row>
     <row r="21" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
@@ -5117,56 +5745,32 @@
         <v>140</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C22" s="14" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="22" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
-      <c r="S22" s="3"/>
-      <c r="T22" s="3"/>
-      <c r="U22" s="3"/>
-      <c r="V22" s="3"/>
-      <c r="W22" s="3"/>
-      <c r="X22" s="3"/>
-      <c r="Y22" s="3"/>
-      <c r="Z22" s="3"/>
-      <c r="AA22" s="3"/>
-    </row>
-    <row r="23" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>140</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>360</v>
+        <v>155</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>361</v>
+        <v>156</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="3"/>
@@ -5193,37 +5797,140 @@
       <c r="Z23" s="3"/>
       <c r="AA23" s="3"/>
     </row>
-    <row r="24" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+    <row r="24" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>360</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
+      <c r="T24" s="3"/>
+      <c r="U24" s="3"/>
+      <c r="V24" s="3"/>
+      <c r="W24" s="3"/>
+      <c r="X24" s="3"/>
+      <c r="Y24" s="3"/>
+      <c r="Z24" s="3"/>
+      <c r="AA24" s="3"/>
+    </row>
+    <row r="25" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>412</v>
+      </c>
+      <c r="D25" s="7"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
+      <c r="T25" s="3"/>
+      <c r="U25" s="3"/>
+      <c r="V25" s="3"/>
+      <c r="W25" s="3"/>
+      <c r="X25" s="3"/>
+      <c r="Y25" s="3"/>
+      <c r="Z25" s="3"/>
+      <c r="AA25" s="3"/>
+    </row>
+    <row r="26" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C26" s="14" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="25" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+    <row r="27" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C27" s="14" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="26" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+    <row r="28" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C28" s="14" t="s">
         <v>160</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>375</v>
       </c>
     </row>
   </sheetData>
@@ -5231,7 +5938,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -5544,10 +6251,10 @@
     </row>
     <row r="31" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>338</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>339</v>
       </c>
       <c r="C31" s="2">
         <v>6</v>
@@ -5556,51 +6263,51 @@
         <v>6</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
   </sheetData>
@@ -5608,7 +6315,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -5908,7 +6615,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -5959,7 +6666,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{486828E7-6691-466E-812C-C9B1F7969124}">
   <dimension ref="A1:J1"/>
   <sheetViews>
@@ -6009,113 +6716,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12640ACA-EB68-4BDC-8A72-44760D4BEB7C}">
-  <dimension ref="A1:G7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>314</v>
-      </c>
-      <c r="B1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D1" t="s">
-        <v>312</v>
-      </c>
-      <c r="E1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F1" t="s">
-        <v>313</v>
-      </c>
-      <c r="G1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="21"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>312</v>
-      </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="25"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="21"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>313</v>
-      </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="25"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>117</v>
-      </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="22"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated stats and rules. Included MTG set doc
</commit_message>
<xml_diff>
--- a/unit stats.xlsx
+++ b/unit stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Nicholas\Documents\wargame\wargame-tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07DC9422-0F47-48D4-B0C6-2C2327332F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150BDB11-BB0A-4302-97BA-C313F85BE390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="units new statlines" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="452">
   <si>
     <t>Name</t>
   </si>
@@ -327,9 +327,6 @@
     <t>Colossal armored melee unit</t>
   </si>
   <si>
-    <t>Relentless 2, Dauntless 2, Mindless</t>
-  </si>
-  <si>
     <t>Spellcaster: Hivecourts, Flying</t>
   </si>
   <si>
@@ -1149,9 +1146,6 @@
     <t>An enemy unit within 1 inch of this unit cannot move unless it takes 2 penalty levels to Movement for the entire Move action.</t>
   </si>
   <si>
-    <t>ss</t>
-  </si>
-  <si>
     <t>Releases a cloud of basic spores that fills an area of radius X (2 if not provided) for 2 turns. Each enemy unit that ends its turn within the cloud either becomes infected with the specific Spore type, or adds a counter to an existing Spore infection.  If no enemy units are infected with this cloud after the 2 turns, then return the unit to the battlefield at full Wounds.  A unit with Spore Cloud may also spend 6 Activation Points to create a cloud until the end of the round centered on their location.  This cloud may be any type of spore the unit may normally make.  Upon dispersal, this cloud does not create a Grunt</t>
   </si>
   <si>
@@ -1336,6 +1330,75 @@
   </si>
   <si>
     <t>When getting the cost for this unit's Movement, it counts as moving one more inch</t>
+  </si>
+  <si>
+    <t>Spirit Host</t>
+  </si>
+  <si>
+    <t>Mindless</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cheap unit that </t>
+  </si>
+  <si>
+    <t>Relentless 2, Dauntless 2, Mindless - Enraged</t>
+  </si>
+  <si>
+    <t>Mindless - Obedient</t>
+  </si>
+  <si>
+    <t>Mindless (can upgrade to Mindless - Obedient for 3 points)</t>
+  </si>
+  <si>
+    <t>Possession, Awakening</t>
+  </si>
+  <si>
+    <t>Spectres</t>
+  </si>
+  <si>
+    <t>Possession</t>
+  </si>
+  <si>
+    <t>Awakening</t>
+  </si>
+  <si>
+    <t>This unit cannot take any Actions.  Nor can it be activated.</t>
+  </si>
+  <si>
+    <t>Mindless - Enraged</t>
+  </si>
+  <si>
+    <t>This unit cannot take any Actions.  Nor can it be activated.  Once all other units are retired, before ending the round, this unit moves towards the closest unit it can find (friend or foe) and attempts to get in base-to-base contact with it.  If it can, it then uses all its remaining points to Attack.  This does not count as an activation</t>
+  </si>
+  <si>
+    <t>This unnit cannot take any Actions. Nor can it be activated.  It can be given an order by a friendly unit without Mindless within 3".  Once all other units are retired, before ending the round, this unit attempts to carry out the specific order and will not stop or deviate until it is done.  Orders must be simple and specific (Go to X position, Kill Y unit).  If it completes its order, it will remain inactive until receiving another one.  The unit may only have a single order at a time.</t>
+  </si>
+  <si>
+    <t>Spectre</t>
+  </si>
+  <si>
+    <t>Activates local Spirit Host</t>
+  </si>
+  <si>
+    <t>Select an unpossessed friendly Spirit Host unit within 3".  Remove the casting model from the table and treat the selected model as though it were this model for the purposes of location and targeting.  The possessed model gains magical attacks and always deals full damage.  It also  gains Relentless 1 and Dauntless 1.  You may cancel this ability as an Ability action.  If so, or if the possessed model dies, place the casting model back on the table within 1" of it.  Each use beyond the first in a Round costs 3 points.</t>
+  </si>
+  <si>
+    <t>Spirit Hosts within 3" of this unit lose Mindless</t>
+  </si>
+  <si>
+    <t>Solitary liches with unthinking slaves</t>
+  </si>
+  <si>
+    <t>Can be small or large numerically.  Each Priest continually grows fields of biomass</t>
+  </si>
+  <si>
+    <t>Varies.  Priority on restoring humanity</t>
+  </si>
+  <si>
+    <t>None for the priests.  They grow and breed new human flesh, but only the priests are sentient</t>
+  </si>
+  <si>
+    <t>Restoring humanity is common, but it varies</t>
   </si>
 </sst>
 </file>
@@ -1511,7 +1574,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1567,6 +1630,7 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1626,9 +1690,9 @@
           <c:invertIfNegative val="1"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Faction breakdown'!$A$2:$A$9</c:f>
+              <c:f>'Faction breakdown'!$A$2:$A$10</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>FCP</c:v>
                 </c:pt>
@@ -1652,16 +1716,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Wanderer</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Spectres</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Faction breakdown'!$B$2:$B$9</c:f>
+              <c:f>'Faction breakdown'!$B$2:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -1682,6 +1749,12 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1733,9 +1806,9 @@
           <c:invertIfNegative val="1"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Faction breakdown'!$A$2:$A$9</c:f>
+              <c:f>'Faction breakdown'!$A$2:$A$10</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>FCP</c:v>
                 </c:pt>
@@ -1759,16 +1832,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Wanderer</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Spectres</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Faction breakdown'!$C$2:$C$9</c:f>
+              <c:f>'Faction breakdown'!$C$2:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -1789,6 +1865,12 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1840,9 +1922,9 @@
           <c:invertIfNegative val="1"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Faction breakdown'!$A$2:$A$9</c:f>
+              <c:f>'Faction breakdown'!$A$2:$A$10</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>FCP</c:v>
                 </c:pt>
@@ -1866,16 +1948,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Wanderer</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Spectres</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Faction breakdown'!$D$2:$D$9</c:f>
+              <c:f>'Faction breakdown'!$D$2:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>4</c:v>
                 </c:pt>
@@ -1895,6 +1980,12 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
@@ -1947,9 +2038,9 @@
           <c:invertIfNegative val="1"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Faction breakdown'!$A$2:$A$9</c:f>
+              <c:f>'Faction breakdown'!$A$2:$A$10</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>FCP</c:v>
                 </c:pt>
@@ -1973,16 +2064,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Wanderer</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Spectres</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Faction breakdown'!$E$2:$E$9</c:f>
+              <c:f>'Faction breakdown'!$E$2:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>4</c:v>
                 </c:pt>
@@ -2003,6 +2097,12 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2054,9 +2154,9 @@
           <c:invertIfNegative val="1"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Faction breakdown'!$A$2:$A$9</c:f>
+              <c:f>'Faction breakdown'!$A$2:$A$10</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>FCP</c:v>
                 </c:pt>
@@ -2080,16 +2180,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Wanderer</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Spectres</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Faction breakdown'!$F$2:$F$9</c:f>
+              <c:f>'Faction breakdown'!$F$2:$F$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -2110,6 +2213,12 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2161,9 +2270,9 @@
           <c:invertIfNegative val="1"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Faction breakdown'!$A$2:$A$9</c:f>
+              <c:f>'Faction breakdown'!$A$2:$A$10</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>FCP</c:v>
                 </c:pt>
@@ -2187,16 +2296,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Wanderer</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Spectres</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Faction breakdown'!$G$2:$G$9</c:f>
+              <c:f>'Faction breakdown'!$G$2:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -2217,6 +2329,12 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2268,9 +2386,9 @@
           <c:invertIfNegative val="1"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Faction breakdown'!$A$2:$A$9</c:f>
+              <c:f>'Faction breakdown'!$A$2:$A$10</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>FCP</c:v>
                 </c:pt>
@@ -2294,16 +2412,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>Wanderer</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Spectres</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Faction breakdown'!$H$2:$H$9</c:f>
+              <c:f>'Faction breakdown'!$H$2:$H$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>4.333333333333333</c:v>
                 </c:pt>
@@ -2324,6 +2445,12 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2524,8 +2651,8 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>87967</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="17821275" cy="3533775"/>
     <xdr:graphicFrame macro="">
@@ -2755,11 +2882,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:O61"/>
+  <dimension ref="A1:O63"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L27" sqref="L27"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2812,10 +2939,10 @@
         <v>13</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -2853,18 +2980,18 @@
         <v>20</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="O2" s="28" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>17</v>
@@ -2897,13 +3024,13 @@
         <v>30</v>
       </c>
       <c r="L3" s="14" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="O3" s="28" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -2944,10 +3071,10 @@
         <v>91</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="O4" s="28" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -2985,13 +3112,13 @@
         <v>70</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>94</v>
+        <v>432</v>
       </c>
       <c r="M5" s="2"/>
     </row>
     <row r="6" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>18</v>
@@ -3021,10 +3148,10 @@
         <v>20</v>
       </c>
       <c r="L6" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3059,7 +3186,7 @@
         <v>15</v>
       </c>
       <c r="L7" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>21</v>
@@ -3067,10 +3194,10 @@
     </row>
     <row r="8" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C8" s="2">
         <v>0.75</v>
@@ -3097,7 +3224,7 @@
         <v>20</v>
       </c>
       <c r="L8" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3135,7 +3262,7 @@
         <v>15</v>
       </c>
       <c r="L10" s="14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3199,7 +3326,7 @@
         <v>15</v>
       </c>
       <c r="L12" s="18" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3231,7 +3358,7 @@
         <v>15</v>
       </c>
       <c r="L13" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3266,7 +3393,7 @@
         <v>30</v>
       </c>
       <c r="L14" s="14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3395,7 +3522,7 @@
         <v>7</v>
       </c>
       <c r="L20" s="14" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3431,12 +3558,12 @@
         <v>10</v>
       </c>
       <c r="L21" s="14" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B22" s="13" t="s">
         <v>39</v>
@@ -3467,15 +3594,15 @@
         <v>9</v>
       </c>
       <c r="L22" s="14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="B23" s="15" t="s">
         <v>240</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>241</v>
       </c>
       <c r="C23" s="16">
         <v>1</v>
@@ -3503,15 +3630,15 @@
         <v>13</v>
       </c>
       <c r="L23" s="14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C24" s="16">
         <v>1</v>
@@ -3541,7 +3668,7 @@
         <v>40</v>
       </c>
       <c r="L24" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3579,7 +3706,7 @@
         <v>10</v>
       </c>
       <c r="L26" s="18" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="M26" s="2" t="s">
         <v>42</v>
@@ -3590,10 +3717,10 @@
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C28" s="2">
         <v>1.5</v>
@@ -3623,15 +3750,15 @@
         <v>20</v>
       </c>
       <c r="L28" s="14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C29" s="2">
         <v>1.5</v>
@@ -3661,15 +3788,15 @@
         <v>20</v>
       </c>
       <c r="L29" s="14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C30" s="2">
         <v>1.5</v>
@@ -3699,15 +3826,15 @@
         <v>20</v>
       </c>
       <c r="L30" s="14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C31" s="2">
         <v>1.5</v>
@@ -3734,7 +3861,7 @@
         <v>20</v>
       </c>
       <c r="L31" s="14" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -3742,7 +3869,7 @@
         <v>44</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C32" s="2">
         <v>0.8</v>
@@ -3772,10 +3899,10 @@
     </row>
     <row r="33" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C33" s="2">
         <v>1.5</v>
@@ -3802,15 +3929,15 @@
         <v>10</v>
       </c>
       <c r="L33" s="14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>261</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>262</v>
       </c>
       <c r="C34" s="2">
         <v>1.5</v>
@@ -3837,12 +3964,12 @@
         <v>20</v>
       </c>
       <c r="L34" s="14" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G35" s="13" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4174,7 +4301,7 @@
         <v>32</v>
       </c>
       <c r="L46" s="14" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4284,7 +4411,7 @@
     </row>
     <row r="50" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>75</v>
@@ -4356,7 +4483,7 @@
     </row>
     <row r="52" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>79</v>
@@ -4386,7 +4513,7 @@
         <v>20</v>
       </c>
       <c r="L52" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4425,7 +4552,7 @@
         <v>10</v>
       </c>
       <c r="L54" s="14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="39" thickBot="1" x14ac:dyDescent="0.25">
@@ -4433,7 +4560,7 @@
         <v>90</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C55" s="2">
         <v>2</v>
@@ -4457,13 +4584,13 @@
         <v>0</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K55" s="2">
         <v>10</v>
       </c>
       <c r="L55" s="14" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4498,7 +4625,7 @@
         <v>5</v>
       </c>
       <c r="L56" s="14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4541,10 +4668,10 @@
     </row>
     <row r="58" spans="1:12" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>100</v>
       </c>
       <c r="C58" s="2">
         <v>2</v>
@@ -4568,13 +4695,13 @@
         <v>0</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K58" s="2">
         <v>10</v>
       </c>
       <c r="L58" s="14" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="39" thickBot="1" x14ac:dyDescent="0.25">
@@ -4606,33 +4733,33 @@
         <v>0</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="K59" s="2">
         <v>10</v>
       </c>
       <c r="L59" s="14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="60" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="C60" s="2">
         <v>2</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E60" s="2">
         <v>2</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G60" s="12">
         <v>8</v>
@@ -4644,16 +4771,92 @@
         <v>0</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K60" s="2">
         <v>10</v>
       </c>
       <c r="L60" s="14" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="61" spans="1:12" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="C62" s="2">
+        <v>1</v>
+      </c>
+      <c r="D62" t="s">
+        <v>32</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G62" s="16">
+        <v>1</v>
+      </c>
+      <c r="H62" s="35">
+        <v>0</v>
+      </c>
+      <c r="I62" s="2">
+        <v>0</v>
+      </c>
+      <c r="J62" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K62" s="2">
+        <v>20</v>
+      </c>
+      <c r="L62" s="18" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="C63" s="2">
+        <v>1</v>
+      </c>
+      <c r="D63">
+        <v>3</v>
+      </c>
+      <c r="E63" s="2">
+        <v>4</v>
+      </c>
+      <c r="F63" s="2">
+        <v>4</v>
+      </c>
+      <c r="G63" s="16">
+        <v>10</v>
+      </c>
+      <c r="H63" s="35">
+        <v>1</v>
+      </c>
+      <c r="I63" s="2">
+        <v>0</v>
+      </c>
+      <c r="J63" s="2">
+        <v>1</v>
+      </c>
+      <c r="K63" s="2">
+        <v>5</v>
+      </c>
+      <c r="L63" s="18" t="s">
+        <v>434</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="O3" r:id="rId1" display="..\Stag knight.jpg" xr:uid="{051090D8-9F0F-4C9A-A707-1EB36D88B061}"/>
@@ -4682,30 +4885,30 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D1" t="s">
+        <v>311</v>
+      </c>
+      <c r="E1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" t="s">
         <v>312</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>116</v>
-      </c>
-      <c r="F1" t="s">
-        <v>313</v>
-      </c>
-      <c r="G1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="21"/>
@@ -4716,7 +4919,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B3" s="21"/>
       <c r="C3" s="25"/>
@@ -4727,7 +4930,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
@@ -4738,7 +4941,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B5" s="24"/>
       <c r="C5" s="27"/>
@@ -4749,7 +4952,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
@@ -4760,7 +4963,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B7" s="25"/>
       <c r="C7" s="25"/>
@@ -4789,29 +4992,29 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B3" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -4836,10 +5039,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4849,33 +5052,33 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B2" s="2">
         <v>5</v>
@@ -4899,14 +5102,11 @@
         <f t="shared" ref="H2:H8" si="0">AVERAGE(B2:G2)</f>
         <v>4.333333333333333</v>
       </c>
-      <c r="I2" s="2">
-        <f t="shared" ref="I2:I8" si="1">AVERAGE(B2:F2)</f>
-        <v>4.5999999999999996</v>
-      </c>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B3" s="2">
         <v>6</v>
@@ -4930,14 +5130,11 @@
         <f t="shared" si="0"/>
         <v>4.333333333333333</v>
       </c>
-      <c r="I3" s="2">
-        <f t="shared" si="1"/>
-        <v>4.2</v>
-      </c>
+      <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B4" s="2">
         <v>4</v>
@@ -4961,14 +5158,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="I4" s="2">
-        <f t="shared" si="1"/>
-        <v>4.2</v>
-      </c>
+      <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B5" s="2">
         <v>2</v>
@@ -4992,14 +5186,11 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="I5" s="2">
-        <f t="shared" si="1"/>
-        <v>3.6</v>
-      </c>
+      <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B6" s="2">
         <v>4</v>
@@ -5023,14 +5214,11 @@
         <f t="shared" si="0"/>
         <v>4.333333333333333</v>
       </c>
-      <c r="I6" s="2">
-        <f t="shared" si="1"/>
-        <v>4.4000000000000004</v>
-      </c>
+      <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B7" s="2">
         <v>1</v>
@@ -5054,14 +5242,11 @@
         <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
-      <c r="I7" s="2">
-        <f t="shared" si="1"/>
-        <v>4.2</v>
-      </c>
+      <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B8" s="2">
         <v>6</v>
@@ -5085,15 +5270,63 @@
         <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
-      <c r="I8" s="2">
-        <f t="shared" si="1"/>
-        <v>4.5999999999999996</v>
-      </c>
+      <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>119</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="B9" s="2">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2">
+        <v>3</v>
+      </c>
+      <c r="D9" s="2">
+        <v>5</v>
+      </c>
+      <c r="E9" s="2">
+        <v>4</v>
+      </c>
+      <c r="F9" s="2">
+        <v>7</v>
+      </c>
+      <c r="G9" s="2">
+        <v>4</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" ref="H9:H10" si="1">AVERAGE(B9:G9)</f>
+        <v>4.5</v>
+      </c>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="B10" s="2">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2">
+        <v>5</v>
+      </c>
+      <c r="D10" s="2">
+        <v>5</v>
+      </c>
+      <c r="E10" s="2">
+        <v>6</v>
+      </c>
+      <c r="F10" s="2">
+        <v>2</v>
+      </c>
+      <c r="G10" s="2">
+        <v>3</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5130,30 +5363,30 @@
         <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
@@ -5162,13 +5395,13 @@
         <v>0</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -5176,13 +5409,13 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -5190,26 +5423,26 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="F5" s="2"/>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -5221,7 +5454,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B7" s="2">
         <v>3</v>
@@ -5237,7 +5470,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B8" s="2">
         <v>4</v>
@@ -5288,7 +5521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAD14A1E-99DD-48DF-BC26-F61D5FC7F987}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -5318,182 +5551,182 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C2" s="27"/>
       <c r="D2" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="E2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="F2" s="29" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C3" s="27"/>
       <c r="E3" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="F3" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B4" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C4" s="27"/>
       <c r="F4" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B5" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="F5" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B6" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C6" s="30"/>
       <c r="F6" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C7" s="30"/>
       <c r="F7" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B8" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C8" s="31"/>
       <c r="D8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E8" t="s">
+        <v>420</v>
+      </c>
+      <c r="F8" s="29" t="s">
         <v>422</v>
-      </c>
-      <c r="F8" s="29" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C9" s="31"/>
       <c r="E9" t="s">
+        <v>419</v>
+      </c>
+      <c r="F9" s="29" t="s">
         <v>421</v>
-      </c>
-      <c r="F9" s="29" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C10" s="31"/>
       <c r="E10" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="F10" s="29" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B11" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C11" s="32"/>
       <c r="D11" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="E11" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="F11" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C12" s="32"/>
       <c r="E12" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="F12" s="29" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B13" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C13" s="32"/>
       <c r="E13" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="F13" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -5507,10 +5740,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA31"/>
+  <dimension ref="A1:AA37"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5522,415 +5755,470 @@
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>129</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>131</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" s="14" t="s">
         <v>133</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>135</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>368</v>
+        <v>115</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>242</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C10" s="14" t="s">
         <v>138</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C11" s="14" t="s">
         <v>237</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="14" t="s">
         <v>141</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C13" s="14" t="s">
         <v>143</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="14" t="s">
         <v>146</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C15" s="14" t="s">
         <v>148</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C16" s="14" t="s">
         <v>150</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="18" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="19" spans="1:27" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" ht="51" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C19" s="14" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="20" spans="1:27" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B21" s="2" t="s">
+      <c r="C24" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="C21" s="14" t="s">
+    </row>
+    <row r="25" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="22" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="23" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B23" s="3" t="s">
+      <c r="C26" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="D26" s="7"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
+      <c r="T26" s="3"/>
+      <c r="U26" s="3"/>
+      <c r="V26" s="3"/>
+      <c r="W26" s="3"/>
+      <c r="X26" s="3"/>
+      <c r="Y26" s="3"/>
+      <c r="Z26" s="3"/>
+      <c r="AA26" s="3"/>
+    </row>
+    <row r="27" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>359</v>
+      </c>
+      <c r="D27" s="7"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="3"/>
+      <c r="T27" s="3"/>
+      <c r="U27" s="3"/>
+      <c r="V27" s="3"/>
+      <c r="W27" s="3"/>
+      <c r="X27" s="3"/>
+      <c r="Y27" s="3"/>
+      <c r="Z27" s="3"/>
+      <c r="AA27" s="3"/>
+    </row>
+    <row r="28" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>410</v>
+      </c>
+      <c r="D28" s="7"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="3"/>
+      <c r="T28" s="3"/>
+      <c r="U28" s="3"/>
+      <c r="V28" s="3"/>
+      <c r="W28" s="3"/>
+      <c r="X28" s="3"/>
+      <c r="Y28" s="3"/>
+      <c r="Z28" s="3"/>
+      <c r="AA28" s="3"/>
+    </row>
+    <row r="29" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="3"/>
-      <c r="S23" s="3"/>
-      <c r="T23" s="3"/>
-      <c r="U23" s="3"/>
-      <c r="V23" s="3"/>
-      <c r="W23" s="3"/>
-      <c r="X23" s="3"/>
-      <c r="Y23" s="3"/>
-      <c r="Z23" s="3"/>
-      <c r="AA23" s="3"/>
-    </row>
-    <row r="24" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>359</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>360</v>
-      </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
-      <c r="R24" s="3"/>
-      <c r="S24" s="3"/>
-      <c r="T24" s="3"/>
-      <c r="U24" s="3"/>
-      <c r="V24" s="3"/>
-      <c r="W24" s="3"/>
-      <c r="X24" s="3"/>
-      <c r="Y24" s="3"/>
-      <c r="Z24" s="3"/>
-      <c r="AA24" s="3"/>
-    </row>
-    <row r="25" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>404</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>412</v>
-      </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="3"/>
-      <c r="R25" s="3"/>
-      <c r="S25" s="3"/>
-      <c r="T25" s="3"/>
-      <c r="U25" s="3"/>
-      <c r="V25" s="3"/>
-      <c r="W25" s="3"/>
-      <c r="X25" s="3"/>
-      <c r="Y25" s="3"/>
-      <c r="Z25" s="3"/>
-      <c r="AA25" s="3"/>
-    </row>
-    <row r="26" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B26" s="2" t="s">
+      <c r="C29" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="C26" s="14" t="s">
+    </row>
+    <row r="30" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="27" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+      <c r="C30" s="14" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="28" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+      <c r="B32" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="29" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B29" s="2" t="s">
+      <c r="B33" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="C29" s="18" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="30" spans="1:27" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="C30" s="18" t="s">
+      <c r="C34" s="18" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="31" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="C31" s="18" t="s">
-        <v>375</v>
+    <row r="36" spans="1:3" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>446</v>
       </c>
     </row>
   </sheetData>
@@ -5945,7 +6233,7 @@
   </sheetPr>
   <dimension ref="A2:E35"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
@@ -5959,200 +6247,200 @@
   <sheetData>
     <row r="2" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>292</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>183</v>
       </c>
       <c r="C25" s="2">
         <v>24</v>
@@ -6161,32 +6449,32 @@
         <v>6</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C26" s="2">
         <v>18</v>
       </c>
       <c r="D26" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="E26" s="14" t="s">
         <v>282</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C27" s="2">
         <v>18</v>
@@ -6195,32 +6483,32 @@
         <v>4</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>186</v>
       </c>
       <c r="D28" s="2">
         <v>8</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C29">
         <v>12</v>
@@ -6229,32 +6517,32 @@
         <v>6</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="C30" s="20" t="s">
-        <v>186</v>
-      </c>
-      <c r="D30" s="2" t="s">
+      <c r="E30" s="14" t="s">
         <v>280</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>337</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>338</v>
       </c>
       <c r="C31" s="2">
         <v>6</v>
@@ -6263,51 +6551,51 @@
         <v>6</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
   </sheetData>
@@ -6334,7 +6622,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B1" s="14">
         <f>6*9</f>
@@ -6347,7 +6635,7 @@
     </row>
     <row r="2" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B2" s="2">
         <f>18*7</f>
@@ -6356,7 +6644,7 @@
     </row>
     <row r="3" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B3" s="2">
         <f>10*2</f>
@@ -6365,7 +6653,7 @@
     </row>
     <row r="6" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B6">
         <v>50</v>
@@ -6373,7 +6661,7 @@
     </row>
     <row r="7" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B7">
         <v>40</v>
@@ -6381,7 +6669,7 @@
     </row>
     <row r="8" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B8">
         <v>40</v>
@@ -6389,7 +6677,7 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B9">
         <v>40</v>
@@ -6397,7 +6685,7 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B10">
         <v>30</v>
@@ -6409,205 +6697,205 @@
     <row r="12" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="71.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="22" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="26" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C29" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="36" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="44" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B45" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="47" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>215</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="50" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B51" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B52" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="55" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="57" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="59" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>223</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="61" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -6635,22 +6923,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>230</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="221.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -6668,10 +6956,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{486828E7-6691-466E-812C-C9B1F7969124}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6683,34 +6971,54 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B1" s="20" t="s">
+        <v>305</v>
+      </c>
+      <c r="C1" s="20" t="s">
         <v>306</v>
       </c>
-      <c r="C1" s="20" t="s">
-        <v>307</v>
-      </c>
       <c r="D1" s="20" t="s">
+        <v>318</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>319</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="F1" s="20" t="s">
         <v>320</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>321</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="H1" s="20" t="s">
         <v>322</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="I1" s="20" t="s">
         <v>323</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="J1" s="20" t="s">
         <v>324</v>
       </c>
-      <c r="J1" s="20" t="s">
-        <v>325</v>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" t="s">
+        <v>447</v>
+      </c>
+      <c r="C2" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2" t="s">
+        <v>449</v>
+      </c>
+      <c r="H2" t="s">
+        <v>450</v>
+      </c>
+      <c r="I2" t="s">
+        <v>451</v>
       </c>
     </row>
   </sheetData>

</xml_diff>